<commit_message>
running all search test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Search.xlsx
+++ b/src/test/resources/xls/Search.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="399">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="398">
   <si>
     <t>TCID</t>
   </si>
@@ -1378,9 +1378,6 @@
   </si>
   <si>
     <t>Search126</t>
-  </si>
-  <si>
-    <t>N</t>
   </si>
 </sst>
 </file>
@@ -1783,8 +1780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
-      <selection activeCell="D120" sqref="D120"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1824,7 +1821,7 @@
         <v>76</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>95</v>
@@ -1841,7 +1838,7 @@
         <v>56</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>95</v>
@@ -1858,7 +1855,7 @@
         <v>57</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>95</v>
@@ -1875,7 +1872,7 @@
         <v>58</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E5" s="8" t="s">
         <v>95</v>
@@ -1892,7 +1889,7 @@
         <v>59</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>95</v>
@@ -1909,7 +1906,7 @@
         <v>60</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E7" s="8" t="s">
         <v>95</v>
@@ -1926,7 +1923,7 @@
         <v>53</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E8" s="8" t="s">
         <v>95</v>
@@ -1943,7 +1940,7 @@
         <v>61</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E9" s="8" t="s">
         <v>95</v>
@@ -1960,7 +1957,7 @@
         <v>62</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E10" s="8" t="s">
         <v>95</v>
@@ -1977,7 +1974,7 @@
         <v>63</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E11" s="8" t="s">
         <v>95</v>
@@ -1994,7 +1991,7 @@
         <v>64</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E12" s="8" t="s">
         <v>95</v>
@@ -2011,7 +2008,7 @@
         <v>77</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E13" s="8" t="s">
         <v>95</v>
@@ -2028,7 +2025,7 @@
         <v>65</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E14" s="8" t="s">
         <v>95</v>
@@ -2045,7 +2042,7 @@
         <v>66</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E15" s="8" t="s">
         <v>95</v>
@@ -2062,7 +2059,7 @@
         <v>67</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E16" s="8" t="s">
         <v>95</v>
@@ -2079,7 +2076,7 @@
         <v>68</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E17" s="8" t="s">
         <v>95</v>
@@ -2096,7 +2093,7 @@
         <v>90</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E18" s="8" t="s">
         <v>95</v>
@@ -2113,7 +2110,7 @@
         <v>69</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E19" s="8" t="s">
         <v>95</v>
@@ -2130,7 +2127,7 @@
         <v>70</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E20" s="8" t="s">
         <v>95</v>
@@ -2147,7 +2144,7 @@
         <v>71</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E21" s="8" t="s">
         <v>95</v>
@@ -2164,7 +2161,7 @@
         <v>72</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E22" s="8" t="s">
         <v>95</v>
@@ -2181,7 +2178,7 @@
         <v>73</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E23" s="8" t="s">
         <v>95</v>
@@ -2198,7 +2195,7 @@
         <v>74</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E24" s="8" t="s">
         <v>95</v>
@@ -2215,7 +2212,7 @@
         <v>75</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E25" s="8" t="s">
         <v>95</v>
@@ -2232,7 +2229,7 @@
         <v>78</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E26" s="8" t="s">
         <v>95</v>
@@ -2249,7 +2246,7 @@
         <v>79</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E27" s="8" t="s">
         <v>95</v>
@@ -2266,7 +2263,7 @@
         <v>80</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E28" s="8" t="s">
         <v>95</v>
@@ -2283,7 +2280,7 @@
         <v>81</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E29" s="8" t="s">
         <v>95</v>
@@ -2300,7 +2297,7 @@
         <v>82</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E30" s="8" t="s">
         <v>95</v>
@@ -2317,7 +2314,7 @@
         <v>83</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E31" s="8" t="s">
         <v>95</v>
@@ -2334,7 +2331,7 @@
         <v>84</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E32" s="8" t="s">
         <v>95</v>
@@ -2351,7 +2348,7 @@
         <v>85</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E33" s="8" t="s">
         <v>95</v>
@@ -2368,7 +2365,7 @@
         <v>86</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E34" s="8" t="s">
         <v>95</v>
@@ -2385,7 +2382,7 @@
         <v>87</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E35" s="8" t="s">
         <v>95</v>
@@ -2402,7 +2399,7 @@
         <v>88</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E36" s="8" t="s">
         <v>95</v>
@@ -2419,7 +2416,7 @@
         <v>89</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E37" s="8" t="s">
         <v>95</v>
@@ -2436,7 +2433,7 @@
         <v>90</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E38" s="8" t="s">
         <v>95</v>
@@ -2453,7 +2450,7 @@
         <v>91</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E39" s="8" t="s">
         <v>95</v>
@@ -2470,7 +2467,7 @@
         <v>92</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E40" s="8" t="s">
         <v>95</v>
@@ -2487,7 +2484,7 @@
         <v>93</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E41" s="8" t="s">
         <v>95</v>
@@ -2504,7 +2501,7 @@
         <v>94</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E42" s="8" t="s">
         <v>95</v>
@@ -2521,7 +2518,7 @@
         <v>96</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E43" s="8" t="s">
         <v>95</v>
@@ -2538,7 +2535,7 @@
         <v>97</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E44" s="8" t="s">
         <v>95</v>
@@ -2572,7 +2569,7 @@
         <v>99</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E46" s="8" t="s">
         <v>95</v>
@@ -2589,7 +2586,7 @@
         <v>100</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E47" s="8" t="s">
         <v>95</v>
@@ -2606,7 +2603,7 @@
         <v>101</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E48" s="8" t="s">
         <v>95</v>
@@ -2623,7 +2620,7 @@
         <v>102</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E49" s="8" t="s">
         <v>95</v>
@@ -2640,7 +2637,7 @@
         <v>103</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E50" s="8" t="s">
         <v>95</v>
@@ -2657,7 +2654,7 @@
         <v>106</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E51" s="8" t="s">
         <v>95</v>
@@ -2674,7 +2671,7 @@
         <v>107</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E52" s="8" t="s">
         <v>95</v>
@@ -2691,7 +2688,7 @@
         <v>108</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E53" s="8" t="s">
         <v>95</v>
@@ -2708,7 +2705,7 @@
         <v>109</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E54" s="8" t="s">
         <v>95</v>
@@ -2725,7 +2722,7 @@
         <v>112</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E55" s="8" t="s">
         <v>95</v>
@@ -2742,7 +2739,7 @@
         <v>113</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E56" s="8" t="s">
         <v>95</v>
@@ -2759,7 +2756,7 @@
         <v>114</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E57" s="8" t="s">
         <v>95</v>
@@ -2776,7 +2773,7 @@
         <v>115</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E58" s="8" t="s">
         <v>95</v>
@@ -2793,7 +2790,7 @@
         <v>118</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E59" s="8" t="s">
         <v>95</v>
@@ -2810,7 +2807,7 @@
         <v>120</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E60" s="8" t="s">
         <v>95</v>
@@ -2827,7 +2824,7 @@
         <v>121</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E61" s="8" t="s">
         <v>95</v>
@@ -2844,7 +2841,7 @@
         <v>122</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E62" s="8" t="s">
         <v>95</v>
@@ -2861,7 +2858,7 @@
         <v>123</v>
       </c>
       <c r="D63" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E63" s="8" t="s">
         <v>95</v>
@@ -2878,7 +2875,7 @@
         <v>53</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E64" s="8" t="s">
         <v>95</v>
@@ -2895,7 +2892,7 @@
         <v>128</v>
       </c>
       <c r="D65" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E65" s="8" t="s">
         <v>95</v>
@@ -2912,7 +2909,7 @@
         <v>126</v>
       </c>
       <c r="D66" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E66" s="8" t="s">
         <v>95</v>
@@ -2929,7 +2926,7 @@
         <v>130</v>
       </c>
       <c r="D67" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E67" s="8" t="s">
         <v>95</v>
@@ -2946,7 +2943,7 @@
         <v>131</v>
       </c>
       <c r="D68" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E68" s="8" t="s">
         <v>95</v>
@@ -2963,7 +2960,7 @@
         <v>133</v>
       </c>
       <c r="D69" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E69" s="8" t="s">
         <v>95</v>
@@ -2980,7 +2977,7 @@
         <v>135</v>
       </c>
       <c r="D70" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E70" s="8" t="s">
         <v>95</v>
@@ -2997,7 +2994,7 @@
         <v>136</v>
       </c>
       <c r="D71" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E71" s="8" t="s">
         <v>95</v>
@@ -3014,7 +3011,7 @@
         <v>139</v>
       </c>
       <c r="D72" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E72" s="8" t="s">
         <v>95</v>
@@ -3031,7 +3028,7 @@
         <v>140</v>
       </c>
       <c r="D73" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E73" s="8" t="s">
         <v>95</v>
@@ -3048,7 +3045,7 @@
         <v>143</v>
       </c>
       <c r="D74" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E74" s="8" t="s">
         <v>95</v>
@@ -3065,7 +3062,7 @@
         <v>145</v>
       </c>
       <c r="D75" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E75" s="8" t="s">
         <v>95</v>
@@ -3082,7 +3079,7 @@
         <v>147</v>
       </c>
       <c r="D76" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E76" s="8" t="s">
         <v>95</v>
@@ -3099,7 +3096,7 @@
         <v>148</v>
       </c>
       <c r="D77" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E77" s="8" t="s">
         <v>95</v>
@@ -3116,7 +3113,7 @@
         <v>150</v>
       </c>
       <c r="D78" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E78" s="8" t="s">
         <v>95</v>
@@ -3133,7 +3130,7 @@
         <v>153</v>
       </c>
       <c r="D79" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E79" s="8" t="s">
         <v>95</v>
@@ -3150,7 +3147,7 @@
         <v>155</v>
       </c>
       <c r="D80" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E80" s="8" t="s">
         <v>95</v>
@@ -3167,7 +3164,7 @@
         <v>156</v>
       </c>
       <c r="D81" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E81" s="8" t="s">
         <v>95</v>
@@ -3184,7 +3181,7 @@
         <v>159</v>
       </c>
       <c r="D82" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E82" s="8" t="s">
         <v>95</v>
@@ -3201,7 +3198,7 @@
         <v>161</v>
       </c>
       <c r="D83" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E83" s="8" t="s">
         <v>95</v>
@@ -3218,7 +3215,7 @@
         <v>162</v>
       </c>
       <c r="D84" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E84" s="8" t="s">
         <v>95</v>
@@ -3235,7 +3232,7 @@
         <v>164</v>
       </c>
       <c r="D85" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E85" s="8" t="s">
         <v>95</v>
@@ -3252,7 +3249,7 @@
         <v>165</v>
       </c>
       <c r="D86" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E86" s="8" t="s">
         <v>95</v>
@@ -3269,7 +3266,7 @@
         <v>168</v>
       </c>
       <c r="D87" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E87" s="8" t="s">
         <v>95</v>
@@ -3286,7 +3283,7 @@
         <v>170</v>
       </c>
       <c r="D88" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E88" s="8" t="s">
         <v>95</v>
@@ -3303,7 +3300,7 @@
         <v>171</v>
       </c>
       <c r="D89" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E89" s="8" t="s">
         <v>95</v>
@@ -3320,7 +3317,7 @@
         <v>175</v>
       </c>
       <c r="D90" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E90" s="8" t="s">
         <v>95</v>
@@ -3337,7 +3334,7 @@
         <v>176</v>
       </c>
       <c r="D91" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E91" s="8" t="s">
         <v>95</v>
@@ -3354,7 +3351,7 @@
         <v>179</v>
       </c>
       <c r="D92" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E92" s="8" t="s">
         <v>95</v>
@@ -3371,7 +3368,7 @@
         <v>181</v>
       </c>
       <c r="D93" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E93" s="8" t="s">
         <v>95</v>
@@ -3388,7 +3385,7 @@
         <v>184</v>
       </c>
       <c r="D94" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E94" s="8" t="s">
         <v>95</v>
@@ -3405,7 +3402,7 @@
         <v>185</v>
       </c>
       <c r="D95" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E95" s="8" t="s">
         <v>95</v>
@@ -3422,7 +3419,7 @@
         <v>189</v>
       </c>
       <c r="D96" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E96" s="8" t="s">
         <v>95</v>
@@ -3439,7 +3436,7 @@
         <v>190</v>
       </c>
       <c r="D97" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E97" s="8" t="s">
         <v>95</v>
@@ -3456,7 +3453,7 @@
         <v>192</v>
       </c>
       <c r="D98" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E98" s="8" t="s">
         <v>95</v>
@@ -3473,7 +3470,7 @@
         <v>194</v>
       </c>
       <c r="D99" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E99" s="8" t="s">
         <v>95</v>
@@ -3490,7 +3487,7 @@
         <v>195</v>
       </c>
       <c r="D100" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E100" s="8" t="s">
         <v>95</v>
@@ -3507,7 +3504,7 @@
         <v>198</v>
       </c>
       <c r="D101" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E101" s="8" t="s">
         <v>95</v>
@@ -3524,7 +3521,7 @@
         <v>200</v>
       </c>
       <c r="D102" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E102" s="8" t="s">
         <v>95</v>
@@ -3541,7 +3538,7 @@
         <v>202</v>
       </c>
       <c r="D103" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E103" s="8" t="s">
         <v>95</v>
@@ -3558,7 +3555,7 @@
         <v>204</v>
       </c>
       <c r="D104" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E104" s="8" t="s">
         <v>95</v>
@@ -3575,7 +3572,7 @@
         <v>206</v>
       </c>
       <c r="D105" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E105" s="8" t="s">
         <v>95</v>
@@ -3592,7 +3589,7 @@
         <v>207</v>
       </c>
       <c r="D106" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E106" s="8" t="s">
         <v>95</v>
@@ -3609,7 +3606,7 @@
         <v>227</v>
       </c>
       <c r="D107" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E107" s="8" t="s">
         <v>95</v>
@@ -3626,7 +3623,7 @@
         <v>210</v>
       </c>
       <c r="D108" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E108" s="8" t="s">
         <v>95</v>
@@ -3643,7 +3640,7 @@
         <v>212</v>
       </c>
       <c r="D109" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E109" s="8" t="s">
         <v>95</v>
@@ -3660,7 +3657,7 @@
         <v>216</v>
       </c>
       <c r="D110" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E110" s="8" t="s">
         <v>95</v>
@@ -3677,7 +3674,7 @@
         <v>214</v>
       </c>
       <c r="D111" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E111" s="8" t="s">
         <v>95</v>
@@ -3694,7 +3691,7 @@
         <v>218</v>
       </c>
       <c r="D112" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E112" s="8" t="s">
         <v>95</v>
@@ -3711,7 +3708,7 @@
         <v>219</v>
       </c>
       <c r="D113" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E113" s="8" t="s">
         <v>95</v>
@@ -3728,7 +3725,7 @@
         <v>222</v>
       </c>
       <c r="D114" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E114" s="8" t="s">
         <v>95</v>
@@ -3745,7 +3742,7 @@
         <v>224</v>
       </c>
       <c r="D115" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E115" s="8" t="s">
         <v>95</v>
@@ -3762,7 +3759,7 @@
         <v>225</v>
       </c>
       <c r="D116" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E116" s="8" t="s">
         <v>95</v>
@@ -3779,7 +3776,7 @@
         <v>229</v>
       </c>
       <c r="D117" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E117" s="8" t="s">
         <v>95</v>
@@ -3830,7 +3827,7 @@
         <v>236</v>
       </c>
       <c r="D120" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E120" s="8" t="s">
         <v>95</v>
@@ -3847,7 +3844,7 @@
         <v>238</v>
       </c>
       <c r="D121" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E121" s="8" t="s">
         <v>95</v>
@@ -3864,7 +3861,7 @@
         <v>240</v>
       </c>
       <c r="D122" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E122" s="8" t="s">
         <v>95</v>
@@ -3881,7 +3878,7 @@
         <v>242</v>
       </c>
       <c r="D123" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E123" s="8" t="s">
         <v>95</v>
@@ -3898,7 +3895,7 @@
         <v>244</v>
       </c>
       <c r="D124" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E124" s="8" t="s">
         <v>180</v>
@@ -3915,7 +3912,7 @@
         <v>246</v>
       </c>
       <c r="D125" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E125" s="3"/>
     </row>
@@ -3930,7 +3927,7 @@
         <v>248</v>
       </c>
       <c r="D126" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E126" s="3"/>
     </row>
@@ -3945,7 +3942,7 @@
         <v>250</v>
       </c>
       <c r="D127" s="8" t="s">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="E127" s="3"/>
     </row>

</xml_diff>

<commit_message>
Fixed testcases in search module
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Search.xlsx
+++ b/src/test/resources/xls/Search.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="384">
   <si>
     <t>TCID</t>
   </si>
@@ -381,17 +381,6 @@
     <t>Verify that user is able to expand and collapse the Institutions filter in ARTICLES content type</t>
   </si>
   <si>
-    <t>Verify that following  content type options are present in the search drop down:
-a)All
-b)Articles
-c)Patents
-d)People
-e)Posts</t>
-  </si>
-  <si>
-    <t>Verify that ALL content type is selected in the search drop down by default</t>
-  </si>
-  <si>
     <t>Verify that user is able to select any of the content types present in search drop down</t>
   </si>
   <si>
@@ -402,24 +391,6 @@
   </si>
   <si>
     <t>OPQA-301</t>
-  </si>
-  <si>
-    <t>OPQA-307</t>
-  </si>
-  <si>
-    <t>Verify that ARTICLES option is selected in the left navigation pane by default when user searches using ARTICLES option in the search drop down</t>
-  </si>
-  <si>
-    <t>Verify that PATENTS option is selected in the left navigation pane by default when user searches using PATENTS option in the search drop down</t>
-  </si>
-  <si>
-    <t>Verify that POSTS option is selected in the left navigation pane by default when user searches using POSTS option in the search drop down</t>
-  </si>
-  <si>
-    <t>Verify that PEOPLE option is selected in the left navigation pane by default when user searches using PEOPLE option in the search drop down</t>
-  </si>
-  <si>
-    <t>OPQA-375</t>
   </si>
   <si>
     <t>OPQA-316</t>
@@ -1134,12 +1105,6 @@
     <t>Search44</t>
   </si>
   <si>
-    <t>Search45</t>
-  </si>
-  <si>
-    <t>Search46</t>
-  </si>
-  <si>
     <t>Search47</t>
   </si>
   <si>
@@ -1147,18 +1112,6 @@
   </si>
   <si>
     <t>Search49</t>
-  </si>
-  <si>
-    <t>Search50</t>
-  </si>
-  <si>
-    <t>Search51</t>
-  </si>
-  <si>
-    <t>Search52</t>
-  </si>
-  <si>
-    <t>Search53</t>
   </si>
   <si>
     <t>Search54</t>
@@ -1778,10 +1731,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E127"/>
+  <dimension ref="A1:E121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D127"/>
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1812,7 +1765,7 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="8" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
@@ -1821,7 +1774,7 @@
         <v>76</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>95</v>
@@ -1829,7 +1782,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="8" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>32</v>
@@ -1838,7 +1791,7 @@
         <v>56</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>95</v>
@@ -1846,7 +1799,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="8" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>33</v>
@@ -1855,7 +1808,7 @@
         <v>57</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>95</v>
@@ -1863,7 +1816,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="8" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>34</v>
@@ -1872,7 +1825,7 @@
         <v>58</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E5" s="8" t="s">
         <v>95</v>
@@ -1880,7 +1833,7 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="8" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>35</v>
@@ -1889,7 +1842,7 @@
         <v>59</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>95</v>
@@ -1897,7 +1850,7 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="8" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>36</v>
@@ -1906,7 +1859,7 @@
         <v>60</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E7" s="8" t="s">
         <v>95</v>
@@ -1914,7 +1867,7 @@
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1">
       <c r="A8" s="8" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>54</v>
@@ -1923,7 +1876,7 @@
         <v>53</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E8" s="8" t="s">
         <v>95</v>
@@ -1931,7 +1884,7 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="8" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>49</v>
@@ -1940,7 +1893,7 @@
         <v>61</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E9" s="8" t="s">
         <v>95</v>
@@ -1948,7 +1901,7 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="8" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>51</v>
@@ -1957,7 +1910,7 @@
         <v>62</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E10" s="8" t="s">
         <v>95</v>
@@ -1965,7 +1918,7 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="8" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>50</v>
@@ -1974,7 +1927,7 @@
         <v>63</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E11" s="8" t="s">
         <v>95</v>
@@ -1982,7 +1935,7 @@
     </row>
     <row r="12" spans="1:5" ht="16.5" customHeight="1">
       <c r="A12" s="8" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>52</v>
@@ -1991,7 +1944,7 @@
         <v>64</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E12" s="8" t="s">
         <v>95</v>
@@ -1999,7 +1952,7 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="8" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>48</v>
@@ -2008,7 +1961,7 @@
         <v>77</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E13" s="8" t="s">
         <v>95</v>
@@ -2016,7 +1969,7 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="8" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>37</v>
@@ -2025,7 +1978,7 @@
         <v>65</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E14" s="8" t="s">
         <v>95</v>
@@ -2033,7 +1986,7 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="8" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>38</v>
@@ -2042,7 +1995,7 @@
         <v>66</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E15" s="8" t="s">
         <v>95</v>
@@ -2050,7 +2003,7 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="8" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>47</v>
@@ -2059,7 +2012,7 @@
         <v>67</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E16" s="8" t="s">
         <v>95</v>
@@ -2067,7 +2020,7 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="8" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>46</v>
@@ -2076,7 +2029,7 @@
         <v>68</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E17" s="8" t="s">
         <v>95</v>
@@ -2084,7 +2037,7 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="8" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>55</v>
@@ -2093,7 +2046,7 @@
         <v>90</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E18" s="8" t="s">
         <v>95</v>
@@ -2101,7 +2054,7 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="8" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>45</v>
@@ -2110,7 +2063,7 @@
         <v>69</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E19" s="8" t="s">
         <v>95</v>
@@ -2118,7 +2071,7 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="8" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>44</v>
@@ -2127,7 +2080,7 @@
         <v>70</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E20" s="8" t="s">
         <v>95</v>
@@ -2135,7 +2088,7 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="8" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
       <c r="B21" s="7" t="s">
         <v>43</v>
@@ -2144,7 +2097,7 @@
         <v>71</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E21" s="8" t="s">
         <v>95</v>
@@ -2152,7 +2105,7 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="8" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>39</v>
@@ -2161,7 +2114,7 @@
         <v>72</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E22" s="8" t="s">
         <v>95</v>
@@ -2169,7 +2122,7 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="8" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="B23" s="7" t="s">
         <v>40</v>
@@ -2178,7 +2131,7 @@
         <v>73</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E23" s="8" t="s">
         <v>95</v>
@@ -2186,7 +2139,7 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="8" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="B24" s="7" t="s">
         <v>41</v>
@@ -2195,7 +2148,7 @@
         <v>74</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E24" s="8" t="s">
         <v>95</v>
@@ -2203,7 +2156,7 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="8" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="B25" s="7" t="s">
         <v>42</v>
@@ -2212,7 +2165,7 @@
         <v>75</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E25" s="8" t="s">
         <v>95</v>
@@ -2220,16 +2173,16 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="8" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>78</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E26" s="8" t="s">
         <v>95</v>
@@ -2237,16 +2190,16 @@
     </row>
     <row r="27" spans="1:5" ht="75">
       <c r="A27" s="8" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="C27" s="7" t="s">
         <v>79</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E27" s="8" t="s">
         <v>95</v>
@@ -2254,16 +2207,16 @@
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="8" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="C28" s="8" t="s">
         <v>80</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E28" s="8" t="s">
         <v>95</v>
@@ -2271,16 +2224,16 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="8" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="C29" s="8" t="s">
         <v>81</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E29" s="8" t="s">
         <v>95</v>
@@ -2288,16 +2241,16 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="8" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="C30" s="8" t="s">
         <v>82</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E30" s="8" t="s">
         <v>95</v>
@@ -2305,16 +2258,16 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="8" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="C31" s="8" t="s">
         <v>83</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E31" s="8" t="s">
         <v>95</v>
@@ -2322,16 +2275,16 @@
     </row>
     <row r="32" spans="1:5" ht="90">
       <c r="A32" s="8" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="C32" s="7" t="s">
         <v>84</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E32" s="8" t="s">
         <v>95</v>
@@ -2339,16 +2292,16 @@
     </row>
     <row r="33" spans="1:5" ht="60">
       <c r="A33" s="8" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="C33" s="7" t="s">
         <v>85</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E33" s="8" t="s">
         <v>95</v>
@@ -2356,16 +2309,16 @@
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="8" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="C34" s="7" t="s">
         <v>86</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E34" s="8" t="s">
         <v>95</v>
@@ -2373,16 +2326,16 @@
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="8" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="C35" s="7" t="s">
         <v>87</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E35" s="8" t="s">
         <v>95</v>
@@ -2390,16 +2343,16 @@
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="8" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="C36" s="8" t="s">
         <v>88</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E36" s="8" t="s">
         <v>95</v>
@@ -2407,16 +2360,16 @@
     </row>
     <row r="37" spans="1:5" ht="90">
       <c r="A37" s="8" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="C37" s="7" t="s">
         <v>89</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E37" s="8" t="s">
         <v>95</v>
@@ -2424,16 +2377,16 @@
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="8" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="C38" s="8" t="s">
         <v>90</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E38" s="8" t="s">
         <v>95</v>
@@ -2441,16 +2394,16 @@
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="8" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="C39" s="8" t="s">
         <v>91</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E39" s="8" t="s">
         <v>95</v>
@@ -2458,16 +2411,16 @@
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="8" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="C40" s="8" t="s">
         <v>92</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E40" s="8" t="s">
         <v>95</v>
@@ -2475,16 +2428,16 @@
     </row>
     <row r="41" spans="1:5" ht="90">
       <c r="A41" s="8" t="s">
-        <v>311</v>
+        <v>303</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="C41" s="7" t="s">
         <v>93</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E41" s="8" t="s">
         <v>95</v>
@@ -2492,16 +2445,16 @@
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="8" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="C42" s="7" t="s">
         <v>94</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E42" s="8" t="s">
         <v>95</v>
@@ -2509,16 +2462,16 @@
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="8" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="C43" s="7" t="s">
         <v>96</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E43" s="8" t="s">
         <v>95</v>
@@ -2526,16 +2479,16 @@
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="8" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="C44" s="7" t="s">
         <v>97</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E44" s="8" t="s">
         <v>95</v>
@@ -2543,33 +2496,33 @@
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="8" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="C45" s="7" t="s">
         <v>98</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E45" s="8" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="90">
+    <row r="46" spans="1:5">
       <c r="A46" s="8" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C46" s="7" t="s">
         <v>99</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E46" s="8" t="s">
         <v>95</v>
@@ -2577,16 +2530,16 @@
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="8" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="C47" s="7" t="s">
         <v>100</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E47" s="8" t="s">
         <v>95</v>
@@ -2594,16 +2547,16 @@
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="8" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>46</v>
+        <v>102</v>
       </c>
       <c r="C48" s="7" t="s">
         <v>101</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E48" s="8" t="s">
         <v>95</v>
@@ -2611,16 +2564,16 @@
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="8" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>55</v>
+        <v>103</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E49" s="8" t="s">
         <v>95</v>
@@ -2628,16 +2581,16 @@
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="8" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>104</v>
+        <v>48</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E50" s="8" t="s">
         <v>95</v>
@@ -2645,16 +2598,16 @@
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="8" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>105</v>
+        <v>52</v>
       </c>
       <c r="C51" s="7" t="s">
         <v>106</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E51" s="8" t="s">
         <v>95</v>
@@ -2662,101 +2615,101 @@
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="8" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>47</v>
+        <v>108</v>
       </c>
       <c r="C52" s="7" t="s">
         <v>107</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E52" s="8" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" ht="120">
       <c r="A53" s="8" t="s">
-        <v>323</v>
+        <v>315</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>50</v>
+        <v>109</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E53" s="8" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" ht="30">
       <c r="A54" s="8" t="s">
-        <v>324</v>
+        <v>316</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E54" s="8" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" ht="30">
       <c r="A55" s="8" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>111</v>
+        <v>49</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E55" s="8" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:5" ht="30">
       <c r="A56" s="8" t="s">
-        <v>326</v>
+        <v>318</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E56" s="8" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="57" spans="1:5">
+    <row r="57" spans="1:5" ht="30">
       <c r="A57" s="8" t="s">
-        <v>327</v>
+        <v>319</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>52</v>
+        <v>116</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E57" s="8" t="s">
         <v>95</v>
@@ -2764,220 +2717,220 @@
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="8" t="s">
-        <v>328</v>
+        <v>320</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>116</v>
+        <v>54</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>115</v>
+        <v>53</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E58" s="8" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="120">
+    <row r="59" spans="1:5">
       <c r="A59" s="8" t="s">
-        <v>329</v>
+        <v>321</v>
       </c>
       <c r="B59" s="7" t="s">
         <v>117</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E59" s="8" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="30">
+    <row r="60" spans="1:5">
       <c r="A60" s="8" t="s">
-        <v>330</v>
+        <v>322</v>
       </c>
       <c r="B60" s="7" t="s">
         <v>119</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E60" s="8" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="30">
+    <row r="61" spans="1:5">
       <c r="A61" s="8" t="s">
-        <v>331</v>
+        <v>323</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>49</v>
+        <v>121</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E61" s="8" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="30">
+    <row r="62" spans="1:5">
       <c r="A62" s="8" t="s">
-        <v>332</v>
+        <v>324</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>51</v>
+        <v>124</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E62" s="8" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="30">
+    <row r="63" spans="1:5">
       <c r="A63" s="8" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>124</v>
+        <v>43</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D63" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E63" s="8" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:5" ht="45">
       <c r="A64" s="8" t="s">
-        <v>334</v>
+        <v>326</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>54</v>
+        <v>126</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>53</v>
+        <v>127</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E64" s="8" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="65" spans="1:5">
+    <row r="65" spans="1:5" ht="30">
       <c r="A65" s="8" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="C65" s="7" t="s">
         <v>128</v>
       </c>
       <c r="D65" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E65" s="8" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="66" spans="1:5">
+    <row r="66" spans="1:5" ht="30">
       <c r="A66" s="8" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="D66" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E66" s="8" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="67" spans="1:5">
+    <row r="67" spans="1:5" ht="30">
       <c r="A67" s="8" t="s">
-        <v>337</v>
+        <v>329</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="C67" s="7" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="D67" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E67" s="8" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="68" spans="1:5">
+    <row r="68" spans="1:5" ht="30">
       <c r="A68" s="8" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="D68" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E68" s="8" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="69" spans="1:5">
+    <row r="69" spans="1:5" ht="30">
       <c r="A69" s="8" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>43</v>
+        <v>136</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="D69" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E69" s="8" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="70" spans="1:5" ht="45">
+    <row r="70" spans="1:5" ht="30">
       <c r="A70" s="8" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="D70" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E70" s="8" t="s">
         <v>95</v>
@@ -2985,16 +2938,16 @@
     </row>
     <row r="71" spans="1:5" ht="30">
       <c r="A71" s="8" t="s">
-        <v>341</v>
+        <v>333</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="D71" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E71" s="8" t="s">
         <v>95</v>
@@ -3002,169 +2955,169 @@
     </row>
     <row r="72" spans="1:5" ht="30">
       <c r="A72" s="8" t="s">
+        <v>334</v>
+      </c>
+      <c r="B72" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="C72" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="D72" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="E72" s="8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" s="8" t="s">
+        <v>335</v>
+      </c>
+      <c r="B73" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="C73" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="D73" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="E73" s="8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="90">
+      <c r="A74" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="B74" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="C74" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="D74" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="E74" s="8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="60">
+      <c r="A75" s="8" t="s">
+        <v>337</v>
+      </c>
+      <c r="B75" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="C75" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="D75" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="E75" s="8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76" s="8" t="s">
+        <v>338</v>
+      </c>
+      <c r="B76" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C76" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="D76" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="E76" s="8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77" s="8" t="s">
+        <v>339</v>
+      </c>
+      <c r="B77" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="C77" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="D77" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="E77" s="8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
+      <c r="A78" s="8" t="s">
+        <v>340</v>
+      </c>
+      <c r="B78" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="C78" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="D78" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="E78" s="8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="120">
+      <c r="A79" s="8" t="s">
+        <v>341</v>
+      </c>
+      <c r="B79" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="C79" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="D79" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="E79" s="8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="120">
+      <c r="A80" s="8" t="s">
         <v>342</v>
       </c>
-      <c r="B72" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="C72" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="D72" s="8" t="s">
-        <v>251</v>
-      </c>
-      <c r="E72" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" ht="30">
-      <c r="A73" s="8" t="s">
+      <c r="B80" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="C80" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="D80" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="E80" s="8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" ht="195">
+      <c r="A81" s="8" t="s">
         <v>343</v>
       </c>
-      <c r="B73" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="C73" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="D73" s="8" t="s">
-        <v>251</v>
-      </c>
-      <c r="E73" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" ht="30">
-      <c r="A74" s="8" t="s">
-        <v>344</v>
-      </c>
-      <c r="B74" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="C74" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="D74" s="8" t="s">
-        <v>251</v>
-      </c>
-      <c r="E74" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" ht="30">
-      <c r="A75" s="8" t="s">
-        <v>345</v>
-      </c>
-      <c r="B75" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="C75" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="D75" s="8" t="s">
-        <v>251</v>
-      </c>
-      <c r="E75" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" ht="30">
-      <c r="A76" s="8" t="s">
-        <v>346</v>
-      </c>
-      <c r="B76" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="C76" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="D76" s="8" t="s">
-        <v>251</v>
-      </c>
-      <c r="E76" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" ht="30">
-      <c r="A77" s="8" t="s">
-        <v>347</v>
-      </c>
-      <c r="B77" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="C77" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="D77" s="8" t="s">
-        <v>251</v>
-      </c>
-      <c r="E77" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" ht="30">
-      <c r="A78" s="8" t="s">
-        <v>348</v>
-      </c>
-      <c r="B78" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="C78" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="D78" s="8" t="s">
-        <v>251</v>
-      </c>
-      <c r="E78" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5">
-      <c r="A79" s="8" t="s">
-        <v>349</v>
-      </c>
-      <c r="B79" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="C79" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="D79" s="8" t="s">
-        <v>251</v>
-      </c>
-      <c r="E79" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" ht="90">
-      <c r="A80" s="8" t="s">
-        <v>350</v>
-      </c>
-      <c r="B80" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="C80" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="D80" s="8" t="s">
-        <v>251</v>
-      </c>
-      <c r="E80" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" ht="60">
-      <c r="A81" s="8" t="s">
-        <v>351</v>
-      </c>
       <c r="B81" s="7" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C81" s="7" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="D81" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E81" s="8" t="s">
         <v>95</v>
@@ -3172,16 +3125,16 @@
     </row>
     <row r="82" spans="1:5">
       <c r="A82" s="8" t="s">
-        <v>352</v>
+        <v>344</v>
       </c>
       <c r="B82" s="7" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="C82" s="7" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="D82" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E82" s="8" t="s">
         <v>95</v>
@@ -3189,16 +3142,16 @@
     </row>
     <row r="83" spans="1:5">
       <c r="A83" s="8" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="C83" s="7" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="D83" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E83" s="8" t="s">
         <v>95</v>
@@ -3206,67 +3159,67 @@
     </row>
     <row r="84" spans="1:5">
       <c r="A84" s="8" t="s">
-        <v>354</v>
+        <v>346</v>
       </c>
       <c r="B84" s="7" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="C84" s="7" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="D84" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E84" s="8" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="85" spans="1:5" ht="120">
+    <row r="85" spans="1:5" ht="30">
       <c r="A85" s="8" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="C85" s="7" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="D85" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E85" s="8" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="86" spans="1:5" ht="120">
+    <row r="86" spans="1:5">
       <c r="A86" s="8" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="B86" s="7" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="C86" s="7" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="D86" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E86" s="8" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="87" spans="1:5" ht="195">
+    <row r="87" spans="1:5">
       <c r="A87" s="8" t="s">
-        <v>357</v>
+        <v>349</v>
       </c>
       <c r="B87" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="C87" s="7" t="s">
-        <v>168</v>
+        <v>174</v>
+      </c>
+      <c r="C87" s="8" t="s">
+        <v>173</v>
       </c>
       <c r="D87" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E87" s="8" t="s">
         <v>95</v>
@@ -3274,16 +3227,16 @@
     </row>
     <row r="88" spans="1:5">
       <c r="A88" s="8" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
       <c r="B88" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="C88" s="7" t="s">
-        <v>170</v>
+        <v>175</v>
+      </c>
+      <c r="C88" s="8" t="s">
+        <v>176</v>
       </c>
       <c r="D88" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E88" s="8" t="s">
         <v>95</v>
@@ -3291,50 +3244,50 @@
     </row>
     <row r="89" spans="1:5">
       <c r="A89" s="8" t="s">
-        <v>359</v>
+        <v>351</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>173</v>
-      </c>
-      <c r="C89" s="7" t="s">
-        <v>171</v>
+        <v>178</v>
+      </c>
+      <c r="C89" s="8" t="s">
+        <v>177</v>
       </c>
       <c r="D89" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E89" s="8" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="90" spans="1:5">
+    <row r="90" spans="1:5" ht="105">
       <c r="A90" s="8" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="C90" s="7" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="D90" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E90" s="8" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="91" spans="1:5" ht="30">
+    <row r="91" spans="1:5" ht="105">
       <c r="A91" s="8" t="s">
-        <v>361</v>
+        <v>353</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="C91" s="7" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="D91" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E91" s="8" t="s">
         <v>95</v>
@@ -3342,16 +3295,16 @@
     </row>
     <row r="92" spans="1:5">
       <c r="A92" s="8" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
       <c r="B92" s="7" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="C92" s="7" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="D92" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E92" s="8" t="s">
         <v>95</v>
@@ -3359,33 +3312,33 @@
     </row>
     <row r="93" spans="1:5">
       <c r="A93" s="8" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="B93" s="7" t="s">
-        <v>182</v>
-      </c>
-      <c r="C93" s="8" t="s">
-        <v>181</v>
+        <v>185</v>
+      </c>
+      <c r="C93" s="7" t="s">
+        <v>186</v>
       </c>
       <c r="D93" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E93" s="8" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="94" spans="1:5">
+    <row r="94" spans="1:5" ht="45">
       <c r="A94" s="8" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>183</v>
-      </c>
-      <c r="C94" s="8" t="s">
-        <v>184</v>
+        <v>188</v>
+      </c>
+      <c r="C94" s="7" t="s">
+        <v>187</v>
       </c>
       <c r="D94" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E94" s="8" t="s">
         <v>95</v>
@@ -3393,50 +3346,50 @@
     </row>
     <row r="95" spans="1:5">
       <c r="A95" s="8" t="s">
-        <v>365</v>
-      </c>
-      <c r="B95" s="7" t="s">
-        <v>186</v>
+        <v>357</v>
+      </c>
+      <c r="B95" s="8" t="s">
+        <v>189</v>
       </c>
       <c r="C95" s="8" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="D95" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E95" s="8" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="96" spans="1:5" ht="105">
+    <row r="96" spans="1:5">
       <c r="A96" s="8" t="s">
-        <v>366</v>
-      </c>
-      <c r="B96" s="7" t="s">
-        <v>187</v>
-      </c>
-      <c r="C96" s="7" t="s">
-        <v>189</v>
+        <v>358</v>
+      </c>
+      <c r="B96" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="C96" s="8" t="s">
+        <v>192</v>
       </c>
       <c r="D96" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E96" s="8" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="97" spans="1:5" ht="105">
+    <row r="97" spans="1:5">
       <c r="A97" s="8" t="s">
-        <v>367</v>
-      </c>
-      <c r="B97" s="7" t="s">
-        <v>188</v>
-      </c>
-      <c r="C97" s="7" t="s">
-        <v>190</v>
+        <v>359</v>
+      </c>
+      <c r="B97" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="C97" s="8" t="s">
+        <v>194</v>
       </c>
       <c r="D97" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E97" s="8" t="s">
         <v>95</v>
@@ -3444,16 +3397,16 @@
     </row>
     <row r="98" spans="1:5">
       <c r="A98" s="8" t="s">
-        <v>368</v>
-      </c>
-      <c r="B98" s="7" t="s">
-        <v>191</v>
-      </c>
-      <c r="C98" s="7" t="s">
-        <v>192</v>
+        <v>360</v>
+      </c>
+      <c r="B98" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="C98" s="8" t="s">
+        <v>196</v>
       </c>
       <c r="D98" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E98" s="8" t="s">
         <v>95</v>
@@ -3461,50 +3414,50 @@
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="8" t="s">
-        <v>369</v>
-      </c>
-      <c r="B99" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="C99" s="7" t="s">
-        <v>194</v>
+        <v>361</v>
+      </c>
+      <c r="B99" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="C99" s="8" t="s">
+        <v>198</v>
       </c>
       <c r="D99" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E99" s="8" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="100" spans="1:5" ht="45">
+    <row r="100" spans="1:5" ht="165">
       <c r="A100" s="8" t="s">
-        <v>370</v>
-      </c>
-      <c r="B100" s="7" t="s">
-        <v>196</v>
+        <v>362</v>
+      </c>
+      <c r="B100" s="8" t="s">
+        <v>200</v>
       </c>
       <c r="C100" s="7" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D100" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E100" s="8" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="101" spans="1:5">
+    <row r="101" spans="1:5" ht="75">
       <c r="A101" s="8" t="s">
-        <v>371</v>
-      </c>
-      <c r="B101" s="8" t="s">
-        <v>197</v>
-      </c>
-      <c r="C101" s="8" t="s">
-        <v>198</v>
+        <v>363</v>
+      </c>
+      <c r="B101" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="C101" s="7" t="s">
+        <v>219</v>
       </c>
       <c r="D101" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E101" s="8" t="s">
         <v>95</v>
@@ -3512,16 +3465,16 @@
     </row>
     <row r="102" spans="1:5">
       <c r="A102" s="8" t="s">
-        <v>372</v>
-      </c>
-      <c r="B102" s="8" t="s">
-        <v>199</v>
-      </c>
-      <c r="C102" s="8" t="s">
-        <v>200</v>
+        <v>364</v>
+      </c>
+      <c r="B102" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="C102" s="7" t="s">
+        <v>202</v>
       </c>
       <c r="D102" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E102" s="8" t="s">
         <v>95</v>
@@ -3529,16 +3482,16 @@
     </row>
     <row r="103" spans="1:5">
       <c r="A103" s="8" t="s">
-        <v>373</v>
-      </c>
-      <c r="B103" s="8" t="s">
-        <v>201</v>
-      </c>
-      <c r="C103" s="8" t="s">
-        <v>202</v>
+        <v>365</v>
+      </c>
+      <c r="B103" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="C103" s="7" t="s">
+        <v>204</v>
       </c>
       <c r="D103" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E103" s="8" t="s">
         <v>95</v>
@@ -3546,16 +3499,16 @@
     </row>
     <row r="104" spans="1:5">
       <c r="A104" s="8" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
       <c r="B104" s="8" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="C104" s="8" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="D104" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E104" s="8" t="s">
         <v>95</v>
@@ -3563,7 +3516,7 @@
     </row>
     <row r="105" spans="1:5">
       <c r="A105" s="8" t="s">
-        <v>375</v>
+        <v>367</v>
       </c>
       <c r="B105" s="8" t="s">
         <v>205</v>
@@ -3572,41 +3525,41 @@
         <v>206</v>
       </c>
       <c r="D105" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E105" s="8" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="106" spans="1:5" ht="165">
+    <row r="106" spans="1:5">
       <c r="A106" s="8" t="s">
-        <v>376</v>
+        <v>368</v>
       </c>
       <c r="B106" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="C106" s="7" t="s">
-        <v>207</v>
+        <v>209</v>
+      </c>
+      <c r="C106" s="8" t="s">
+        <v>210</v>
       </c>
       <c r="D106" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E106" s="8" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="107" spans="1:5" ht="75">
+    <row r="107" spans="1:5">
       <c r="A107" s="8" t="s">
-        <v>377</v>
-      </c>
-      <c r="B107" s="9" t="s">
-        <v>228</v>
-      </c>
-      <c r="C107" s="7" t="s">
-        <v>227</v>
+        <v>369</v>
+      </c>
+      <c r="B107" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="C107" s="8" t="s">
+        <v>211</v>
       </c>
       <c r="D107" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E107" s="8" t="s">
         <v>95</v>
@@ -3614,16 +3567,16 @@
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="8" t="s">
-        <v>378</v>
-      </c>
-      <c r="B108" s="7" t="s">
-        <v>209</v>
-      </c>
-      <c r="C108" s="7" t="s">
-        <v>210</v>
+        <v>370</v>
+      </c>
+      <c r="B108" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="C108" s="8" t="s">
+        <v>214</v>
       </c>
       <c r="D108" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E108" s="8" t="s">
         <v>95</v>
@@ -3631,16 +3584,16 @@
     </row>
     <row r="109" spans="1:5">
       <c r="A109" s="8" t="s">
-        <v>379</v>
-      </c>
-      <c r="B109" s="7" t="s">
-        <v>211</v>
-      </c>
-      <c r="C109" s="7" t="s">
-        <v>212</v>
+        <v>371</v>
+      </c>
+      <c r="B109" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="C109" s="8" t="s">
+        <v>216</v>
       </c>
       <c r="D109" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E109" s="8" t="s">
         <v>95</v>
@@ -3648,16 +3601,16 @@
     </row>
     <row r="110" spans="1:5">
       <c r="A110" s="8" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="B110" s="8" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="C110" s="8" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D110" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E110" s="8" t="s">
         <v>95</v>
@@ -3665,101 +3618,101 @@
     </row>
     <row r="111" spans="1:5">
       <c r="A111" s="8" t="s">
-        <v>381</v>
-      </c>
-      <c r="B111" s="8" t="s">
-        <v>213</v>
-      </c>
-      <c r="C111" s="8" t="s">
-        <v>214</v>
+        <v>373</v>
+      </c>
+      <c r="B111" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="C111" s="9" t="s">
+        <v>221</v>
       </c>
       <c r="D111" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E111" s="8" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="112" spans="1:5">
+    <row r="112" spans="1:5" ht="30">
       <c r="A112" s="8" t="s">
-        <v>382</v>
-      </c>
-      <c r="B112" s="8" t="s">
-        <v>217</v>
-      </c>
-      <c r="C112" s="8" t="s">
-        <v>218</v>
+        <v>374</v>
+      </c>
+      <c r="B112" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="C112" s="10" t="s">
+        <v>223</v>
       </c>
       <c r="D112" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E112" s="8" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="113" spans="1:5">
+    <row r="113" spans="1:5" ht="75">
       <c r="A113" s="8" t="s">
-        <v>383</v>
+        <v>375</v>
       </c>
       <c r="B113" s="8" t="s">
-        <v>220</v>
-      </c>
-      <c r="C113" s="8" t="s">
-        <v>219</v>
+        <v>225</v>
+      </c>
+      <c r="C113" s="7" t="s">
+        <v>226</v>
       </c>
       <c r="D113" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E113" s="8" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="114" spans="1:5">
+    <row r="114" spans="1:5" ht="60">
       <c r="A114" s="8" t="s">
-        <v>384</v>
-      </c>
-      <c r="B114" s="8" t="s">
-        <v>221</v>
-      </c>
-      <c r="C114" s="8" t="s">
-        <v>222</v>
+        <v>376</v>
+      </c>
+      <c r="B114" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="C114" s="7" t="s">
+        <v>228</v>
       </c>
       <c r="D114" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E114" s="8" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="115" spans="1:5">
+    <row r="115" spans="1:5" ht="105">
       <c r="A115" s="8" t="s">
-        <v>385</v>
-      </c>
-      <c r="B115" s="8" t="s">
-        <v>223</v>
-      </c>
-      <c r="C115" s="8" t="s">
-        <v>224</v>
+        <v>377</v>
+      </c>
+      <c r="B115" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="C115" s="7" t="s">
+        <v>230</v>
       </c>
       <c r="D115" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E115" s="8" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="116" spans="1:5">
+    <row r="116" spans="1:5" ht="105">
       <c r="A116" s="8" t="s">
-        <v>386</v>
-      </c>
-      <c r="B116" s="8" t="s">
-        <v>226</v>
-      </c>
-      <c r="C116" s="8" t="s">
-        <v>225</v>
+        <v>378</v>
+      </c>
+      <c r="B116" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C116" s="7" t="s">
+        <v>232</v>
       </c>
       <c r="D116" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E116" s="8" t="s">
         <v>95</v>
@@ -3767,184 +3720,82 @@
     </row>
     <row r="117" spans="1:5">
       <c r="A117" s="8" t="s">
-        <v>387</v>
-      </c>
-      <c r="B117" s="9" t="s">
-        <v>230</v>
-      </c>
-      <c r="C117" s="9" t="s">
-        <v>229</v>
+        <v>379</v>
+      </c>
+      <c r="B117" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="C117" s="8" t="s">
+        <v>234</v>
       </c>
       <c r="D117" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E117" s="8" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="118" spans="1:5" ht="30">
+    <row r="118" spans="1:5">
       <c r="A118" s="8" t="s">
-        <v>388</v>
-      </c>
-      <c r="B118" s="9" t="s">
-        <v>232</v>
-      </c>
-      <c r="C118" s="10" t="s">
-        <v>231</v>
+        <v>380</v>
+      </c>
+      <c r="B118" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="C118" s="3" t="s">
+        <v>236</v>
       </c>
       <c r="D118" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E118" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" ht="75">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5">
       <c r="A119" s="8" t="s">
-        <v>389</v>
-      </c>
-      <c r="B119" s="8" t="s">
-        <v>233</v>
-      </c>
-      <c r="C119" s="7" t="s">
-        <v>234</v>
+        <v>381</v>
+      </c>
+      <c r="B119" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="C119" s="3" t="s">
+        <v>238</v>
       </c>
       <c r="D119" s="8" t="s">
-        <v>251</v>
-      </c>
-      <c r="E119" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" ht="60">
+        <v>243</v>
+      </c>
+      <c r="E119" s="3"/>
+    </row>
+    <row r="120" spans="1:5">
       <c r="A120" s="8" t="s">
-        <v>390</v>
-      </c>
-      <c r="B120" s="7" t="s">
-        <v>235</v>
-      </c>
-      <c r="C120" s="7" t="s">
-        <v>236</v>
+        <v>382</v>
+      </c>
+      <c r="B120" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="C120" s="3" t="s">
+        <v>240</v>
       </c>
       <c r="D120" s="8" t="s">
-        <v>251</v>
-      </c>
-      <c r="E120" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5" ht="105">
+        <v>243</v>
+      </c>
+      <c r="E120" s="3"/>
+    </row>
+    <row r="121" spans="1:5" ht="150">
       <c r="A121" s="8" t="s">
-        <v>391</v>
-      </c>
-      <c r="B121" s="7" t="s">
-        <v>237</v>
-      </c>
-      <c r="C121" s="7" t="s">
-        <v>238</v>
+        <v>383</v>
+      </c>
+      <c r="B121" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="C121" s="4" t="s">
+        <v>242</v>
       </c>
       <c r="D121" s="8" t="s">
-        <v>251</v>
-      </c>
-      <c r="E121" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="122" spans="1:5" ht="105">
-      <c r="A122" s="8" t="s">
-        <v>392</v>
-      </c>
-      <c r="B122" s="7" t="s">
-        <v>239</v>
-      </c>
-      <c r="C122" s="7" t="s">
-        <v>240</v>
-      </c>
-      <c r="D122" s="8" t="s">
-        <v>251</v>
-      </c>
-      <c r="E122" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="123" spans="1:5">
-      <c r="A123" s="8" t="s">
-        <v>393</v>
-      </c>
-      <c r="B123" s="7" t="s">
-        <v>241</v>
-      </c>
-      <c r="C123" s="8" t="s">
-        <v>242</v>
-      </c>
-      <c r="D123" s="8" t="s">
-        <v>251</v>
-      </c>
-      <c r="E123" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="124" spans="1:5">
-      <c r="A124" s="8" t="s">
-        <v>394</v>
-      </c>
-      <c r="B124" s="7" t="s">
-        <v>243</v>
-      </c>
-      <c r="C124" s="3" t="s">
-        <v>244</v>
-      </c>
-      <c r="D124" s="8" t="s">
-        <v>251</v>
-      </c>
-      <c r="E124" s="8" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="125" spans="1:5">
-      <c r="A125" s="8" t="s">
-        <v>395</v>
-      </c>
-      <c r="B125" s="3" t="s">
-        <v>245</v>
-      </c>
-      <c r="C125" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="D125" s="8" t="s">
-        <v>251</v>
-      </c>
-      <c r="E125" s="3"/>
-    </row>
-    <row r="126" spans="1:5">
-      <c r="A126" s="8" t="s">
-        <v>396</v>
-      </c>
-      <c r="B126" s="3" t="s">
-        <v>247</v>
-      </c>
-      <c r="C126" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="D126" s="8" t="s">
-        <v>251</v>
-      </c>
-      <c r="E126" s="3"/>
-    </row>
-    <row r="127" spans="1:5" ht="150">
-      <c r="A127" s="8" t="s">
-        <v>397</v>
-      </c>
-      <c r="B127" s="3" t="s">
-        <v>249</v>
-      </c>
-      <c r="C127" s="4" t="s">
-        <v>250</v>
-      </c>
-      <c r="D127" s="8" t="s">
-        <v>251</v>
-      </c>
-      <c r="E127" s="3"/>
+        <v>243</v>
+      </c>
+      <c r="E121" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Removed depricated test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Search.xlsx
+++ b/src/test/resources/xls/Search.xlsx
@@ -414,15 +414,6 @@
     <t>OPQA-287</t>
   </si>
   <si>
-    <t>Verify that the following sections get displayed in the search type ahead when user searches using ALL option in the search drop down and that the searched keyword is present in all the sections:
-a)Autocompleted keyword
-b)4 suggestions in CATEGORY section
-c)4 suggestions in ARTICLES section
-d)4 suggestions in PATENTS section
-e)4 suggestions in POSTS section
-f)4 suggestions in PEOPLE section</t>
-  </si>
-  <si>
     <t>OPQA-311</t>
   </si>
   <si>
@@ -821,10 +812,6 @@
     <t>OPQA-1228</t>
   </si>
   <si>
-    <t>Verify that sorting is retained when user navigates back to POSTS search results page from record view page
-Verify that search drop down content type is retained when user navigates back to POSTS search results page from record view page</t>
-  </si>
-  <si>
     <t>OPQA-1229|OPQA-1230</t>
   </si>
   <si>
@@ -910,427 +897,440 @@
 g)DETAILS link</t>
   </si>
   <si>
+    <t>OPQA-1434</t>
+  </si>
+  <si>
+    <t>OPQA-1435</t>
+  </si>
+  <si>
+    <t>OPQA-1436</t>
+  </si>
+  <si>
+    <t>OPQA-1437</t>
+  </si>
+  <si>
+    <t>OPQA-1438</t>
+  </si>
+  <si>
+    <t>OPQA-1439</t>
+  </si>
+  <si>
+    <t>OPQA-1440</t>
+  </si>
+  <si>
+    <t>OPQA-1441</t>
+  </si>
+  <si>
+    <t>OPQA-1442</t>
+  </si>
+  <si>
+    <t>OPQA-1443</t>
+  </si>
+  <si>
+    <t>OPQA-1444</t>
+  </si>
+  <si>
+    <t>OPQA-1445</t>
+  </si>
+  <si>
+    <t>OPQA-1447</t>
+  </si>
+  <si>
+    <t>OPQA-1449</t>
+  </si>
+  <si>
+    <t>OPQA-1450</t>
+  </si>
+  <si>
+    <t>OPQA-1452</t>
+  </si>
+  <si>
+    <t>OPQA-1453</t>
+  </si>
+  <si>
+    <t>OPQA-1455</t>
+  </si>
+  <si>
+    <t>OPQA-1456</t>
+  </si>
+  <si>
+    <t>OPQA-1501</t>
+  </si>
+  <si>
+    <t>Search1</t>
+  </si>
+  <si>
+    <t>Search2</t>
+  </si>
+  <si>
+    <t>Search3</t>
+  </si>
+  <si>
+    <t>Search4</t>
+  </si>
+  <si>
+    <t>Search5</t>
+  </si>
+  <si>
+    <t>Search6</t>
+  </si>
+  <si>
+    <t>Search7</t>
+  </si>
+  <si>
+    <t>Search8</t>
+  </si>
+  <si>
+    <t>Search9</t>
+  </si>
+  <si>
+    <t>Search10</t>
+  </si>
+  <si>
+    <t>Search11</t>
+  </si>
+  <si>
+    <t>Search12</t>
+  </si>
+  <si>
+    <t>Search13</t>
+  </si>
+  <si>
+    <t>Search14</t>
+  </si>
+  <si>
+    <t>Search15</t>
+  </si>
+  <si>
+    <t>Search16</t>
+  </si>
+  <si>
+    <t>Search17</t>
+  </si>
+  <si>
+    <t>Search18</t>
+  </si>
+  <si>
+    <t>Search19</t>
+  </si>
+  <si>
+    <t>Search20</t>
+  </si>
+  <si>
+    <t>Search21</t>
+  </si>
+  <si>
+    <t>Search22</t>
+  </si>
+  <si>
+    <t>Search23</t>
+  </si>
+  <si>
+    <t>Search24</t>
+  </si>
+  <si>
+    <t>Search25</t>
+  </si>
+  <si>
+    <t>Search26</t>
+  </si>
+  <si>
+    <t>Search27</t>
+  </si>
+  <si>
+    <t>Search28</t>
+  </si>
+  <si>
+    <t>Search29</t>
+  </si>
+  <si>
+    <t>Search30</t>
+  </si>
+  <si>
+    <t>Search31</t>
+  </si>
+  <si>
+    <t>Search32</t>
+  </si>
+  <si>
+    <t>Search33</t>
+  </si>
+  <si>
+    <t>Search34</t>
+  </si>
+  <si>
+    <t>Search35</t>
+  </si>
+  <si>
+    <t>Search36</t>
+  </si>
+  <si>
+    <t>Search37</t>
+  </si>
+  <si>
+    <t>Search38</t>
+  </si>
+  <si>
+    <t>Search39</t>
+  </si>
+  <si>
+    <t>Search40</t>
+  </si>
+  <si>
+    <t>Search41</t>
+  </si>
+  <si>
+    <t>Search42</t>
+  </si>
+  <si>
+    <t>Search43</t>
+  </si>
+  <si>
+    <t>Search44</t>
+  </si>
+  <si>
+    <t>Search47</t>
+  </si>
+  <si>
+    <t>Search48</t>
+  </si>
+  <si>
+    <t>Search49</t>
+  </si>
+  <si>
+    <t>Search54</t>
+  </si>
+  <si>
+    <t>Search55</t>
+  </si>
+  <si>
+    <t>Search56</t>
+  </si>
+  <si>
+    <t>Search57</t>
+  </si>
+  <si>
+    <t>Search58</t>
+  </si>
+  <si>
+    <t>Search59</t>
+  </si>
+  <si>
+    <t>Search60</t>
+  </si>
+  <si>
+    <t>Search61</t>
+  </si>
+  <si>
+    <t>Search62</t>
+  </si>
+  <si>
+    <t>Search63</t>
+  </si>
+  <si>
+    <t>Search64</t>
+  </si>
+  <si>
+    <t>Search65</t>
+  </si>
+  <si>
+    <t>Search66</t>
+  </si>
+  <si>
+    <t>Search67</t>
+  </si>
+  <si>
+    <t>Search68</t>
+  </si>
+  <si>
+    <t>Search69</t>
+  </si>
+  <si>
+    <t>Search70</t>
+  </si>
+  <si>
+    <t>Search71</t>
+  </si>
+  <si>
+    <t>Search72</t>
+  </si>
+  <si>
+    <t>Search73</t>
+  </si>
+  <si>
+    <t>Search74</t>
+  </si>
+  <si>
+    <t>Search75</t>
+  </si>
+  <si>
+    <t>Search76</t>
+  </si>
+  <si>
+    <t>Search77</t>
+  </si>
+  <si>
+    <t>Search78</t>
+  </si>
+  <si>
+    <t>Search79</t>
+  </si>
+  <si>
+    <t>Search80</t>
+  </si>
+  <si>
+    <t>Search81</t>
+  </si>
+  <si>
+    <t>Search82</t>
+  </si>
+  <si>
+    <t>Search83</t>
+  </si>
+  <si>
+    <t>Search84</t>
+  </si>
+  <si>
+    <t>Search85</t>
+  </si>
+  <si>
+    <t>Search86</t>
+  </si>
+  <si>
+    <t>Search87</t>
+  </si>
+  <si>
+    <t>Search88</t>
+  </si>
+  <si>
+    <t>Search89</t>
+  </si>
+  <si>
+    <t>Search90</t>
+  </si>
+  <si>
+    <t>Search91</t>
+  </si>
+  <si>
+    <t>Search92</t>
+  </si>
+  <si>
+    <t>Search93</t>
+  </si>
+  <si>
+    <t>Search94</t>
+  </si>
+  <si>
+    <t>Search95</t>
+  </si>
+  <si>
+    <t>Search96</t>
+  </si>
+  <si>
+    <t>Search97</t>
+  </si>
+  <si>
+    <t>Search98</t>
+  </si>
+  <si>
+    <t>Search99</t>
+  </si>
+  <si>
+    <t>Search100</t>
+  </si>
+  <si>
+    <t>Search101</t>
+  </si>
+  <si>
+    <t>Search102</t>
+  </si>
+  <si>
+    <t>Search103</t>
+  </si>
+  <si>
+    <t>Search104</t>
+  </si>
+  <si>
+    <t>Search105</t>
+  </si>
+  <si>
+    <t>Search106</t>
+  </si>
+  <si>
+    <t>Search107</t>
+  </si>
+  <si>
+    <t>Search108</t>
+  </si>
+  <si>
+    <t>Search109</t>
+  </si>
+  <si>
+    <t>Search110</t>
+  </si>
+  <si>
+    <t>Search111</t>
+  </si>
+  <si>
+    <t>Search112</t>
+  </si>
+  <si>
+    <t>Search113</t>
+  </si>
+  <si>
+    <t>Search114</t>
+  </si>
+  <si>
+    <t>Search115</t>
+  </si>
+  <si>
+    <t>Search116</t>
+  </si>
+  <si>
+    <t>Search117</t>
+  </si>
+  <si>
+    <t>Search118</t>
+  </si>
+  <si>
+    <t>Search119</t>
+  </si>
+  <si>
+    <t>Search120</t>
+  </si>
+  <si>
+    <t>Search121</t>
+  </si>
+  <si>
+    <t>Search122</t>
+  </si>
+  <si>
+    <t>Search123</t>
+  </si>
+  <si>
+    <t>Search124</t>
+  </si>
+  <si>
+    <t>Search125</t>
+  </si>
+  <si>
+    <t>Search126</t>
+  </si>
+  <si>
     <t>Y</t>
   </si>
   <si>
-    <t>OPQA-1434</t>
-  </si>
-  <si>
-    <t>OPQA-1435</t>
-  </si>
-  <si>
-    <t>OPQA-1436</t>
-  </si>
-  <si>
-    <t>OPQA-1437</t>
-  </si>
-  <si>
-    <t>OPQA-1438</t>
-  </si>
-  <si>
-    <t>OPQA-1439</t>
-  </si>
-  <si>
-    <t>OPQA-1440</t>
-  </si>
-  <si>
-    <t>OPQA-1441</t>
-  </si>
-  <si>
-    <t>OPQA-1442</t>
-  </si>
-  <si>
-    <t>OPQA-1443</t>
-  </si>
-  <si>
-    <t>OPQA-1444</t>
-  </si>
-  <si>
-    <t>OPQA-1445</t>
-  </si>
-  <si>
-    <t>OPQA-1447</t>
-  </si>
-  <si>
-    <t>OPQA-1449</t>
-  </si>
-  <si>
-    <t>OPQA-1450</t>
-  </si>
-  <si>
-    <t>OPQA-1452</t>
-  </si>
-  <si>
-    <t>OPQA-1453</t>
-  </si>
-  <si>
-    <t>OPQA-1455</t>
-  </si>
-  <si>
-    <t>OPQA-1456</t>
-  </si>
-  <si>
-    <t>OPQA-1501</t>
-  </si>
-  <si>
-    <t>Search1</t>
-  </si>
-  <si>
-    <t>Search2</t>
-  </si>
-  <si>
-    <t>Search3</t>
-  </si>
-  <si>
-    <t>Search4</t>
-  </si>
-  <si>
-    <t>Search5</t>
-  </si>
-  <si>
-    <t>Search6</t>
-  </si>
-  <si>
-    <t>Search7</t>
-  </si>
-  <si>
-    <t>Search8</t>
-  </si>
-  <si>
-    <t>Search9</t>
-  </si>
-  <si>
-    <t>Search10</t>
-  </si>
-  <si>
-    <t>Search11</t>
-  </si>
-  <si>
-    <t>Search12</t>
-  </si>
-  <si>
-    <t>Search13</t>
-  </si>
-  <si>
-    <t>Search14</t>
-  </si>
-  <si>
-    <t>Search15</t>
-  </si>
-  <si>
-    <t>Search16</t>
-  </si>
-  <si>
-    <t>Search17</t>
-  </si>
-  <si>
-    <t>Search18</t>
-  </si>
-  <si>
-    <t>Search19</t>
-  </si>
-  <si>
-    <t>Search20</t>
-  </si>
-  <si>
-    <t>Search21</t>
-  </si>
-  <si>
-    <t>Search22</t>
-  </si>
-  <si>
-    <t>Search23</t>
-  </si>
-  <si>
-    <t>Search24</t>
-  </si>
-  <si>
-    <t>Search25</t>
-  </si>
-  <si>
-    <t>Search26</t>
-  </si>
-  <si>
-    <t>Search27</t>
-  </si>
-  <si>
-    <t>Search28</t>
-  </si>
-  <si>
-    <t>Search29</t>
-  </si>
-  <si>
-    <t>Search30</t>
-  </si>
-  <si>
-    <t>Search31</t>
-  </si>
-  <si>
-    <t>Search32</t>
-  </si>
-  <si>
-    <t>Search33</t>
-  </si>
-  <si>
-    <t>Search34</t>
-  </si>
-  <si>
-    <t>Search35</t>
-  </si>
-  <si>
-    <t>Search36</t>
-  </si>
-  <si>
-    <t>Search37</t>
-  </si>
-  <si>
-    <t>Search38</t>
-  </si>
-  <si>
-    <t>Search39</t>
-  </si>
-  <si>
-    <t>Search40</t>
-  </si>
-  <si>
-    <t>Search41</t>
-  </si>
-  <si>
-    <t>Search42</t>
-  </si>
-  <si>
-    <t>Search43</t>
-  </si>
-  <si>
-    <t>Search44</t>
-  </si>
-  <si>
-    <t>Search47</t>
-  </si>
-  <si>
-    <t>Search48</t>
-  </si>
-  <si>
-    <t>Search49</t>
-  </si>
-  <si>
-    <t>Search54</t>
-  </si>
-  <si>
-    <t>Search55</t>
-  </si>
-  <si>
-    <t>Search56</t>
-  </si>
-  <si>
-    <t>Search57</t>
-  </si>
-  <si>
-    <t>Search58</t>
-  </si>
-  <si>
-    <t>Search59</t>
-  </si>
-  <si>
-    <t>Search60</t>
-  </si>
-  <si>
-    <t>Search61</t>
-  </si>
-  <si>
-    <t>Search62</t>
-  </si>
-  <si>
-    <t>Search63</t>
-  </si>
-  <si>
-    <t>Search64</t>
-  </si>
-  <si>
-    <t>Search65</t>
-  </si>
-  <si>
-    <t>Search66</t>
-  </si>
-  <si>
-    <t>Search67</t>
-  </si>
-  <si>
-    <t>Search68</t>
-  </si>
-  <si>
-    <t>Search69</t>
-  </si>
-  <si>
-    <t>Search70</t>
-  </si>
-  <si>
-    <t>Search71</t>
-  </si>
-  <si>
-    <t>Search72</t>
-  </si>
-  <si>
-    <t>Search73</t>
-  </si>
-  <si>
-    <t>Search74</t>
-  </si>
-  <si>
-    <t>Search75</t>
-  </si>
-  <si>
-    <t>Search76</t>
-  </si>
-  <si>
-    <t>Search77</t>
-  </si>
-  <si>
-    <t>Search78</t>
-  </si>
-  <si>
-    <t>Search79</t>
-  </si>
-  <si>
-    <t>Search80</t>
-  </si>
-  <si>
-    <t>Search81</t>
-  </si>
-  <si>
-    <t>Search82</t>
-  </si>
-  <si>
-    <t>Search83</t>
-  </si>
-  <si>
-    <t>Search84</t>
-  </si>
-  <si>
-    <t>Search85</t>
-  </si>
-  <si>
-    <t>Search86</t>
-  </si>
-  <si>
-    <t>Search87</t>
-  </si>
-  <si>
-    <t>Search88</t>
-  </si>
-  <si>
-    <t>Search89</t>
-  </si>
-  <si>
-    <t>Search90</t>
-  </si>
-  <si>
-    <t>Search91</t>
-  </si>
-  <si>
-    <t>Search92</t>
-  </si>
-  <si>
-    <t>Search93</t>
-  </si>
-  <si>
-    <t>Search94</t>
-  </si>
-  <si>
-    <t>Search95</t>
-  </si>
-  <si>
-    <t>Search96</t>
-  </si>
-  <si>
-    <t>Search97</t>
-  </si>
-  <si>
-    <t>Search98</t>
-  </si>
-  <si>
-    <t>Search99</t>
-  </si>
-  <si>
-    <t>Search100</t>
-  </si>
-  <si>
-    <t>Search101</t>
-  </si>
-  <si>
-    <t>Search102</t>
-  </si>
-  <si>
-    <t>Search103</t>
-  </si>
-  <si>
-    <t>Search104</t>
-  </si>
-  <si>
-    <t>Search105</t>
-  </si>
-  <si>
-    <t>Search106</t>
-  </si>
-  <si>
-    <t>Search107</t>
-  </si>
-  <si>
-    <t>Search108</t>
-  </si>
-  <si>
-    <t>Search109</t>
-  </si>
-  <si>
-    <t>Search110</t>
-  </si>
-  <si>
-    <t>Search111</t>
-  </si>
-  <si>
-    <t>Search112</t>
-  </si>
-  <si>
-    <t>Search113</t>
-  </si>
-  <si>
-    <t>Search114</t>
-  </si>
-  <si>
-    <t>Search115</t>
-  </si>
-  <si>
-    <t>Search116</t>
-  </si>
-  <si>
-    <t>Search117</t>
-  </si>
-  <si>
-    <t>Search118</t>
-  </si>
-  <si>
-    <t>Search119</t>
-  </si>
-  <si>
-    <t>Search120</t>
-  </si>
-  <si>
-    <t>Search121</t>
-  </si>
-  <si>
-    <t>Search122</t>
-  </si>
-  <si>
-    <t>Search123</t>
-  </si>
-  <si>
-    <t>Search124</t>
-  </si>
-  <si>
-    <t>Search125</t>
-  </si>
-  <si>
-    <t>Search126</t>
+    <t>Verify that the following sections get displayed in the search type ahead when user searches using ALL option selected in the Left navigation pane of serach result page and that the searched keyword is present in all the sections:
+a)Autocompleted keyword
+b)4 suggestions in CATEGORY section
+c)4 suggestions in ARTICLES section
+d)4 suggestions in PATENTS section
+e)4 suggestions in POSTS section
+f)4 suggestions in PEOPLE section</t>
+  </si>
+  <si>
+    <t>Verify that sorting is retained when user navigates back to POSTS search results page from record view page
+Verify that Left Navigation content type is retained when user navigates back to POSTS search results page from record view page</t>
   </si>
 </sst>
 </file>
@@ -1733,8 +1733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E121"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+    <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
+      <selection activeCell="C112" sqref="C112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1765,7 +1765,7 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="8" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
@@ -1774,7 +1774,7 @@
         <v>76</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>95</v>
@@ -1782,7 +1782,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="8" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>32</v>
@@ -1791,7 +1791,7 @@
         <v>56</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>95</v>
@@ -1799,7 +1799,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="8" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>33</v>
@@ -1808,7 +1808,7 @@
         <v>57</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>95</v>
@@ -1816,7 +1816,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="8" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>34</v>
@@ -1825,7 +1825,7 @@
         <v>58</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E5" s="8" t="s">
         <v>95</v>
@@ -1833,7 +1833,7 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="8" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>35</v>
@@ -1842,7 +1842,7 @@
         <v>59</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>95</v>
@@ -1850,7 +1850,7 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="8" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>36</v>
@@ -1859,7 +1859,7 @@
         <v>60</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E7" s="8" t="s">
         <v>95</v>
@@ -1867,7 +1867,7 @@
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1">
       <c r="A8" s="8" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>54</v>
@@ -1876,7 +1876,7 @@
         <v>53</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E8" s="8" t="s">
         <v>95</v>
@@ -1884,7 +1884,7 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="8" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>49</v>
@@ -1893,7 +1893,7 @@
         <v>61</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E9" s="8" t="s">
         <v>95</v>
@@ -1901,7 +1901,7 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="8" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>51</v>
@@ -1910,7 +1910,7 @@
         <v>62</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E10" s="8" t="s">
         <v>95</v>
@@ -1918,7 +1918,7 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="8" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>50</v>
@@ -1927,7 +1927,7 @@
         <v>63</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E11" s="8" t="s">
         <v>95</v>
@@ -1935,7 +1935,7 @@
     </row>
     <row r="12" spans="1:5" ht="16.5" customHeight="1">
       <c r="A12" s="8" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>52</v>
@@ -1944,7 +1944,7 @@
         <v>64</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E12" s="8" t="s">
         <v>95</v>
@@ -1952,7 +1952,7 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="8" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>48</v>
@@ -1961,7 +1961,7 @@
         <v>77</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E13" s="8" t="s">
         <v>95</v>
@@ -1969,7 +1969,7 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="8" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>37</v>
@@ -1978,7 +1978,7 @@
         <v>65</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E14" s="8" t="s">
         <v>95</v>
@@ -1986,7 +1986,7 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="8" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>38</v>
@@ -1995,7 +1995,7 @@
         <v>66</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E15" s="8" t="s">
         <v>95</v>
@@ -2003,7 +2003,7 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="8" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>47</v>
@@ -2012,7 +2012,7 @@
         <v>67</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E16" s="8" t="s">
         <v>95</v>
@@ -2020,7 +2020,7 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="8" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>46</v>
@@ -2029,7 +2029,7 @@
         <v>68</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E17" s="8" t="s">
         <v>95</v>
@@ -2037,7 +2037,7 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="8" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>55</v>
@@ -2046,7 +2046,7 @@
         <v>90</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E18" s="8" t="s">
         <v>95</v>
@@ -2054,7 +2054,7 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="8" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>45</v>
@@ -2063,7 +2063,7 @@
         <v>69</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E19" s="8" t="s">
         <v>95</v>
@@ -2071,7 +2071,7 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="8" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>44</v>
@@ -2080,7 +2080,7 @@
         <v>70</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E20" s="8" t="s">
         <v>95</v>
@@ -2088,7 +2088,7 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="8" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="B21" s="7" t="s">
         <v>43</v>
@@ -2097,7 +2097,7 @@
         <v>71</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E21" s="8" t="s">
         <v>95</v>
@@ -2105,7 +2105,7 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="8" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>39</v>
@@ -2114,7 +2114,7 @@
         <v>72</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E22" s="8" t="s">
         <v>95</v>
@@ -2122,7 +2122,7 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="8" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B23" s="7" t="s">
         <v>40</v>
@@ -2131,7 +2131,7 @@
         <v>73</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E23" s="8" t="s">
         <v>95</v>
@@ -2139,7 +2139,7 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="8" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="B24" s="7" t="s">
         <v>41</v>
@@ -2148,7 +2148,7 @@
         <v>74</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E24" s="8" t="s">
         <v>95</v>
@@ -2156,7 +2156,7 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="8" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="B25" s="7" t="s">
         <v>42</v>
@@ -2165,7 +2165,7 @@
         <v>75</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E25" s="8" t="s">
         <v>95</v>
@@ -2173,16 +2173,16 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="8" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>78</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E26" s="8" t="s">
         <v>95</v>
@@ -2190,16 +2190,16 @@
     </row>
     <row r="27" spans="1:5" ht="75">
       <c r="A27" s="8" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C27" s="7" t="s">
         <v>79</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E27" s="8" t="s">
         <v>95</v>
@@ -2207,16 +2207,16 @@
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="8" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C28" s="8" t="s">
         <v>80</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E28" s="8" t="s">
         <v>95</v>
@@ -2224,16 +2224,16 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="8" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C29" s="8" t="s">
         <v>81</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E29" s="8" t="s">
         <v>95</v>
@@ -2241,16 +2241,16 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="8" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="C30" s="8" t="s">
         <v>82</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E30" s="8" t="s">
         <v>95</v>
@@ -2258,16 +2258,16 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="8" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C31" s="8" t="s">
         <v>83</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E31" s="8" t="s">
         <v>95</v>
@@ -2275,16 +2275,16 @@
     </row>
     <row r="32" spans="1:5" ht="90">
       <c r="A32" s="8" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="C32" s="7" t="s">
         <v>84</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E32" s="8" t="s">
         <v>95</v>
@@ -2292,16 +2292,16 @@
     </row>
     <row r="33" spans="1:5" ht="60">
       <c r="A33" s="8" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C33" s="7" t="s">
         <v>85</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E33" s="8" t="s">
         <v>95</v>
@@ -2309,16 +2309,16 @@
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="8" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C34" s="7" t="s">
         <v>86</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E34" s="8" t="s">
         <v>95</v>
@@ -2326,16 +2326,16 @@
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="8" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C35" s="7" t="s">
         <v>87</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E35" s="8" t="s">
         <v>95</v>
@@ -2343,16 +2343,16 @@
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="8" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="C36" s="8" t="s">
         <v>88</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E36" s="8" t="s">
         <v>95</v>
@@ -2360,16 +2360,16 @@
     </row>
     <row r="37" spans="1:5" ht="90">
       <c r="A37" s="8" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C37" s="7" t="s">
         <v>89</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E37" s="8" t="s">
         <v>95</v>
@@ -2377,16 +2377,16 @@
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="8" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C38" s="8" t="s">
         <v>90</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E38" s="8" t="s">
         <v>95</v>
@@ -2394,16 +2394,16 @@
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="8" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C39" s="8" t="s">
         <v>91</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E39" s="8" t="s">
         <v>95</v>
@@ -2411,16 +2411,16 @@
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="8" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C40" s="8" t="s">
         <v>92</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E40" s="8" t="s">
         <v>95</v>
@@ -2428,16 +2428,16 @@
     </row>
     <row r="41" spans="1:5" ht="90">
       <c r="A41" s="8" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C41" s="7" t="s">
         <v>93</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E41" s="8" t="s">
         <v>95</v>
@@ -2445,16 +2445,16 @@
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="8" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C42" s="7" t="s">
         <v>94</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E42" s="8" t="s">
         <v>95</v>
@@ -2462,16 +2462,16 @@
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="8" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C43" s="7" t="s">
         <v>96</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E43" s="8" t="s">
         <v>95</v>
@@ -2479,16 +2479,16 @@
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="8" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="C44" s="7" t="s">
         <v>97</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E44" s="8" t="s">
         <v>95</v>
@@ -2496,16 +2496,16 @@
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="8" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C45" s="7" t="s">
         <v>98</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E45" s="8" t="s">
         <v>95</v>
@@ -2513,7 +2513,7 @@
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="8" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B46" s="7" t="s">
         <v>46</v>
@@ -2522,7 +2522,7 @@
         <v>99</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E46" s="8" t="s">
         <v>95</v>
@@ -2530,7 +2530,7 @@
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="8" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="B47" s="7" t="s">
         <v>55</v>
@@ -2539,7 +2539,7 @@
         <v>100</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E47" s="8" t="s">
         <v>95</v>
@@ -2547,7 +2547,7 @@
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="8" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="B48" s="7" t="s">
         <v>102</v>
@@ -2556,7 +2556,7 @@
         <v>101</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E48" s="8" t="s">
         <v>95</v>
@@ -2564,7 +2564,7 @@
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="8" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="B49" s="7" t="s">
         <v>103</v>
@@ -2573,7 +2573,7 @@
         <v>104</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E49" s="8" t="s">
         <v>95</v>
@@ -2581,7 +2581,7 @@
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="8" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="B50" s="7" t="s">
         <v>48</v>
@@ -2590,7 +2590,7 @@
         <v>105</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E50" s="8" t="s">
         <v>95</v>
@@ -2598,7 +2598,7 @@
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="8" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="B51" s="7" t="s">
         <v>52</v>
@@ -2607,7 +2607,7 @@
         <v>106</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E51" s="8" t="s">
         <v>95</v>
@@ -2615,7 +2615,7 @@
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="8" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="B52" s="7" t="s">
         <v>108</v>
@@ -2624,7 +2624,7 @@
         <v>107</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E52" s="8" t="s">
         <v>95</v>
@@ -2632,16 +2632,16 @@
     </row>
     <row r="53" spans="1:5" ht="120">
       <c r="A53" s="8" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="B53" s="7" t="s">
         <v>109</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>110</v>
+        <v>382</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E53" s="8" t="s">
         <v>95</v>
@@ -2649,16 +2649,16 @@
     </row>
     <row r="54" spans="1:5" ht="30">
       <c r="A54" s="8" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="B54" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="C54" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="C54" s="7" t="s">
-        <v>112</v>
-      </c>
       <c r="D54" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E54" s="8" t="s">
         <v>95</v>
@@ -2666,16 +2666,16 @@
     </row>
     <row r="55" spans="1:5" ht="30">
       <c r="A55" s="8" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="B55" s="7" t="s">
         <v>49</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E55" s="8" t="s">
         <v>95</v>
@@ -2683,16 +2683,16 @@
     </row>
     <row r="56" spans="1:5" ht="30">
       <c r="A56" s="8" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="B56" s="7" t="s">
         <v>51</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E56" s="8" t="s">
         <v>95</v>
@@ -2700,16 +2700,16 @@
     </row>
     <row r="57" spans="1:5" ht="30">
       <c r="A57" s="8" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E57" s="8" t="s">
         <v>95</v>
@@ -2717,7 +2717,7 @@
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="8" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B58" s="7" t="s">
         <v>54</v>
@@ -2726,7 +2726,7 @@
         <v>53</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E58" s="8" t="s">
         <v>95</v>
@@ -2734,16 +2734,16 @@
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="8" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E59" s="8" t="s">
         <v>95</v>
@@ -2751,16 +2751,16 @@
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="8" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E60" s="8" t="s">
         <v>95</v>
@@ -2768,16 +2768,16 @@
     </row>
     <row r="61" spans="1:5">
       <c r="A61" s="8" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="B61" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="C61" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="C61" s="7" t="s">
-        <v>122</v>
-      </c>
       <c r="D61" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E61" s="8" t="s">
         <v>95</v>
@@ -2785,16 +2785,16 @@
     </row>
     <row r="62" spans="1:5">
       <c r="A62" s="8" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E62" s="8" t="s">
         <v>95</v>
@@ -2802,16 +2802,16 @@
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="8" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="B63" s="7" t="s">
         <v>43</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D63" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E63" s="8" t="s">
         <v>95</v>
@@ -2819,16 +2819,16 @@
     </row>
     <row r="64" spans="1:5" ht="45">
       <c r="A64" s="8" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="B64" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="C64" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="C64" s="7" t="s">
-        <v>127</v>
-      </c>
       <c r="D64" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E64" s="8" t="s">
         <v>95</v>
@@ -2836,16 +2836,16 @@
     </row>
     <row r="65" spans="1:5" ht="30">
       <c r="A65" s="8" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C65" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D65" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E65" s="8" t="s">
         <v>95</v>
@@ -2853,16 +2853,16 @@
     </row>
     <row r="66" spans="1:5" ht="30">
       <c r="A66" s="8" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="B66" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="C66" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="C66" s="7" t="s">
-        <v>131</v>
-      </c>
       <c r="D66" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E66" s="8" t="s">
         <v>95</v>
@@ -2870,16 +2870,16 @@
     </row>
     <row r="67" spans="1:5" ht="30">
       <c r="A67" s="8" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C67" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D67" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E67" s="8" t="s">
         <v>95</v>
@@ -2887,16 +2887,16 @@
     </row>
     <row r="68" spans="1:5" ht="30">
       <c r="A68" s="8" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="B68" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="C68" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="C68" s="7" t="s">
-        <v>135</v>
-      </c>
       <c r="D68" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E68" s="8" t="s">
         <v>95</v>
@@ -2904,16 +2904,16 @@
     </row>
     <row r="69" spans="1:5" ht="30">
       <c r="A69" s="8" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="B69" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C69" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="C69" s="7" t="s">
-        <v>137</v>
-      </c>
       <c r="D69" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E69" s="8" t="s">
         <v>95</v>
@@ -2921,16 +2921,16 @@
     </row>
     <row r="70" spans="1:5" ht="30">
       <c r="A70" s="8" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="B70" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="C70" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="C70" s="7" t="s">
-        <v>139</v>
-      </c>
       <c r="D70" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E70" s="8" t="s">
         <v>95</v>
@@ -2938,16 +2938,16 @@
     </row>
     <row r="71" spans="1:5" ht="30">
       <c r="A71" s="8" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D71" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E71" s="8" t="s">
         <v>95</v>
@@ -2955,16 +2955,16 @@
     </row>
     <row r="72" spans="1:5" ht="30">
       <c r="A72" s="8" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D72" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E72" s="8" t="s">
         <v>95</v>
@@ -2972,16 +2972,16 @@
     </row>
     <row r="73" spans="1:5">
       <c r="A73" s="8" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="B73" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="C73" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="C73" s="7" t="s">
-        <v>145</v>
-      </c>
       <c r="D73" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E73" s="8" t="s">
         <v>95</v>
@@ -2989,16 +2989,16 @@
     </row>
     <row r="74" spans="1:5" ht="90">
       <c r="A74" s="8" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="B74" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="C74" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="C74" s="7" t="s">
-        <v>147</v>
-      </c>
       <c r="D74" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E74" s="8" t="s">
         <v>95</v>
@@ -3006,16 +3006,16 @@
     </row>
     <row r="75" spans="1:5" ht="60">
       <c r="A75" s="8" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C75" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D75" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E75" s="8" t="s">
         <v>95</v>
@@ -3023,16 +3023,16 @@
     </row>
     <row r="76" spans="1:5">
       <c r="A76" s="8" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="B76" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="C76" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="C76" s="7" t="s">
-        <v>151</v>
-      </c>
       <c r="D76" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E76" s="8" t="s">
         <v>95</v>
@@ -3040,16 +3040,16 @@
     </row>
     <row r="77" spans="1:5">
       <c r="A77" s="8" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="B77" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="C77" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="C77" s="7" t="s">
-        <v>153</v>
-      </c>
       <c r="D77" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E77" s="8" t="s">
         <v>95</v>
@@ -3057,16 +3057,16 @@
     </row>
     <row r="78" spans="1:5">
       <c r="A78" s="8" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C78" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D78" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E78" s="8" t="s">
         <v>95</v>
@@ -3074,16 +3074,16 @@
     </row>
     <row r="79" spans="1:5" ht="120">
       <c r="A79" s="8" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C79" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D79" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E79" s="8" t="s">
         <v>95</v>
@@ -3091,16 +3091,16 @@
     </row>
     <row r="80" spans="1:5" ht="120">
       <c r="A80" s="8" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C80" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D80" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E80" s="8" t="s">
         <v>95</v>
@@ -3108,16 +3108,16 @@
     </row>
     <row r="81" spans="1:5" ht="195">
       <c r="A81" s="8" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="B81" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C81" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D81" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E81" s="8" t="s">
         <v>95</v>
@@ -3125,16 +3125,16 @@
     </row>
     <row r="82" spans="1:5">
       <c r="A82" s="8" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="B82" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C82" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D82" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E82" s="8" t="s">
         <v>95</v>
@@ -3142,16 +3142,16 @@
     </row>
     <row r="83" spans="1:5">
       <c r="A83" s="8" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C83" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D83" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E83" s="8" t="s">
         <v>95</v>
@@ -3159,16 +3159,16 @@
     </row>
     <row r="84" spans="1:5">
       <c r="A84" s="8" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="B84" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="C84" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="C84" s="7" t="s">
-        <v>167</v>
-      </c>
       <c r="D84" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E84" s="8" t="s">
         <v>95</v>
@@ -3176,16 +3176,16 @@
     </row>
     <row r="85" spans="1:5" ht="30">
       <c r="A85" s="8" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C85" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D85" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E85" s="8" t="s">
         <v>95</v>
@@ -3193,16 +3193,16 @@
     </row>
     <row r="86" spans="1:5">
       <c r="A86" s="8" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="B86" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="C86" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="C86" s="7" t="s">
-        <v>171</v>
-      </c>
       <c r="D86" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E86" s="8" t="s">
         <v>95</v>
@@ -3210,16 +3210,16 @@
     </row>
     <row r="87" spans="1:5">
       <c r="A87" s="8" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="B87" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C87" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D87" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E87" s="8" t="s">
         <v>95</v>
@@ -3227,16 +3227,16 @@
     </row>
     <row r="88" spans="1:5">
       <c r="A88" s="8" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="B88" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="C88" s="8" t="s">
         <v>175</v>
       </c>
-      <c r="C88" s="8" t="s">
-        <v>176</v>
-      </c>
       <c r="D88" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E88" s="8" t="s">
         <v>95</v>
@@ -3244,16 +3244,16 @@
     </row>
     <row r="89" spans="1:5">
       <c r="A89" s="8" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C89" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D89" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E89" s="8" t="s">
         <v>95</v>
@@ -3261,16 +3261,16 @@
     </row>
     <row r="90" spans="1:5" ht="105">
       <c r="A90" s="8" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C90" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D90" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E90" s="8" t="s">
         <v>95</v>
@@ -3278,16 +3278,16 @@
     </row>
     <row r="91" spans="1:5" ht="105">
       <c r="A91" s="8" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C91" s="7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D91" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E91" s="8" t="s">
         <v>95</v>
@@ -3295,16 +3295,16 @@
     </row>
     <row r="92" spans="1:5">
       <c r="A92" s="8" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="B92" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="C92" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="C92" s="7" t="s">
-        <v>184</v>
-      </c>
       <c r="D92" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E92" s="8" t="s">
         <v>95</v>
@@ -3312,16 +3312,16 @@
     </row>
     <row r="93" spans="1:5">
       <c r="A93" s="8" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="B93" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="C93" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="C93" s="7" t="s">
-        <v>186</v>
-      </c>
       <c r="D93" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E93" s="8" t="s">
         <v>95</v>
@@ -3329,16 +3329,16 @@
     </row>
     <row r="94" spans="1:5" ht="45">
       <c r="A94" s="8" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C94" s="7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D94" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E94" s="8" t="s">
         <v>95</v>
@@ -3346,16 +3346,16 @@
     </row>
     <row r="95" spans="1:5">
       <c r="A95" s="8" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="B95" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="C95" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="C95" s="8" t="s">
-        <v>190</v>
-      </c>
       <c r="D95" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E95" s="8" t="s">
         <v>95</v>
@@ -3363,16 +3363,16 @@
     </row>
     <row r="96" spans="1:5">
       <c r="A96" s="8" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="B96" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="C96" s="8" t="s">
         <v>191</v>
       </c>
-      <c r="C96" s="8" t="s">
-        <v>192</v>
-      </c>
       <c r="D96" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E96" s="8" t="s">
         <v>95</v>
@@ -3380,16 +3380,16 @@
     </row>
     <row r="97" spans="1:5">
       <c r="A97" s="8" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="B97" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="C97" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="C97" s="8" t="s">
-        <v>194</v>
-      </c>
       <c r="D97" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E97" s="8" t="s">
         <v>95</v>
@@ -3397,16 +3397,16 @@
     </row>
     <row r="98" spans="1:5">
       <c r="A98" s="8" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="B98" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="C98" s="8" t="s">
         <v>195</v>
       </c>
-      <c r="C98" s="8" t="s">
-        <v>196</v>
-      </c>
       <c r="D98" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E98" s="8" t="s">
         <v>95</v>
@@ -3414,16 +3414,16 @@
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="8" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="B99" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="C99" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="C99" s="8" t="s">
-        <v>198</v>
-      </c>
       <c r="D99" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E99" s="8" t="s">
         <v>95</v>
@@ -3431,16 +3431,16 @@
     </row>
     <row r="100" spans="1:5" ht="165">
       <c r="A100" s="8" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="B100" s="8" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C100" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D100" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E100" s="8" t="s">
         <v>95</v>
@@ -3448,16 +3448,16 @@
     </row>
     <row r="101" spans="1:5" ht="75">
       <c r="A101" s="8" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="B101" s="9" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C101" s="7" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D101" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E101" s="8" t="s">
         <v>95</v>
@@ -3465,16 +3465,16 @@
     </row>
     <row r="102" spans="1:5">
       <c r="A102" s="8" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="B102" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="C102" s="7" t="s">
         <v>201</v>
       </c>
-      <c r="C102" s="7" t="s">
-        <v>202</v>
-      </c>
       <c r="D102" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E102" s="8" t="s">
         <v>95</v>
@@ -3482,16 +3482,16 @@
     </row>
     <row r="103" spans="1:5">
       <c r="A103" s="8" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="B103" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="C103" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="C103" s="7" t="s">
-        <v>204</v>
-      </c>
       <c r="D103" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E103" s="8" t="s">
         <v>95</v>
@@ -3499,16 +3499,16 @@
     </row>
     <row r="104" spans="1:5">
       <c r="A104" s="8" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="B104" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="C104" s="8" t="s">
         <v>207</v>
       </c>
-      <c r="C104" s="8" t="s">
-        <v>208</v>
-      </c>
       <c r="D104" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E104" s="8" t="s">
         <v>95</v>
@@ -3516,16 +3516,16 @@
     </row>
     <row r="105" spans="1:5">
       <c r="A105" s="8" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="B105" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="C105" s="8" t="s">
         <v>205</v>
       </c>
-      <c r="C105" s="8" t="s">
-        <v>206</v>
-      </c>
       <c r="D105" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E105" s="8" t="s">
         <v>95</v>
@@ -3533,16 +3533,16 @@
     </row>
     <row r="106" spans="1:5">
       <c r="A106" s="8" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="B106" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="C106" s="8" t="s">
         <v>209</v>
       </c>
-      <c r="C106" s="8" t="s">
-        <v>210</v>
-      </c>
       <c r="D106" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E106" s="8" t="s">
         <v>95</v>
@@ -3550,16 +3550,16 @@
     </row>
     <row r="107" spans="1:5">
       <c r="A107" s="8" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="B107" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C107" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D107" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E107" s="8" t="s">
         <v>95</v>
@@ -3567,16 +3567,16 @@
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="8" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="B108" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="C108" s="8" t="s">
         <v>213</v>
       </c>
-      <c r="C108" s="8" t="s">
-        <v>214</v>
-      </c>
       <c r="D108" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E108" s="8" t="s">
         <v>95</v>
@@ -3584,16 +3584,16 @@
     </row>
     <row r="109" spans="1:5">
       <c r="A109" s="8" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="B109" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="C109" s="8" t="s">
         <v>215</v>
       </c>
-      <c r="C109" s="8" t="s">
-        <v>216</v>
-      </c>
       <c r="D109" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E109" s="8" t="s">
         <v>95</v>
@@ -3601,16 +3601,16 @@
     </row>
     <row r="110" spans="1:5">
       <c r="A110" s="8" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="B110" s="8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C110" s="8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D110" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E110" s="8" t="s">
         <v>95</v>
@@ -3618,16 +3618,16 @@
     </row>
     <row r="111" spans="1:5">
       <c r="A111" s="8" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="B111" s="9" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C111" s="9" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D111" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E111" s="8" t="s">
         <v>95</v>
@@ -3635,16 +3635,16 @@
     </row>
     <row r="112" spans="1:5" ht="30">
       <c r="A112" s="8" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="B112" s="9" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C112" s="10" t="s">
-        <v>223</v>
+        <v>383</v>
       </c>
       <c r="D112" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E112" s="8" t="s">
         <v>95</v>
@@ -3652,16 +3652,16 @@
     </row>
     <row r="113" spans="1:5" ht="75">
       <c r="A113" s="8" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="B113" s="8" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C113" s="7" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D113" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E113" s="8" t="s">
         <v>95</v>
@@ -3669,16 +3669,16 @@
     </row>
     <row r="114" spans="1:5" ht="60">
       <c r="A114" s="8" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="B114" s="7" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C114" s="7" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D114" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E114" s="8" t="s">
         <v>95</v>
@@ -3686,16 +3686,16 @@
     </row>
     <row r="115" spans="1:5" ht="105">
       <c r="A115" s="8" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="B115" s="7" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C115" s="7" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D115" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E115" s="8" t="s">
         <v>95</v>
@@ -3703,16 +3703,16 @@
     </row>
     <row r="116" spans="1:5" ht="105">
       <c r="A116" s="8" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="B116" s="7" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C116" s="7" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D116" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E116" s="8" t="s">
         <v>95</v>
@@ -3720,16 +3720,16 @@
     </row>
     <row r="117" spans="1:5">
       <c r="A117" s="8" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="B117" s="7" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C117" s="8" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D117" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E117" s="8" t="s">
         <v>95</v>
@@ -3737,63 +3737,63 @@
     </row>
     <row r="118" spans="1:5">
       <c r="A118" s="8" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="B118" s="7" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C118" s="3" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D118" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E118" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="119" spans="1:5">
       <c r="A119" s="8" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C119" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D119" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E119" s="3"/>
     </row>
     <row r="120" spans="1:5">
       <c r="A120" s="8" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C120" s="3" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D120" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E120" s="3"/>
     </row>
     <row r="121" spans="1:5" ht="150">
       <c r="A121" s="8" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C121" s="4" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D121" s="8" t="s">
-        <v>243</v>
+        <v>381</v>
       </c>
       <c r="E121" s="3"/>
     </row>

</xml_diff>

<commit_message>
Modified Search.xls and changed few test description
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Search.xlsx
+++ b/src/test/resources/xls/Search.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="346">
   <si>
     <t>TCID</t>
   </si>
@@ -200,24 +200,12 @@
     <t>OPQA-274</t>
   </si>
   <si>
-    <t>OPQA-279</t>
-  </si>
-  <si>
     <t>OPQA-358</t>
   </si>
   <si>
-    <t>OPQA-366</t>
-  </si>
-  <si>
-    <t>OPQA-362</t>
-  </si>
-  <si>
     <t>OPQA-368</t>
   </si>
   <si>
-    <t>OPQA-371</t>
-  </si>
-  <si>
     <t>OPQA-744</t>
   </si>
   <si>
@@ -248,15 +236,9 @@
     <t>Verify that number of displayed documents gets increased as and when user scrolls down the search results page</t>
   </si>
   <si>
-    <t>Verify that sorting is retained when user navigates back to search results page from record view page</t>
-  </si>
-  <si>
     <t>Verify that filtering is retained when user navigates back to search results page from record view page</t>
   </si>
   <si>
-    <t>Verify that sorting and filtering are retained when user navigates back to search results page from record view page</t>
-  </si>
-  <si>
     <t>Verify that NOT is not treated as a boolean</t>
   </si>
   <si>
@@ -291,9 +273,6 @@
   </si>
   <si>
     <t>Verify that MINIMUM SHOULD MATCH rule is working correctly</t>
-  </si>
-  <si>
-    <t>Verify that ALL content type count is equal to the sum of the counts of other content types</t>
   </si>
   <si>
     <t>Verify that autocomplete feature is working correctly</t>
@@ -381,69 +360,24 @@
     <t>Verify that user is able to expand and collapse the Institutions filter in ARTICLES content type</t>
   </si>
   <si>
-    <t>Verify that user is able to select any of the content types present in search drop down</t>
-  </si>
-  <si>
-    <t>Verify that ALL option is selected in the left navigation pane by default when user searches using ALL option in the search drop down</t>
-  </si>
-  <si>
-    <t>Verify that search results related to all content types get displayed in the summary page when user searches using ALL option in search drop down</t>
-  </si>
-  <si>
     <t>OPQA-301</t>
   </si>
   <si>
     <t>OPQA-316</t>
   </si>
   <si>
-    <t>Verify that only articles get displayed in the summary page when user searches using ARTICLES content type in search drop down</t>
-  </si>
-  <si>
-    <t>Verify that only patents get displayed in the summary page when user searches using PATENTS content type in search drop down</t>
-  </si>
-  <si>
-    <t>Verify that only posts get displayed in the summary page when user searches using POSTS content type in search drop down</t>
-  </si>
-  <si>
-    <t>Verify that only people get displayed in the summary page when user searches using people content type in search drop down</t>
-  </si>
-  <si>
     <t>OPQA-380</t>
   </si>
   <si>
     <t>OPQA-287</t>
   </si>
   <si>
-    <t>OPQA-311</t>
-  </si>
-  <si>
-    <t>Verify that 10 article suggestions get displayed in the search type ahead when user searches using ARTICLES option in the search drop down and that the searched keyword is present in all the suggestions</t>
-  </si>
-  <si>
-    <t>Verify that 10 patent suggestions get displayed in the search type ahead when user searches using PATENTS option in the search drop down and that the searched keyword is present in all the suggestions</t>
-  </si>
-  <si>
-    <t>Verify that 10 post suggestions get displayed in the search type ahead when user searches using POSTS option in the search drop down and that the searched keyword is present in all the suggestions</t>
-  </si>
-  <si>
-    <t>Verify that 10 people suggestions get displayed in the search type ahead when user searches using PEOPLE option in the search drop down and that the searched keyword is present in all the suggestions</t>
-  </si>
-  <si>
-    <t>OPQA-378</t>
-  </si>
-  <si>
-    <t>OPQA-557</t>
-  </si>
-  <si>
     <t>Verify that the searched keyword doesn't change in the search text box if any other content type is selected in the left navigation pane</t>
   </si>
   <si>
     <t>OPQA-386</t>
   </si>
   <si>
-    <t>Verify that the searched keyword present in the search text box doesn't change if any other content type is selected in the search drop down</t>
-  </si>
-  <si>
     <t>OPQA-387</t>
   </si>
   <si>
@@ -462,59 +396,18 @@
     <t>OPQA-384</t>
   </si>
   <si>
-    <t>Verify that the following changes take place when user switches over to any other content type in the left navigation pane:
-a)Search results related to the switched content type get displayed in the summary page
-b)Search drop down option gets changed automatically to the switched content type</t>
-  </si>
-  <si>
-    <t>Verify that record view of an article gets displayed when user clicks on any article option in the search type ahead while ALL option is selected in the search drop down</t>
-  </si>
-  <si>
     <t>OPQA-396</t>
   </si>
   <si>
     <t>OPQA-398</t>
   </si>
   <si>
-    <t>Verify that record view of a patent gets displayed when user clicks on any patent option in the search type ahead while ALL option is selected in the search drop down</t>
-  </si>
-  <si>
-    <t>Verify that record view of a post gets displayed when user clicks on any post option in the search type ahead while ALL option is selected in the search drop down</t>
-  </si>
-  <si>
     <t>OPQA-401</t>
   </si>
   <si>
     <t>OPQA-402</t>
   </si>
   <si>
-    <t>Verify that profile page of a person gets displayed when user clicks on any PEOPLE option in the search type ahead while ALL option is selected in the search drop down</t>
-  </si>
-  <si>
-    <t>OPQA-403</t>
-  </si>
-  <si>
-    <t>Verify that record view of an article gets displayed when user clicks on any article option in the search type ahead while ARTICLES option is selected in the search drop down</t>
-  </si>
-  <si>
-    <t>OPQA-404</t>
-  </si>
-  <si>
-    <t>Verify that record view of a patent gets displayed when user clicks on any patent option in the search type ahead while PATENTS option is selected in the search drop down</t>
-  </si>
-  <si>
-    <t>Verify that record view of a post gets displayed when user clicks on any post option in the search type ahead while POSTS option is selected in the search drop down</t>
-  </si>
-  <si>
-    <t>OPQA-407</t>
-  </si>
-  <si>
-    <t>Verify that profile page of a person gets displayed when user clicks on any PEOPLE option in the search type ahead while PEOPLE option is selected in the search drop down</t>
-  </si>
-  <si>
-    <t>OPQA-409</t>
-  </si>
-  <si>
     <t>OPQA-412</t>
   </si>
   <si>
@@ -522,19 +415,6 @@
   </si>
   <si>
     <t>OPQA-392</t>
-  </si>
-  <si>
-    <t>Verify that the following changes take place when user clicks on any CATEGORIES option in the search type ahead while ALL option is selected in the search drop down:
-a)Correct keyword gets displayed in the search box
-b)ARTICLES option gets selected both in the search drop down and left navigation pane
-c)Only articles get displayed in the search results page
-d)Correct category gets selected in CATEGORIES filter in the left navigation pane with filter in expanded state</t>
-  </si>
-  <si>
-    <t>Verify that following options get displayed in SORT BY drop down in ALL search results page:
-a)Relevance
-b)Times Cited
-c)Date</t>
   </si>
   <si>
     <t>OPQA-413</t>
@@ -602,9 +482,6 @@
     <t>OPQA-562</t>
   </si>
   <si>
-    <t>Verify that record view page of a patent gets displayed when user clicks on article title in ALL search results page</t>
-  </si>
-  <si>
     <t>Verify that record view page of a patent gets displayed when user clicks a patent title in PATENTS search results page</t>
   </si>
   <si>
@@ -790,12 +667,6 @@
     <t>Verify that left navigation pane content type is retained when user navigates back to PATENTS search results page from record view page</t>
   </si>
   <si>
-    <t>Verify that search drop down content type is retained when user navigates back to PEOPLE search results page from profile page</t>
-  </si>
-  <si>
-    <t>OPQA-1244</t>
-  </si>
-  <si>
     <t>Verify that following options get displayed in SORT BY drop down in POSTS search results page: 
 a)Relevance 
 b)Create Date(Newest) 
@@ -981,18 +852,9 @@
     <t>Search8</t>
   </si>
   <si>
-    <t>Search9</t>
-  </si>
-  <si>
     <t>Search10</t>
   </si>
   <si>
-    <t>Search11</t>
-  </si>
-  <si>
-    <t>Search12</t>
-  </si>
-  <si>
     <t>Search13</t>
   </si>
   <si>
@@ -1089,12 +951,6 @@
     <t>Search44</t>
   </si>
   <si>
-    <t>Search47</t>
-  </si>
-  <si>
-    <t>Search48</t>
-  </si>
-  <si>
     <t>Search49</t>
   </si>
   <si>
@@ -1113,24 +969,9 @@
     <t>Search58</t>
   </si>
   <si>
-    <t>Search59</t>
-  </si>
-  <si>
-    <t>Search60</t>
-  </si>
-  <si>
-    <t>Search61</t>
-  </si>
-  <si>
-    <t>Search62</t>
-  </si>
-  <si>
     <t>Search63</t>
   </si>
   <si>
-    <t>Search64</t>
-  </si>
-  <si>
     <t>Search65</t>
   </si>
   <si>
@@ -1158,18 +999,6 @@
     <t>Search73</t>
   </si>
   <si>
-    <t>Search74</t>
-  </si>
-  <si>
-    <t>Search75</t>
-  </si>
-  <si>
-    <t>Search76</t>
-  </si>
-  <si>
-    <t>Search77</t>
-  </si>
-  <si>
     <t>Search78</t>
   </si>
   <si>
@@ -1279,9 +1108,6 @@
   </si>
   <si>
     <t>Search114</t>
-  </si>
-  <si>
-    <t>Search115</t>
   </si>
   <si>
     <t>Search116</t>
@@ -1331,6 +1157,66 @@
   <si>
     <t>Verify that sorting is retained when user navigates back to POSTS search results page from record view page
 Verify that Left Navigation content type is retained when user navigates back to POSTS search results page from record view page</t>
+  </si>
+  <si>
+    <t>OPQA-2899</t>
+  </si>
+  <si>
+    <t>OPQA-2900</t>
+  </si>
+  <si>
+    <t>Verify that only patents get displayed in the summary page when user searches using PATENTS  as content type in Left Navigation pane</t>
+  </si>
+  <si>
+    <t>Verify that only articles get displayed in the summary page when user searches using ARTICLES as content type in Left navigation pane</t>
+  </si>
+  <si>
+    <t>Verify that only posts get displayed in the summary page when user selects post content type in left navigation pane</t>
+  </si>
+  <si>
+    <t>Verify that only people get displayed in the summary page when user searches using people as content type in left navigation pane</t>
+  </si>
+  <si>
+    <t>Verify that search results related to all content types get displayed in the summary page when user searches using ALL option in Left navigation pane</t>
+  </si>
+  <si>
+    <t>OPQA-2908</t>
+  </si>
+  <si>
+    <t>OPQA-2918</t>
+  </si>
+  <si>
+    <t>Verify that the following changes take place when user switches over to any other content type in the left navigation pane:
+a)Search results related to the switched content type get displayed in the summary page</t>
+  </si>
+  <si>
+    <t>Verify that the following changes take place when user clicks on any CATEGORIES option in the search type ahead while ALL option is selected in the search drop down:
+a)Correct keyword gets displayed in the search box
+b)ARTICLES option gets selected both in the  left navigation pane
+c)Only articles get displayed in the search results page
+d)Correct category gets selected in CATEGORIES filter in the left navigation pane with filter in expanded state</t>
+  </si>
+  <si>
+    <t>Verify that following options get displayed in SORT BY drop down in ALL search results page:
+a)Relevance
+b)Times Cited
+c)Date(Newest)
+d)Date(Oldest)</t>
+  </si>
+  <si>
+    <t>Verify that record view page of a artcle gets displayed when user clicks on article title in ALL search results page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that record view of a patent gets displayed when user clicks on any patent option in the search type ahead </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that record view of a post gets displayed when user clicks on any post option in the search type ahead </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that profile page of a person gets displayed when user clicks on any PEOPLE option in the search type ahead </t>
+  </si>
+  <si>
+    <t>Verify that record view of an article gets displayed when user clicks on any article option in the search type ahead</t>
   </si>
 </sst>
 </file>
@@ -1731,10 +1617,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E121"/>
+  <dimension ref="A1:E106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
-      <selection activeCell="C112" sqref="C112"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1765,2037 +1651,1782 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="8" t="s">
-        <v>261</v>
+        <v>221</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="8" t="s">
-        <v>262</v>
+        <v>222</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>32</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="8" t="s">
-        <v>263</v>
+        <v>223</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>33</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="8" t="s">
-        <v>264</v>
+        <v>224</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>34</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="8" t="s">
-        <v>265</v>
+        <v>225</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>35</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="8" t="s">
-        <v>266</v>
+        <v>226</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>36</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1">
       <c r="A8" s="8" t="s">
-        <v>267</v>
+        <v>227</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="8" t="s">
-        <v>268</v>
+        <v>228</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>49</v>
+        <v>329</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="8" t="s">
-        <v>269</v>
+        <v>229</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="8" t="s">
-        <v>270</v>
+        <v>230</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="16.5" customHeight="1">
       <c r="A12" s="8" t="s">
-        <v>271</v>
+        <v>231</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="8" t="s">
-        <v>272</v>
+        <v>232</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="8" t="s">
-        <v>273</v>
+        <v>233</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>65</v>
+        <v>330</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>62</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="8" t="s">
-        <v>274</v>
+        <v>234</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>66</v>
+        <v>51</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="8" t="s">
-        <v>275</v>
+        <v>235</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="8" t="s">
-        <v>276</v>
+        <v>236</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="8" t="s">
-        <v>277</v>
+        <v>237</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>90</v>
+        <v>65</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="8" t="s">
-        <v>278</v>
+        <v>238</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>69</v>
+        <v>39</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>66</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="8" t="s">
-        <v>279</v>
+        <v>239</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>70</v>
+        <v>40</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>67</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="8" t="s">
-        <v>280</v>
+        <v>240</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>71</v>
+        <v>41</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>68</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="8" t="s">
-        <v>281</v>
+        <v>241</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="8" t="s">
-        <v>282</v>
+        <v>242</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>73</v>
+        <v>201</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>71</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="75">
       <c r="A24" s="8" t="s">
-        <v>283</v>
+        <v>243</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>41</v>
+        <v>202</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="8" t="s">
-        <v>284</v>
+        <v>244</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>75</v>
+        <v>203</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>73</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="8" t="s">
-        <v>285</v>
+        <v>245</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>241</v>
+        <v>204</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="75">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
       <c r="A27" s="8" t="s">
-        <v>286</v>
+        <v>246</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>242</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>79</v>
+        <v>205</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>75</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="8" t="s">
-        <v>287</v>
+        <v>247</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>243</v>
+        <v>206</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="90">
       <c r="A29" s="8" t="s">
-        <v>288</v>
+        <v>248</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>244</v>
-      </c>
-      <c r="C29" s="8" t="s">
-        <v>81</v>
+        <v>207</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>77</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="60">
       <c r="A30" s="8" t="s">
-        <v>289</v>
+        <v>249</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>245</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>82</v>
+        <v>208</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>78</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="8" t="s">
-        <v>290</v>
+        <v>250</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>246</v>
-      </c>
-      <c r="C31" s="8" t="s">
-        <v>83</v>
+        <v>209</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>79</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="90">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
       <c r="A32" s="8" t="s">
-        <v>291</v>
+        <v>251</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>247</v>
+        <v>210</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="60">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
       <c r="A33" s="8" t="s">
-        <v>292</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>248</v>
-      </c>
-      <c r="C33" s="7" t="s">
-        <v>85</v>
+        <v>252</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>81</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="90">
       <c r="A34" s="8" t="s">
-        <v>293</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>249</v>
+        <v>253</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>212</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="8" t="s">
-        <v>294</v>
-      </c>
-      <c r="B35" s="7" t="s">
-        <v>250</v>
-      </c>
-      <c r="C35" s="7" t="s">
-        <v>87</v>
+        <v>254</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="8" t="s">
-        <v>295</v>
+        <v>255</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>251</v>
+        <v>214</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E36" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="90">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
       <c r="A37" s="8" t="s">
-        <v>296</v>
+        <v>256</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>252</v>
-      </c>
-      <c r="C37" s="7" t="s">
-        <v>89</v>
+        <v>215</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>85</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="90">
       <c r="A38" s="8" t="s">
-        <v>297</v>
+        <v>257</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>253</v>
-      </c>
-      <c r="C38" s="8" t="s">
-        <v>90</v>
+        <v>216</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>86</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="8" t="s">
-        <v>298</v>
+        <v>258</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>254</v>
-      </c>
-      <c r="C39" s="8" t="s">
-        <v>91</v>
+        <v>217</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>87</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="8" t="s">
-        <v>299</v>
+        <v>259</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>255</v>
-      </c>
-      <c r="C40" s="8" t="s">
-        <v>92</v>
+        <v>218</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>89</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E40" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="90">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
       <c r="A41" s="8" t="s">
-        <v>300</v>
+        <v>260</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>256</v>
+        <v>219</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E41" s="8" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="8" t="s">
-        <v>301</v>
+        <v>261</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>257</v>
+        <v>220</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E42" s="8" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="8" t="s">
-        <v>302</v>
-      </c>
-      <c r="B43" s="8" t="s">
-        <v>258</v>
+        <v>262</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>92</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>96</v>
+        <v>335</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E43" s="8" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="8" t="s">
-        <v>303</v>
-      </c>
-      <c r="B44" s="8" t="s">
-        <v>259</v>
+        <v>263</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>93</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>97</v>
+        <v>332</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E44" s="8" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="8" t="s">
-        <v>304</v>
-      </c>
-      <c r="B45" s="8" t="s">
-        <v>260</v>
+        <v>264</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>336</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>98</v>
+        <v>331</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E45" s="8" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="8" t="s">
-        <v>305</v>
+        <v>265</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>99</v>
+        <v>333</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E46" s="8" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="8" t="s">
-        <v>306</v>
+        <v>266</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>55</v>
+        <v>94</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>100</v>
+        <v>334</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E47" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="120">
+      <c r="A48" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="B48" s="7" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="48" spans="1:5">
-      <c r="A48" s="8" t="s">
-        <v>307</v>
-      </c>
-      <c r="B48" s="7" t="s">
-        <v>102</v>
-      </c>
       <c r="C48" s="7" t="s">
-        <v>101</v>
+        <v>327</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E48" s="8" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="8" t="s">
-        <v>308</v>
+        <v>268</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>103</v>
+        <v>50</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>104</v>
+        <v>49</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E49" s="8" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="8" t="s">
-        <v>309</v>
+        <v>269</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>48</v>
+        <v>97</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E50" s="8" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="8" t="s">
-        <v>310</v>
+        <v>270</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>52</v>
+        <v>98</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E51" s="8" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="8" t="s">
-        <v>311</v>
+        <v>271</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E52" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" ht="120">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
       <c r="A53" s="8" t="s">
-        <v>312</v>
+        <v>272</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>109</v>
+        <v>337</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>382</v>
+        <v>102</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E53" s="8" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="30">
       <c r="A54" s="8" t="s">
-        <v>313</v>
+        <v>273</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>111</v>
+        <v>338</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E54" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" ht="30">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
       <c r="A55" s="8" t="s">
-        <v>314</v>
+        <v>274</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>49</v>
+        <v>104</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>112</v>
+        <v>345</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E55" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" ht="30">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
       <c r="A56" s="8" t="s">
-        <v>315</v>
+        <v>275</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>51</v>
+        <v>105</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>113</v>
+        <v>342</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E56" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" ht="30">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
       <c r="A57" s="8" t="s">
-        <v>316</v>
+        <v>276</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>114</v>
+        <v>343</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E57" s="8" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="8" t="s">
-        <v>317</v>
+        <v>277</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>54</v>
+        <v>107</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>53</v>
+        <v>344</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E58" s="8" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="8" t="s">
-        <v>318</v>
+        <v>278</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E59" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="90">
       <c r="A60" s="8" t="s">
-        <v>319</v>
+        <v>279</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>117</v>
+        <v>339</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E60" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="75">
       <c r="A61" s="8" t="s">
-        <v>320</v>
+        <v>280</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>121</v>
+        <v>340</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E61" s="8" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="62" spans="1:5">
       <c r="A62" s="8" t="s">
-        <v>321</v>
+        <v>281</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E62" s="8" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="8" t="s">
-        <v>322</v>
+        <v>282</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>43</v>
+        <v>114</v>
       </c>
       <c r="C63" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="D63" s="8" t="s">
+        <v>326</v>
+      </c>
+      <c r="E63" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="B64" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="C64" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="D64" s="8" t="s">
+        <v>326</v>
+      </c>
+      <c r="E64" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="120">
+      <c r="A65" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="B65" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="C65" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="D65" s="8" t="s">
+        <v>326</v>
+      </c>
+      <c r="E65" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="120">
+      <c r="A66" s="8" t="s">
+        <v>285</v>
+      </c>
+      <c r="B66" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="C66" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D66" s="8" t="s">
+        <v>326</v>
+      </c>
+      <c r="E66" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="195">
+      <c r="A67" s="8" t="s">
+        <v>286</v>
+      </c>
+      <c r="B67" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="C67" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="D67" s="8" t="s">
+        <v>326</v>
+      </c>
+      <c r="E67" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68" s="8" t="s">
+        <v>287</v>
+      </c>
+      <c r="B68" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="C68" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="D68" s="8" t="s">
+        <v>326</v>
+      </c>
+      <c r="E68" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69" s="8" t="s">
+        <v>288</v>
+      </c>
+      <c r="B69" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C69" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="D63" s="8" t="s">
-        <v>381</v>
-      </c>
-      <c r="E63" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" ht="45">
-      <c r="A64" s="8" t="s">
-        <v>323</v>
-      </c>
-      <c r="B64" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="C64" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="D64" s="8" t="s">
-        <v>381</v>
-      </c>
-      <c r="E64" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" ht="30">
-      <c r="A65" s="8" t="s">
-        <v>324</v>
-      </c>
-      <c r="B65" s="7" t="s">
+      <c r="D69" s="8" t="s">
+        <v>326</v>
+      </c>
+      <c r="E69" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70" s="8" t="s">
+        <v>289</v>
+      </c>
+      <c r="B70" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="C70" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="C65" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="D65" s="8" t="s">
-        <v>381</v>
-      </c>
-      <c r="E65" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" ht="30">
-      <c r="A66" s="8" t="s">
-        <v>325</v>
-      </c>
-      <c r="B66" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="C66" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="D66" s="8" t="s">
-        <v>381</v>
-      </c>
-      <c r="E66" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" ht="30">
-      <c r="A67" s="8" t="s">
-        <v>326</v>
-      </c>
-      <c r="B67" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="C67" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="D67" s="8" t="s">
-        <v>381</v>
-      </c>
-      <c r="E67" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" ht="30">
-      <c r="A68" s="8" t="s">
-        <v>327</v>
-      </c>
-      <c r="B68" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="C68" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="D68" s="8" t="s">
-        <v>381</v>
-      </c>
-      <c r="E68" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" ht="30">
-      <c r="A69" s="8" t="s">
-        <v>328</v>
-      </c>
-      <c r="B69" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="C69" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="D69" s="8" t="s">
-        <v>381</v>
-      </c>
-      <c r="E69" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" ht="30">
-      <c r="A70" s="8" t="s">
-        <v>329</v>
-      </c>
-      <c r="B70" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="C70" s="7" t="s">
-        <v>138</v>
-      </c>
       <c r="D70" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E70" s="8" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="30">
       <c r="A71" s="8" t="s">
-        <v>330</v>
+        <v>290</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="D71" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E71" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" ht="30">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
       <c r="A72" s="8" t="s">
-        <v>331</v>
+        <v>291</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="D72" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E72" s="8" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="73" spans="1:5">
       <c r="A73" s="8" t="s">
-        <v>332</v>
+        <v>292</v>
       </c>
       <c r="B73" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C73" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="D73" s="8" t="s">
+        <v>326</v>
+      </c>
+      <c r="E73" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74" s="8" t="s">
+        <v>293</v>
+      </c>
+      <c r="B74" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="C74" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="D74" s="8" t="s">
+        <v>326</v>
+      </c>
+      <c r="E74" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="B75" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="C75" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="D75" s="8" t="s">
+        <v>326</v>
+      </c>
+      <c r="E75" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="105">
+      <c r="A76" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="B76" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="C76" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="D76" s="8" t="s">
+        <v>326</v>
+      </c>
+      <c r="E76" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="105">
+      <c r="A77" s="8" t="s">
+        <v>296</v>
+      </c>
+      <c r="B77" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="C77" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="C73" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="D73" s="8" t="s">
-        <v>381</v>
-      </c>
-      <c r="E73" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" ht="90">
-      <c r="A74" s="8" t="s">
-        <v>333</v>
-      </c>
-      <c r="B74" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="C74" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="D74" s="8" t="s">
-        <v>381</v>
-      </c>
-      <c r="E74" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" ht="60">
-      <c r="A75" s="8" t="s">
-        <v>334</v>
-      </c>
-      <c r="B75" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="C75" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="D75" s="8" t="s">
-        <v>381</v>
-      </c>
-      <c r="E75" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5">
-      <c r="A76" s="8" t="s">
-        <v>335</v>
-      </c>
-      <c r="B76" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="C76" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="D76" s="8" t="s">
-        <v>381</v>
-      </c>
-      <c r="E76" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5">
-      <c r="A77" s="8" t="s">
-        <v>336</v>
-      </c>
-      <c r="B77" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="C77" s="7" t="s">
-        <v>152</v>
-      </c>
       <c r="D77" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E77" s="8" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="78" spans="1:5">
       <c r="A78" s="8" t="s">
-        <v>337</v>
+        <v>297</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="C78" s="7" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="D78" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E78" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" ht="120">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
       <c r="A79" s="8" t="s">
-        <v>338</v>
+        <v>298</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="C79" s="7" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="D79" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E79" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" ht="120">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="45">
       <c r="A80" s="8" t="s">
-        <v>339</v>
+        <v>299</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="C80" s="7" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="D80" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E80" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" ht="195">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
       <c r="A81" s="8" t="s">
-        <v>340</v>
-      </c>
-      <c r="B81" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="C81" s="7" t="s">
-        <v>159</v>
+        <v>300</v>
+      </c>
+      <c r="B81" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="C81" s="8" t="s">
+        <v>151</v>
       </c>
       <c r="D81" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E81" s="8" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="82" spans="1:5">
       <c r="A82" s="8" t="s">
-        <v>341</v>
-      </c>
-      <c r="B82" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="C82" s="7" t="s">
-        <v>161</v>
+        <v>301</v>
+      </c>
+      <c r="B82" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="C82" s="8" t="s">
+        <v>153</v>
       </c>
       <c r="D82" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E82" s="8" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="83" spans="1:5">
       <c r="A83" s="8" t="s">
-        <v>342</v>
-      </c>
-      <c r="B83" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="C83" s="7" t="s">
-        <v>162</v>
+        <v>302</v>
+      </c>
+      <c r="B83" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="C83" s="8" t="s">
+        <v>155</v>
       </c>
       <c r="D83" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E83" s="8" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="84" spans="1:5">
       <c r="A84" s="8" t="s">
-        <v>343</v>
-      </c>
-      <c r="B84" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="C84" s="7" t="s">
-        <v>166</v>
+        <v>303</v>
+      </c>
+      <c r="B84" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="C84" s="8" t="s">
+        <v>157</v>
       </c>
       <c r="D84" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E84" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" ht="30">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
       <c r="A85" s="8" t="s">
-        <v>344</v>
-      </c>
-      <c r="B85" s="7" t="s">
-        <v>168</v>
-      </c>
-      <c r="C85" s="7" t="s">
-        <v>167</v>
+        <v>304</v>
+      </c>
+      <c r="B85" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="C85" s="8" t="s">
+        <v>159</v>
       </c>
       <c r="D85" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E85" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="165">
       <c r="A86" s="8" t="s">
-        <v>345</v>
-      </c>
-      <c r="B86" s="7" t="s">
-        <v>169</v>
+        <v>305</v>
+      </c>
+      <c r="B86" s="8" t="s">
+        <v>161</v>
       </c>
       <c r="C86" s="7" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="D86" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E86" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="75">
       <c r="A87" s="8" t="s">
-        <v>346</v>
-      </c>
-      <c r="B87" s="7" t="s">
-        <v>173</v>
-      </c>
-      <c r="C87" s="8" t="s">
-        <v>172</v>
+        <v>306</v>
+      </c>
+      <c r="B87" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="C87" s="7" t="s">
+        <v>178</v>
       </c>
       <c r="D87" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E87" s="8" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="88" spans="1:5">
       <c r="A88" s="8" t="s">
-        <v>347</v>
+        <v>307</v>
       </c>
       <c r="B88" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="C88" s="8" t="s">
-        <v>175</v>
+        <v>162</v>
+      </c>
+      <c r="C88" s="7" t="s">
+        <v>163</v>
       </c>
       <c r="D88" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E88" s="8" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="89" spans="1:5">
       <c r="A89" s="8" t="s">
-        <v>348</v>
+        <v>308</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="C89" s="8" t="s">
-        <v>176</v>
+        <v>164</v>
+      </c>
+      <c r="C89" s="7" t="s">
+        <v>165</v>
       </c>
       <c r="D89" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E89" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" ht="105">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
       <c r="A90" s="8" t="s">
-        <v>349</v>
-      </c>
-      <c r="B90" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="C90" s="7" t="s">
-        <v>180</v>
+        <v>309</v>
+      </c>
+      <c r="B90" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="C90" s="8" t="s">
+        <v>169</v>
       </c>
       <c r="D90" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E90" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" ht="105">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
       <c r="A91" s="8" t="s">
-        <v>350</v>
-      </c>
-      <c r="B91" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="C91" s="7" t="s">
-        <v>181</v>
+        <v>310</v>
+      </c>
+      <c r="B91" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="C91" s="8" t="s">
+        <v>167</v>
       </c>
       <c r="D91" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E91" s="8" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="92" spans="1:5">
       <c r="A92" s="8" t="s">
-        <v>351</v>
-      </c>
-      <c r="B92" s="7" t="s">
-        <v>182</v>
-      </c>
-      <c r="C92" s="7" t="s">
-        <v>183</v>
+        <v>311</v>
+      </c>
+      <c r="B92" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="C92" s="8" t="s">
+        <v>171</v>
       </c>
       <c r="D92" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E92" s="8" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="93" spans="1:5">
       <c r="A93" s="8" t="s">
-        <v>352</v>
-      </c>
-      <c r="B93" s="7" t="s">
-        <v>184</v>
-      </c>
-      <c r="C93" s="7" t="s">
-        <v>185</v>
+        <v>312</v>
+      </c>
+      <c r="B93" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="C93" s="8" t="s">
+        <v>172</v>
       </c>
       <c r="D93" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E93" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" ht="45">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5">
       <c r="A94" s="8" t="s">
-        <v>353</v>
-      </c>
-      <c r="B94" s="7" t="s">
-        <v>187</v>
-      </c>
-      <c r="C94" s="7" t="s">
-        <v>186</v>
+        <v>313</v>
+      </c>
+      <c r="B94" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="C94" s="8" t="s">
+        <v>175</v>
       </c>
       <c r="D94" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E94" s="8" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="95" spans="1:5">
       <c r="A95" s="8" t="s">
-        <v>354</v>
+        <v>314</v>
       </c>
       <c r="B95" s="8" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="C95" s="8" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="D95" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E95" s="8" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="96" spans="1:5">
       <c r="A96" s="8" t="s">
-        <v>355</v>
-      </c>
-      <c r="B96" s="8" t="s">
+        <v>315</v>
+      </c>
+      <c r="B96" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="C96" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="D96" s="8" t="s">
+        <v>326</v>
+      </c>
+      <c r="E96" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" ht="30">
+      <c r="A97" s="8" t="s">
+        <v>316</v>
+      </c>
+      <c r="B97" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="C97" s="10" t="s">
+        <v>328</v>
+      </c>
+      <c r="D97" s="8" t="s">
+        <v>326</v>
+      </c>
+      <c r="E97" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" ht="75">
+      <c r="A98" s="8" t="s">
+        <v>317</v>
+      </c>
+      <c r="B98" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="C98" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="D98" s="8" t="s">
+        <v>326</v>
+      </c>
+      <c r="E98" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" ht="60">
+      <c r="A99" s="8" t="s">
+        <v>318</v>
+      </c>
+      <c r="B99" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="C99" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="D99" s="8" t="s">
+        <v>326</v>
+      </c>
+      <c r="E99" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" ht="105">
+      <c r="A100" s="8" t="s">
+        <v>319</v>
+      </c>
+      <c r="B100" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="C100" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="D100" s="8" t="s">
+        <v>326</v>
+      </c>
+      <c r="E100" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" ht="105">
+      <c r="A101" s="8" t="s">
+        <v>320</v>
+      </c>
+      <c r="B101" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="C101" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="C96" s="8" t="s">
-        <v>191</v>
-      </c>
-      <c r="D96" s="8" t="s">
-        <v>381</v>
-      </c>
-      <c r="E96" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5">
-      <c r="A97" s="8" t="s">
-        <v>356</v>
-      </c>
-      <c r="B97" s="8" t="s">
-        <v>192</v>
-      </c>
-      <c r="C97" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="D97" s="8" t="s">
-        <v>381</v>
-      </c>
-      <c r="E97" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5">
-      <c r="A98" s="8" t="s">
-        <v>357</v>
-      </c>
-      <c r="B98" s="8" t="s">
-        <v>194</v>
-      </c>
-      <c r="C98" s="8" t="s">
-        <v>195</v>
-      </c>
-      <c r="D98" s="8" t="s">
-        <v>381</v>
-      </c>
-      <c r="E98" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5">
-      <c r="A99" s="8" t="s">
-        <v>358</v>
-      </c>
-      <c r="B99" s="8" t="s">
-        <v>196</v>
-      </c>
-      <c r="C99" s="8" t="s">
-        <v>197</v>
-      </c>
-      <c r="D99" s="8" t="s">
-        <v>381</v>
-      </c>
-      <c r="E99" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" ht="165">
-      <c r="A100" s="8" t="s">
-        <v>359</v>
-      </c>
-      <c r="B100" s="8" t="s">
-        <v>199</v>
-      </c>
-      <c r="C100" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="D100" s="8" t="s">
-        <v>381</v>
-      </c>
-      <c r="E100" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" ht="75">
-      <c r="A101" s="8" t="s">
-        <v>360</v>
-      </c>
-      <c r="B101" s="9" t="s">
-        <v>219</v>
-      </c>
-      <c r="C101" s="7" t="s">
-        <v>218</v>
-      </c>
       <c r="D101" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E101" s="8" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="102" spans="1:5">
       <c r="A102" s="8" t="s">
-        <v>361</v>
+        <v>321</v>
       </c>
       <c r="B102" s="7" t="s">
-        <v>200</v>
-      </c>
-      <c r="C102" s="7" t="s">
-        <v>201</v>
+        <v>191</v>
+      </c>
+      <c r="C102" s="8" t="s">
+        <v>192</v>
       </c>
       <c r="D102" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E102" s="8" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="103" spans="1:5">
       <c r="A103" s="8" t="s">
-        <v>362</v>
+        <v>322</v>
       </c>
       <c r="B103" s="7" t="s">
-        <v>202</v>
-      </c>
-      <c r="C103" s="7" t="s">
-        <v>203</v>
+        <v>193</v>
+      </c>
+      <c r="C103" s="3" t="s">
+        <v>194</v>
       </c>
       <c r="D103" s="8" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E103" s="8" t="s">
-        <v>95</v>
+        <v>133</v>
       </c>
     </row>
     <row r="104" spans="1:5">
       <c r="A104" s="8" t="s">
-        <v>363</v>
-      </c>
-      <c r="B104" s="8" t="s">
-        <v>206</v>
-      </c>
-      <c r="C104" s="8" t="s">
-        <v>207</v>
+        <v>323</v>
+      </c>
+      <c r="B104" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="C104" s="3" t="s">
+        <v>196</v>
       </c>
       <c r="D104" s="8" t="s">
-        <v>381</v>
-      </c>
-      <c r="E104" s="8" t="s">
-        <v>95</v>
-      </c>
+        <v>326</v>
+      </c>
+      <c r="E104" s="3"/>
     </row>
     <row r="105" spans="1:5">
       <c r="A105" s="8" t="s">
-        <v>364</v>
-      </c>
-      <c r="B105" s="8" t="s">
-        <v>204</v>
-      </c>
-      <c r="C105" s="8" t="s">
-        <v>205</v>
+        <v>324</v>
+      </c>
+      <c r="B105" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="C105" s="3" t="s">
+        <v>198</v>
       </c>
       <c r="D105" s="8" t="s">
-        <v>381</v>
-      </c>
-      <c r="E105" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5">
+        <v>326</v>
+      </c>
+      <c r="E105" s="3"/>
+    </row>
+    <row r="106" spans="1:5" ht="150">
       <c r="A106" s="8" t="s">
-        <v>365</v>
-      </c>
-      <c r="B106" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="C106" s="8" t="s">
-        <v>209</v>
+        <v>325</v>
+      </c>
+      <c r="B106" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="C106" s="4" t="s">
+        <v>200</v>
       </c>
       <c r="D106" s="8" t="s">
-        <v>381</v>
-      </c>
-      <c r="E106" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5">
-      <c r="A107" s="8" t="s">
-        <v>366</v>
-      </c>
-      <c r="B107" s="8" t="s">
-        <v>211</v>
-      </c>
-      <c r="C107" s="8" t="s">
-        <v>210</v>
-      </c>
-      <c r="D107" s="8" t="s">
-        <v>381</v>
-      </c>
-      <c r="E107" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5">
-      <c r="A108" s="8" t="s">
-        <v>367</v>
-      </c>
-      <c r="B108" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="C108" s="8" t="s">
-        <v>213</v>
-      </c>
-      <c r="D108" s="8" t="s">
-        <v>381</v>
-      </c>
-      <c r="E108" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5">
-      <c r="A109" s="8" t="s">
-        <v>368</v>
-      </c>
-      <c r="B109" s="8" t="s">
-        <v>214</v>
-      </c>
-      <c r="C109" s="8" t="s">
-        <v>215</v>
-      </c>
-      <c r="D109" s="8" t="s">
-        <v>381</v>
-      </c>
-      <c r="E109" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5">
-      <c r="A110" s="8" t="s">
-        <v>369</v>
-      </c>
-      <c r="B110" s="8" t="s">
-        <v>217</v>
-      </c>
-      <c r="C110" s="8" t="s">
-        <v>216</v>
-      </c>
-      <c r="D110" s="8" t="s">
-        <v>381</v>
-      </c>
-      <c r="E110" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5">
-      <c r="A111" s="8" t="s">
-        <v>370</v>
-      </c>
-      <c r="B111" s="9" t="s">
-        <v>221</v>
-      </c>
-      <c r="C111" s="9" t="s">
-        <v>220</v>
-      </c>
-      <c r="D111" s="8" t="s">
-        <v>381</v>
-      </c>
-      <c r="E111" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" ht="30">
-      <c r="A112" s="8" t="s">
-        <v>371</v>
-      </c>
-      <c r="B112" s="9" t="s">
-        <v>222</v>
-      </c>
-      <c r="C112" s="10" t="s">
-        <v>383</v>
-      </c>
-      <c r="D112" s="8" t="s">
-        <v>381</v>
-      </c>
-      <c r="E112" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" ht="75">
-      <c r="A113" s="8" t="s">
-        <v>372</v>
-      </c>
-      <c r="B113" s="8" t="s">
-        <v>223</v>
-      </c>
-      <c r="C113" s="7" t="s">
-        <v>224</v>
-      </c>
-      <c r="D113" s="8" t="s">
-        <v>381</v>
-      </c>
-      <c r="E113" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" ht="60">
-      <c r="A114" s="8" t="s">
-        <v>373</v>
-      </c>
-      <c r="B114" s="7" t="s">
-        <v>225</v>
-      </c>
-      <c r="C114" s="7" t="s">
-        <v>226</v>
-      </c>
-      <c r="D114" s="8" t="s">
-        <v>381</v>
-      </c>
-      <c r="E114" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5" ht="105">
-      <c r="A115" s="8" t="s">
-        <v>374</v>
-      </c>
-      <c r="B115" s="7" t="s">
-        <v>227</v>
-      </c>
-      <c r="C115" s="7" t="s">
-        <v>228</v>
-      </c>
-      <c r="D115" s="8" t="s">
-        <v>381</v>
-      </c>
-      <c r="E115" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5" ht="105">
-      <c r="A116" s="8" t="s">
-        <v>375</v>
-      </c>
-      <c r="B116" s="7" t="s">
-        <v>229</v>
-      </c>
-      <c r="C116" s="7" t="s">
-        <v>230</v>
-      </c>
-      <c r="D116" s="8" t="s">
-        <v>381</v>
-      </c>
-      <c r="E116" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5">
-      <c r="A117" s="8" t="s">
-        <v>376</v>
-      </c>
-      <c r="B117" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C117" s="8" t="s">
-        <v>232</v>
-      </c>
-      <c r="D117" s="8" t="s">
-        <v>381</v>
-      </c>
-      <c r="E117" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5">
-      <c r="A118" s="8" t="s">
-        <v>377</v>
-      </c>
-      <c r="B118" s="7" t="s">
-        <v>233</v>
-      </c>
-      <c r="C118" s="3" t="s">
-        <v>234</v>
-      </c>
-      <c r="D118" s="8" t="s">
-        <v>381</v>
-      </c>
-      <c r="E118" s="8" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5">
-      <c r="A119" s="8" t="s">
-        <v>378</v>
-      </c>
-      <c r="B119" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="C119" s="3" t="s">
-        <v>236</v>
-      </c>
-      <c r="D119" s="8" t="s">
-        <v>381</v>
-      </c>
-      <c r="E119" s="3"/>
-    </row>
-    <row r="120" spans="1:5">
-      <c r="A120" s="8" t="s">
-        <v>379</v>
-      </c>
-      <c r="B120" s="3" t="s">
-        <v>237</v>
-      </c>
-      <c r="C120" s="3" t="s">
-        <v>238</v>
-      </c>
-      <c r="D120" s="8" t="s">
-        <v>381</v>
-      </c>
-      <c r="E120" s="3"/>
-    </row>
-    <row r="121" spans="1:5" ht="150">
-      <c r="A121" s="8" t="s">
-        <v>380</v>
-      </c>
-      <c r="B121" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="C121" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="D121" s="8" t="s">
-        <v>381</v>
-      </c>
-      <c r="E121" s="3"/>
+        <v>326</v>
+      </c>
+      <c r="E106" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Deeplinking test cases has been added in search module
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Search.xlsx
+++ b/src/test/resources/xls/Search.xlsx
@@ -8,14 +8,15 @@
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
-    <sheet name="Test Case Steps" sheetId="2" r:id="rId2"/>
+    <sheet name="deek_linking" sheetId="3" r:id="rId2"/>
+    <sheet name="Test Case Steps" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="374">
   <si>
     <t>TCID</t>
   </si>
@@ -1218,12 +1219,96 @@
   <si>
     <t>Verify that record view of an article gets displayed when user clicks on any article option in the search type ahead</t>
   </si>
+  <si>
+    <t>url</t>
+  </si>
+  <si>
+    <t>Search127</t>
+  </si>
+  <si>
+    <t>#/search?query=science&amp;offsetIndex=0&amp;searchType=ALL</t>
+  </si>
+  <si>
+    <t>#/search?query=science&amp;offsetIndex=0&amp;sortType=_score:desc&amp;searchType=ARTICLES</t>
+  </si>
+  <si>
+    <t>#/search?query=science&amp;offsetIndex=0&amp;sortType=_score:desc&amp;searchType=PATENTS</t>
+  </si>
+  <si>
+    <t>#/search?query=science&amp;offsetIndex=0&amp;sortType=_score:desc&amp;searchType=PEOPLE</t>
+  </si>
+  <si>
+    <t>#/search?query=science&amp;offsetIndex=0&amp;sortType=sortdate:desc&amp;searchType=POSTS</t>
+  </si>
+  <si>
+    <t>#/search?query=post&amp;offsetIndex=0&amp;sortType=sortdate:desc&amp;searchType=POSTS</t>
+  </si>
+  <si>
+    <t>#/search?query=biology&amp;offsetIndex=0&amp;sortType=citingsrcslocalcount:desc&amp;searchType=ALL</t>
+  </si>
+  <si>
+    <t>#/search?query=biology&amp;offsetIndex=0&amp;sortType=sortdate:desc&amp;searchType=ALL</t>
+  </si>
+  <si>
+    <t>#/search?query=biology&amp;offsetIndex=0&amp;sortType=sortdate:asc&amp;searchType=ALL</t>
+  </si>
+  <si>
+    <t>#/search?query=biology&amp;offsetIndex=0&amp;sortType=citingsrcslocalcount:desc&amp;searchType=ARTICLES</t>
+  </si>
+  <si>
+    <t>#/search?query=biology&amp;offsetIndex=0&amp;sortType=sortdate:desc&amp;searchType=ARTICLES</t>
+  </si>
+  <si>
+    <t>#/search?query=biology&amp;offsetIndex=0&amp;sortType=sortdate:asc&amp;searchType=ARTICLES</t>
+  </si>
+  <si>
+    <t>#/search?query=biology&amp;offsetIndex=0&amp;sortType=citingsrcscount:desc&amp;searchType=PATENTS</t>
+  </si>
+  <si>
+    <t>#/search?query=biology&amp;offsetIndex=0&amp;sortType=sortdate:desc&amp;searchType=PATENTS</t>
+  </si>
+  <si>
+    <t>#/search?query=biology&amp;offsetIndex=0&amp;sortType=sortdate:asc&amp;searchType=PATENTS</t>
+  </si>
+  <si>
+    <t>#/search?query=biology&amp;offsetIndex=0&amp;sortType=loadtime:desc&amp;searchType=PEOPLE</t>
+  </si>
+  <si>
+    <t>#/search?query=biology&amp;offsetIndex=0&amp;sortType=sortdate:asc&amp;searchType=POSTS</t>
+  </si>
+  <si>
+    <t>#/search?query=biology&amp;offsetIndex=0&amp;sortType=_score:desc&amp;searchType=POSTS</t>
+  </si>
+  <si>
+    <t>recordtype</t>
+  </si>
+  <si>
+    <t>All Search Page</t>
+  </si>
+  <si>
+    <t>Articles Search page</t>
+  </si>
+  <si>
+    <t>Patents Search Page</t>
+  </si>
+  <si>
+    <t>People Search Page</t>
+  </si>
+  <si>
+    <t>Posts Search post</t>
+  </si>
+  <si>
+    <t>OPQA-2801|OPQA-2802|OPQA-2803|OPQA-2804|OPQA-2805|OPQA-2808|OPQA-2809|OPQA-2810|OPQA-2811|OPQA-2812|OPQA-2813|OPQA-2814|OPQA-2815|OPQA-2816|OPQA-2817|OPQA-2818|OPQA-2819|OPQA-2820</t>
+  </si>
+  <si>
+    <t>Verify that Deeplinking is working for Search result page using steam account</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1245,6 +1330,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1291,10 +1383,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1318,8 +1414,11 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1617,10 +1716,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E106"/>
+  <dimension ref="A1:E107"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B61" sqref="B61"/>
+    <sheetView tabSelected="1" topLeftCell="B103" workbookViewId="0">
+      <selection activeCell="B110" sqref="B110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3428,6 +3527,21 @@
       </c>
       <c r="E106" s="3"/>
     </row>
+    <row r="107" spans="1:5">
+      <c r="A107" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="B107" s="12" t="s">
+        <v>372</v>
+      </c>
+      <c r="C107" s="12" t="s">
+        <v>373</v>
+      </c>
+      <c r="D107" s="8" t="s">
+        <v>326</v>
+      </c>
+      <c r="E107" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3436,10 +3550,262 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="88.85546875" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>346</v>
+      </c>
+      <c r="B1" t="s">
+        <v>366</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="11" t="s">
+        <v>348</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>367</v>
+      </c>
+      <c r="C2" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="11" t="s">
+        <v>349</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>368</v>
+      </c>
+      <c r="C3" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="11" t="s">
+        <v>350</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>369</v>
+      </c>
+      <c r="C4" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="11" t="s">
+        <v>351</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>370</v>
+      </c>
+      <c r="C5" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="11" t="s">
+        <v>352</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>371</v>
+      </c>
+      <c r="C6" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="11" t="s">
+        <v>354</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>367</v>
+      </c>
+      <c r="C7" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="11" t="s">
+        <v>355</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>367</v>
+      </c>
+      <c r="C8" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="11" t="s">
+        <v>356</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>367</v>
+      </c>
+      <c r="C9" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="11" t="s">
+        <v>357</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>368</v>
+      </c>
+      <c r="C10" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="11" t="s">
+        <v>358</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>368</v>
+      </c>
+      <c r="C11" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="11" t="s">
+        <v>359</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>368</v>
+      </c>
+      <c r="C12" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="11" t="s">
+        <v>360</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>369</v>
+      </c>
+      <c r="C13" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="11" t="s">
+        <v>361</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>369</v>
+      </c>
+      <c r="C14" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="11" t="s">
+        <v>362</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>369</v>
+      </c>
+      <c r="C15" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="11" t="s">
+        <v>363</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>370</v>
+      </c>
+      <c r="C16" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="11" t="s">
+        <v>353</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>371</v>
+      </c>
+      <c r="C17" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="11" t="s">
+        <v>364</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>371</v>
+      </c>
+      <c r="C18" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="11" t="s">
+        <v>365</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>371</v>
+      </c>
+      <c r="C19" t="s">
+        <v>326</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" location="/search?query=science&amp;offsetIndex=0&amp;searchType=ALL" display="https://dev-stable.1p.thomsonreuters.com/ - /search?query=science&amp;offsetIndex=0&amp;searchType=ALL"/>
+    <hyperlink ref="A3" r:id="rId2" location="/search?query=science&amp;offsetIndex=0&amp;sortType=_score:desc&amp;searchType=ARTICLES" display="https://dev-stable.1p.thomsonreuters.com/ - /search?query=science&amp;offsetIndex=0&amp;sortType=_score:desc&amp;searchType=ARTICLES"/>
+    <hyperlink ref="A4" r:id="rId3" location="/search?query=science&amp;offsetIndex=0&amp;sortType=_score:desc&amp;searchType=PATENTS" display="https://dev-stable.1p.thomsonreuters.com/ - /search?query=science&amp;offsetIndex=0&amp;sortType=_score:desc&amp;searchType=PATENTS"/>
+    <hyperlink ref="A5" r:id="rId4" location="/search?query=science&amp;offsetIndex=0&amp;sortType=_score:desc&amp;searchType=PEOPLE" display="https://dev-stable.1p.thomsonreuters.com/ - /search?query=science&amp;offsetIndex=0&amp;sortType=_score:desc&amp;searchType=PEOPLE"/>
+    <hyperlink ref="A6" r:id="rId5" location="/search?query=science&amp;offsetIndex=0&amp;sortType=sortdate:desc&amp;searchType=POSTS" display="https://dev-stable.1p.thomsonreuters.com/ - /search?query=science&amp;offsetIndex=0&amp;sortType=sortdate:desc&amp;searchType=POSTS"/>
+    <hyperlink ref="A7" r:id="rId6" location="/search?query=biology&amp;offsetIndex=0&amp;sortType=citingsrcslocalcount:desc&amp;searchType=ALL" display="http://dev-stable.1p.thomsonreuters.com/ - /search?query=biology&amp;offsetIndex=0&amp;sortType=citingsrcslocalcount:desc&amp;searchType=ALL"/>
+    <hyperlink ref="A8" r:id="rId7" location="/search?query=biology&amp;offsetIndex=0&amp;sortType=sortdate:desc&amp;searchType=ALL" display="http://dev-stable.1p.thomsonreuters.com/ - /search?query=biology&amp;offsetIndex=0&amp;sortType=sortdate:desc&amp;searchType=ALL"/>
+    <hyperlink ref="A9" r:id="rId8" location="/search?query=biology&amp;offsetIndex=0&amp;sortType=sortdate:asc&amp;searchType=ALL" display="http://dev-stable.1p.thomsonreuters.com/ - /search?query=biology&amp;offsetIndex=0&amp;sortType=sortdate:asc&amp;searchType=ALL"/>
+    <hyperlink ref="A10" r:id="rId9" location="/search?query=biology&amp;offsetIndex=0&amp;sortType=citingsrcslocalcount:desc&amp;searchType=ARTICLES" display="http://dev-stable.1p.thomsonreuters.com/ - /search?query=biology&amp;offsetIndex=0&amp;sortType=citingsrcslocalcount:desc&amp;searchType=ARTICLES"/>
+    <hyperlink ref="A11" r:id="rId10" location="/search?query=biology&amp;offsetIndex=0&amp;sortType=sortdate:desc&amp;searchType=ARTICLES" display="http://dev-stable.1p.thomsonreuters.com/ - /search?query=biology&amp;offsetIndex=0&amp;sortType=sortdate:desc&amp;searchType=ARTICLES"/>
+    <hyperlink ref="A12" r:id="rId11" location="/search?query=biology&amp;offsetIndex=0&amp;sortType=sortdate:asc&amp;searchType=ARTICLES" display="http://dev-stable.1p.thomsonreuters.com/ - /search?query=biology&amp;offsetIndex=0&amp;sortType=sortdate:asc&amp;searchType=ARTICLES"/>
+    <hyperlink ref="A13" r:id="rId12" location="/search?query=biology&amp;offsetIndex=0&amp;sortType=citingsrcscount:desc&amp;searchType=PATENTS" display="http://dev-stable.1p.thomsonreuters.com/ - /search?query=biology&amp;offsetIndex=0&amp;sortType=citingsrcscount:desc&amp;searchType=PATENTS"/>
+    <hyperlink ref="A14" r:id="rId13" location="/search?query=biology&amp;offsetIndex=0&amp;sortType=sortdate:desc&amp;searchType=PATENTS" display="http://dev-stable.1p.thomsonreuters.com/ - /search?query=biology&amp;offsetIndex=0&amp;sortType=sortdate:desc&amp;searchType=PATENTS"/>
+    <hyperlink ref="A15" r:id="rId14" location="/search?query=biology&amp;offsetIndex=0&amp;sortType=sortdate:asc&amp;searchType=PATENTS" display="http://dev-stable.1p.thomsonreuters.com/ - /search?query=biology&amp;offsetIndex=0&amp;sortType=sortdate:asc&amp;searchType=PATENTS"/>
+    <hyperlink ref="A16" r:id="rId15" location="/search?query=biology&amp;offsetIndex=0&amp;sortType=loadtime:desc&amp;searchType=PEOPLE" display="http://dev-stable.1p.thomsonreuters.com/ - /search?query=biology&amp;offsetIndex=0&amp;sortType=loadtime:desc&amp;searchType=PEOPLE"/>
+    <hyperlink ref="A17" r:id="rId16" location="/search?query=post&amp;offsetIndex=0&amp;sortType=sortdate:desc&amp;searchType=POSTS" display="https://dev-stable.1p.thomsonreuters.com/ - /search?query=post&amp;offsetIndex=0&amp;sortType=sortdate:desc&amp;searchType=POSTS"/>
+    <hyperlink ref="A18" r:id="rId17" location="/search?query=biology&amp;offsetIndex=0&amp;sortType=sortdate:asc&amp;searchType=POSTS" display="http://dev-stable.1p.thomsonreuters.com/#/search?query=biology&amp;offsetIndex=0&amp;sortType=sortdate:asc&amp;searchType=POSTS"/>
+    <hyperlink ref="A19" r:id="rId18" location="/search?query=biology&amp;offsetIndex=0&amp;sortType=_score:desc&amp;searchType=POSTS" display="http://dev-stable.1p.thomsonreuters.com/ - /search?query=biology&amp;offsetIndex=0&amp;sortType=_score:desc&amp;searchType=POSTS"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId19"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Test case is added in Search.xlsx file
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Search.xlsx
+++ b/src/test/resources/xls/Search.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="14715" windowHeight="8040" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="14715" windowHeight="8040"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -1259,9 +1259,6 @@
     <t>Search127</t>
   </si>
   <si>
-    <t>Verify that Deeplinking is working for Search result page using steam account</t>
-  </si>
-  <si>
     <t>#/search?query=science&amp;offsetIndex=0&amp;searchType=ALL</t>
   </si>
   <si>
@@ -1317,6 +1314,9 @@
   </si>
   <si>
     <t>OPQA-2801|OPQA-2802|OPQA-2803|OPQA-2804|OPQA-2805|OPQA-2808|OPQA-2809|OPQA-2810|OPQA-2811|OPQA-2812|OPQA-2813|OPQA-2814|OPQA-2815|OPQA-2816|OPQA-2817|OPQA-2818|OPQA-2819|OPQA-2820</t>
+  </si>
+  <si>
+    <t>Verify that Deep linking is working for Search result page using steam account</t>
   </si>
 </sst>
 </file>
@@ -1720,8 +1720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E107"/>
   <sheetViews>
-    <sheetView topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="C112" sqref="C112"/>
+    <sheetView tabSelected="1" topLeftCell="C103" workbookViewId="0">
+      <selection activeCell="C107" sqref="C107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3534,10 +3534,10 @@
         <v>358</v>
       </c>
       <c r="B107" s="3" t="s">
+        <v>377</v>
+      </c>
+      <c r="C107" s="11" t="s">
         <v>378</v>
-      </c>
-      <c r="C107" s="11" t="s">
-        <v>359</v>
       </c>
       <c r="D107" s="8" t="s">
         <v>326</v>
@@ -3554,9 +3554,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -3581,7 +3579,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B2" t="s">
         <v>349</v>
@@ -3592,7 +3590,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B3" t="s">
         <v>350</v>
@@ -3603,7 +3601,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B4" t="s">
         <v>351</v>
@@ -3614,7 +3612,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B5" t="s">
         <v>352</v>
@@ -3625,7 +3623,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B6" t="s">
         <v>353</v>
@@ -3636,7 +3634,7 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B7" t="s">
         <v>349</v>
@@ -3647,7 +3645,7 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B8" t="s">
         <v>349</v>
@@ -3658,7 +3656,7 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B9" t="s">
         <v>349</v>
@@ -3669,7 +3667,7 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B10" t="s">
         <v>354</v>
@@ -3680,7 +3678,7 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B11" t="s">
         <v>350</v>
@@ -3691,7 +3689,7 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B12" t="s">
         <v>350</v>
@@ -3702,7 +3700,7 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B13" t="s">
         <v>355</v>
@@ -3713,7 +3711,7 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B14" t="s">
         <v>356</v>
@@ -3724,7 +3722,7 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B15" t="s">
         <v>356</v>
@@ -3735,7 +3733,7 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B16" t="s">
         <v>352</v>
@@ -3746,7 +3744,7 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B17" t="s">
         <v>357</v>
@@ -3757,7 +3755,7 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B18" t="s">
         <v>357</v>
@@ -3768,7 +3766,7 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B19" t="s">
         <v>357</v>

</xml_diff>

<commit_message>
Failed test script in search module
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Search.xlsx
+++ b/src/test/resources/xls/Search.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="14715" windowHeight="8040"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="14715" windowHeight="8040" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -1259,64 +1259,64 @@
     <t>Search127</t>
   </si>
   <si>
-    <t>#/search?query=science&amp;offsetIndex=0&amp;searchType=ALL</t>
-  </si>
-  <si>
-    <t>#/search?query=science&amp;offsetIndex=0&amp;sortType=_score:desc&amp;searchType=ARTICLES</t>
-  </si>
-  <si>
-    <t>#/search?query=science&amp;offsetIndex=0&amp;sortType=_score:desc&amp;searchType=PATENTS</t>
-  </si>
-  <si>
-    <t>#/search?query=science&amp;offsetIndex=0&amp;sortType=_score:desc&amp;searchType=PEOPLE</t>
-  </si>
-  <si>
-    <t>#/search?query=science&amp;offsetIndex=0&amp;sortType=sortdate:desc&amp;searchType=POSTS</t>
-  </si>
-  <si>
-    <t>#/search?query=biology&amp;offsetIndex=0&amp;sortType=citingsrcslocalcount:desc&amp;searchType=ALL</t>
-  </si>
-  <si>
-    <t>#/search?query=biology&amp;offsetIndex=0&amp;sortType=sortdate:desc&amp;searchType=ALL</t>
-  </si>
-  <si>
-    <t>#/search?query=biology&amp;offsetIndex=0&amp;sortType=sortdate:asc&amp;searchType=ALL</t>
-  </si>
-  <si>
-    <t>#/search?query=biology&amp;offsetIndex=0&amp;sortType=citingsrcslocalcount:desc&amp;searchType=ARTICLES</t>
-  </si>
-  <si>
-    <t>#/search?query=biology&amp;offsetIndex=0&amp;sortType=sortdate:desc&amp;searchType=ARTICLES</t>
-  </si>
-  <si>
-    <t>#/search?query=biology&amp;offsetIndex=0&amp;sortType=sortdate:asc&amp;searchType=ARTICLES</t>
-  </si>
-  <si>
-    <t>#/search?query=biology&amp;offsetIndex=0&amp;sortType=citingsrcscount:desc&amp;searchType=PATENTS</t>
-  </si>
-  <si>
-    <t>#/search?query=biology&amp;offsetIndex=0&amp;sortType=sortdate:desc&amp;searchType=PATENTS</t>
-  </si>
-  <si>
-    <t>#/search?query=biology&amp;offsetIndex=0&amp;sortType=sortdate:asc&amp;searchType=PATENTS</t>
-  </si>
-  <si>
-    <t>#/search?query=biology&amp;offsetIndex=0&amp;sortType=loadtime:desc&amp;searchType=PEOPLE</t>
-  </si>
-  <si>
-    <t>#/search?query=post&amp;offsetIndex=0&amp;sortType=sortdate:desc&amp;searchType=POSTS</t>
-  </si>
-  <si>
-    <t>#/search?query=biology&amp;offsetIndex=0&amp;sortType=sortdate:asc&amp;searchType=POSTS</t>
-  </si>
-  <si>
-    <t>#/search?query=biology&amp;offsetIndex=0&amp;sortType=_score:desc&amp;searchType=POSTS</t>
-  </si>
-  <si>
     <t>OPQA-2801|OPQA-2802|OPQA-2803|OPQA-2804|OPQA-2805|OPQA-2808|OPQA-2809|OPQA-2810|OPQA-2811|OPQA-2812|OPQA-2813|OPQA-2814|OPQA-2815|OPQA-2816|OPQA-2817|OPQA-2818|OPQA-2819|OPQA-2820</t>
   </si>
   <si>
     <t>Verify that Deep linking is working for Search result page using steam account</t>
+  </si>
+  <si>
+    <t>/#/search?query=science&amp;offsetIndex=0&amp;searchType=ALL</t>
+  </si>
+  <si>
+    <t>/#/search?query=science&amp;offsetIndex=0&amp;sortType=_score:desc&amp;searchType=ARTICLES</t>
+  </si>
+  <si>
+    <t>/#/search?query=science&amp;offsetIndex=0&amp;sortType=_score:desc&amp;searchType=PATENTS</t>
+  </si>
+  <si>
+    <t>/#/search?query=science&amp;offsetIndex=0&amp;sortType=_score:desc&amp;searchType=PEOPLE</t>
+  </si>
+  <si>
+    <t>/#/search?query=science&amp;offsetIndex=0&amp;sortType=sortdate:desc&amp;searchType=POSTS</t>
+  </si>
+  <si>
+    <t>/#/search?query=biology&amp;offsetIndex=0&amp;sortType=citingsrcslocalcount:desc&amp;searchType=ALL</t>
+  </si>
+  <si>
+    <t>/#/search?query=biology&amp;offsetIndex=0&amp;sortType=sortdate:desc&amp;searchType=ALL</t>
+  </si>
+  <si>
+    <t>/#/search?query=biology&amp;offsetIndex=0&amp;sortType=sortdate:asc&amp;searchType=ALL</t>
+  </si>
+  <si>
+    <t>/#/search?query=biology&amp;offsetIndex=0&amp;sortType=citingsrcslocalcount:desc&amp;searchType=ARTICLES</t>
+  </si>
+  <si>
+    <t>/#/search?query=biology&amp;offsetIndex=0&amp;sortType=sortdate:desc&amp;searchType=ARTICLES</t>
+  </si>
+  <si>
+    <t>/#/search?query=biology&amp;offsetIndex=0&amp;sortType=sortdate:asc&amp;searchType=ARTICLES</t>
+  </si>
+  <si>
+    <t>/#/search?query=biology&amp;offsetIndex=0&amp;sortType=citingsrcscount:desc&amp;searchType=PATENTS</t>
+  </si>
+  <si>
+    <t>/#/search?query=biology&amp;offsetIndex=0&amp;sortType=sortdate:desc&amp;searchType=PATENTS</t>
+  </si>
+  <si>
+    <t>/#/search?query=biology&amp;offsetIndex=0&amp;sortType=sortdate:asc&amp;searchType=PATENTS</t>
+  </si>
+  <si>
+    <t>/#/search?query=biology&amp;offsetIndex=0&amp;sortType=loadtime:desc&amp;searchType=PEOPLE</t>
+  </si>
+  <si>
+    <t>/#/search?query=post&amp;offsetIndex=0&amp;sortType=sortdate:desc&amp;searchType=POSTS</t>
+  </si>
+  <si>
+    <t>/#/search?query=biology&amp;offsetIndex=0&amp;sortType=sortdate:asc&amp;searchType=POSTS</t>
+  </si>
+  <si>
+    <t>/#/search?query=biology&amp;offsetIndex=0&amp;sortType=_score:desc&amp;searchType=POSTS</t>
   </si>
 </sst>
 </file>
@@ -1720,7 +1720,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C103" workbookViewId="0">
+    <sheetView topLeftCell="C103" workbookViewId="0">
       <selection activeCell="C107" sqref="C107"/>
     </sheetView>
   </sheetViews>
@@ -3534,10 +3534,10 @@
         <v>358</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>377</v>
+        <v>359</v>
       </c>
       <c r="C107" s="11" t="s">
-        <v>378</v>
+        <v>360</v>
       </c>
       <c r="D107" s="8" t="s">
         <v>326</v>
@@ -3554,7 +3554,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -3579,7 +3581,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="B2" t="s">
         <v>349</v>
@@ -3590,7 +3592,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="B3" t="s">
         <v>350</v>
@@ -3601,7 +3603,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="B4" t="s">
         <v>351</v>
@@ -3612,7 +3614,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="B5" t="s">
         <v>352</v>
@@ -3623,7 +3625,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="B6" t="s">
         <v>353</v>
@@ -3634,7 +3636,7 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="B7" t="s">
         <v>349</v>
@@ -3645,7 +3647,7 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="B8" t="s">
         <v>349</v>
@@ -3656,7 +3658,7 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="B9" t="s">
         <v>349</v>
@@ -3667,7 +3669,7 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="B10" t="s">
         <v>354</v>
@@ -3678,7 +3680,7 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="B11" t="s">
         <v>350</v>
@@ -3689,7 +3691,7 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="B12" t="s">
         <v>350</v>
@@ -3700,7 +3702,7 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="B13" t="s">
         <v>355</v>
@@ -3711,7 +3713,7 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="B14" t="s">
         <v>356</v>
@@ -3722,7 +3724,7 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="B15" t="s">
         <v>356</v>
@@ -3733,7 +3735,7 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="B16" t="s">
         <v>352</v>
@@ -3744,7 +3746,7 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="B17" t="s">
         <v>357</v>
@@ -3755,7 +3757,7 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="B18" t="s">
         <v>357</v>
@@ -3766,7 +3768,7 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="B19" t="s">
         <v>357</v>

</xml_diff>

<commit_message>
Added new test cases in search module
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Search.xlsx
+++ b/src/test/resources/xls/Search.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="14715" windowHeight="8040" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="14715" windowHeight="8040"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="382">
   <si>
     <t>TCID</t>
   </si>
@@ -1317,6 +1317,15 @@
   </si>
   <si>
     <t>/#/search?query=biology&amp;offsetIndex=0&amp;sortType=_score:desc&amp;searchType=POSTS</t>
+  </si>
+  <si>
+    <t>Search128</t>
+  </si>
+  <si>
+    <t>OPQA-3152|OPQA-3153|OPQA-3154|OPQA-3155</t>
+  </si>
+  <si>
+    <t>Verify that show all functionality of type ahead is working properly for all categories in type ahead</t>
   </si>
 </sst>
 </file>
@@ -1718,10 +1727,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E107"/>
+  <dimension ref="A1:E108"/>
   <sheetViews>
-    <sheetView topLeftCell="C103" workbookViewId="0">
-      <selection activeCell="C107" sqref="C107"/>
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="A116" sqref="A116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3544,6 +3553,21 @@
       </c>
       <c r="E107" s="3"/>
     </row>
+    <row r="108" spans="1:5">
+      <c r="A108" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="B108" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="C108" s="11" t="s">
+        <v>381</v>
+      </c>
+      <c r="D108" s="8" t="s">
+        <v>326</v>
+      </c>
+      <c r="E108" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3554,7 +3578,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added new test scripts in search module
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Search.xlsx
+++ b/src/test/resources/xls/Search.xlsx
@@ -449,20 +449,7 @@
 g)Comments count</t>
   </si>
   <si>
-    <t>Verify that following fields get displayed correctly for a patent in PATENTS search results page:
-a)Title
-b)Inventors
-c)Assignees
-d)Patent number
-e)Publication date
-f)Times cited count
-g)Comments count</t>
-  </si>
-  <si>
     <t>OPQA-613</t>
-  </si>
-  <si>
-    <t>OPQA-614</t>
   </si>
   <si>
     <t>Verify that following fields get displayed correctly for an patent in record view page:
@@ -531,22 +518,10 @@
     <t>OPQA-1239</t>
   </si>
   <si>
-    <t>OPQA-599</t>
-  </si>
-  <si>
     <t>OPQA-553</t>
   </si>
   <si>
     <t>Verify that following fields get displayed correctly for a post in ALL search results page: 
-a)Title 
-b)Creation date and time 
-c)Author 
-d)Author details 
-e)Likes count 
-f)Comments count</t>
-  </si>
-  <si>
-    <t>Verify that following fields get displayed correctly for a post in POSTS search results page: 
 a)Title 
 b)Creation date and time 
 c)Author 
@@ -721,15 +696,6 @@
     <t>OPQA-580</t>
   </si>
   <si>
-    <t>Verify that following fields get displayed correctly for an article in ARTICLES search results page:
-a)Title
-b)Authors
-c)Publication name
-d)Publication date
-e)Times cited count
-f)Comments count</t>
-  </si>
-  <si>
     <t>OPQA-1245</t>
   </si>
   <si>
@@ -1126,9 +1092,6 @@
     <t>Search120</t>
   </si>
   <si>
-    <t>Search121</t>
-  </si>
-  <si>
     <t>Search122</t>
   </si>
   <si>
@@ -1326,6 +1289,47 @@
   </si>
   <si>
     <t>Verify that show all functionality of type ahead is working properly for all categories in type ahead</t>
+  </si>
+  <si>
+    <t>Search121|OPQA-3173</t>
+  </si>
+  <si>
+    <t>Verify that following fields get displayed correctly for an article in ARTICLES search results page:
+a)Title
+b)Authors
+c)Publication name
+d)Publication date
+e)Times cited count
+f)Comments count
+g)Snippet of abstract</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that following fields get displayed correctly for a post in POSTS search results page: 
+a)Title 
+b)Creation date and time 
+c)Author 
+d)Author details 
+e)Likes count 
+f)Comments count
+g)Abstarct of snippet
+</t>
+  </si>
+  <si>
+    <t>OPQA-599|OPQA-3174</t>
+  </si>
+  <si>
+    <t>Verify that following fields get displayed correctly for a patent in PATENTS search results page:
+a)Title
+b)Inventors
+c)Assignees
+d)Patent number
+e)Publication date
+f)Times cited count
+g)Comments count
+h)Abstarct of snippet</t>
+  </si>
+  <si>
+    <t>OPQA-614|OPQA-3172</t>
   </si>
 </sst>
 </file>
@@ -1729,8 +1733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="A116" sqref="A116"/>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1761,7 +1765,7 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="8" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
@@ -1770,7 +1774,7 @@
         <v>70</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>88</v>
@@ -1778,7 +1782,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="8" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>32</v>
@@ -1787,7 +1791,7 @@
         <v>52</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>88</v>
@@ -1795,7 +1799,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="8" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>33</v>
@@ -1804,7 +1808,7 @@
         <v>53</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>88</v>
@@ -1812,7 +1816,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="8" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>34</v>
@@ -1821,7 +1825,7 @@
         <v>54</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E5" s="8" t="s">
         <v>88</v>
@@ -1829,7 +1833,7 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="8" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>35</v>
@@ -1838,7 +1842,7 @@
         <v>55</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>88</v>
@@ -1846,7 +1850,7 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="8" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>36</v>
@@ -1855,7 +1859,7 @@
         <v>56</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E7" s="8" t="s">
         <v>88</v>
@@ -1863,7 +1867,7 @@
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1">
       <c r="A8" s="8" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>50</v>
@@ -1872,7 +1876,7 @@
         <v>49</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E8" s="8" t="s">
         <v>88</v>
@@ -1880,16 +1884,16 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="8" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>57</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E9" s="8" t="s">
         <v>88</v>
@@ -1897,7 +1901,7 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="8" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>47</v>
@@ -1906,7 +1910,7 @@
         <v>58</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E10" s="8" t="s">
         <v>88</v>
@@ -1914,7 +1918,7 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="8" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>37</v>
@@ -1923,7 +1927,7 @@
         <v>59</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E11" s="8" t="s">
         <v>88</v>
@@ -1931,7 +1935,7 @@
     </row>
     <row r="12" spans="1:5" ht="16.5" customHeight="1">
       <c r="A12" s="8" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>38</v>
@@ -1940,7 +1944,7 @@
         <v>60</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E12" s="8" t="s">
         <v>88</v>
@@ -1948,7 +1952,7 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="8" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>46</v>
@@ -1957,7 +1961,7 @@
         <v>61</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E13" s="8" t="s">
         <v>88</v>
@@ -1965,16 +1969,16 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="8" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>62</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E14" s="8" t="s">
         <v>88</v>
@@ -1982,7 +1986,7 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="8" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>51</v>
@@ -1991,7 +1995,7 @@
         <v>83</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E15" s="8" t="s">
         <v>88</v>
@@ -1999,7 +2003,7 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="8" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>45</v>
@@ -2008,7 +2012,7 @@
         <v>63</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E16" s="8" t="s">
         <v>88</v>
@@ -2016,7 +2020,7 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="8" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>44</v>
@@ -2025,7 +2029,7 @@
         <v>64</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E17" s="8" t="s">
         <v>88</v>
@@ -2033,7 +2037,7 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="8" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>43</v>
@@ -2042,7 +2046,7 @@
         <v>65</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E18" s="8" t="s">
         <v>88</v>
@@ -2050,7 +2054,7 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="8" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>39</v>
@@ -2059,7 +2063,7 @@
         <v>66</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E19" s="8" t="s">
         <v>88</v>
@@ -2067,7 +2071,7 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="8" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>40</v>
@@ -2076,7 +2080,7 @@
         <v>67</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E20" s="8" t="s">
         <v>88</v>
@@ -2084,7 +2088,7 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="8" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="B21" s="7" t="s">
         <v>41</v>
@@ -2093,7 +2097,7 @@
         <v>68</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E21" s="8" t="s">
         <v>88</v>
@@ -2101,7 +2105,7 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="8" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>42</v>
@@ -2110,7 +2114,7 @@
         <v>69</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E22" s="8" t="s">
         <v>88</v>
@@ -2118,16 +2122,16 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="8" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="C23" s="8" t="s">
         <v>71</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E23" s="8" t="s">
         <v>88</v>
@@ -2135,16 +2139,16 @@
     </row>
     <row r="24" spans="1:5" ht="75">
       <c r="A24" s="8" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>72</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E24" s="8" t="s">
         <v>88</v>
@@ -2152,16 +2156,16 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="8" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C25" s="8" t="s">
         <v>73</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E25" s="8" t="s">
         <v>88</v>
@@ -2169,16 +2173,16 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="8" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>74</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E26" s="8" t="s">
         <v>88</v>
@@ -2186,16 +2190,16 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="8" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="C27" s="8" t="s">
         <v>75</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E27" s="8" t="s">
         <v>88</v>
@@ -2203,16 +2207,16 @@
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="8" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="C28" s="8" t="s">
         <v>76</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E28" s="8" t="s">
         <v>88</v>
@@ -2220,16 +2224,16 @@
     </row>
     <row r="29" spans="1:5" ht="90">
       <c r="A29" s="8" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="C29" s="7" t="s">
         <v>77</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E29" s="8" t="s">
         <v>88</v>
@@ -2237,16 +2241,16 @@
     </row>
     <row r="30" spans="1:5" ht="60">
       <c r="A30" s="8" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="C30" s="7" t="s">
         <v>78</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E30" s="8" t="s">
         <v>88</v>
@@ -2254,16 +2258,16 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="8" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="C31" s="7" t="s">
         <v>79</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E31" s="8" t="s">
         <v>88</v>
@@ -2271,16 +2275,16 @@
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="8" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="C32" s="7" t="s">
         <v>80</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E32" s="8" t="s">
         <v>88</v>
@@ -2288,16 +2292,16 @@
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="8" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="C33" s="8" t="s">
         <v>81</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E33" s="8" t="s">
         <v>88</v>
@@ -2305,16 +2309,16 @@
     </row>
     <row r="34" spans="1:5" ht="90">
       <c r="A34" s="8" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="C34" s="7" t="s">
         <v>82</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E34" s="8" t="s">
         <v>88</v>
@@ -2322,16 +2326,16 @@
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="8" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="C35" s="8" t="s">
         <v>83</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E35" s="8" t="s">
         <v>88</v>
@@ -2339,16 +2343,16 @@
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="8" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="C36" s="8" t="s">
         <v>84</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E36" s="8" t="s">
         <v>88</v>
@@ -2356,16 +2360,16 @@
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="8" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C37" s="8" t="s">
         <v>85</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E37" s="8" t="s">
         <v>88</v>
@@ -2373,16 +2377,16 @@
     </row>
     <row r="38" spans="1:5" ht="90">
       <c r="A38" s="8" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="C38" s="7" t="s">
         <v>86</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E38" s="8" t="s">
         <v>88</v>
@@ -2390,16 +2394,16 @@
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="8" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="C39" s="7" t="s">
         <v>87</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E39" s="8" t="s">
         <v>88</v>
@@ -2407,16 +2411,16 @@
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="8" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="C40" s="7" t="s">
         <v>89</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E40" s="8" t="s">
         <v>88</v>
@@ -2424,16 +2428,16 @@
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="8" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="C41" s="7" t="s">
         <v>90</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E41" s="8" t="s">
         <v>88</v>
@@ -2441,16 +2445,16 @@
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="8" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="C42" s="7" t="s">
         <v>91</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E42" s="8" t="s">
         <v>88</v>
@@ -2458,16 +2462,16 @@
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="8" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="B43" s="7" t="s">
         <v>92</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E43" s="8" t="s">
         <v>88</v>
@@ -2475,16 +2479,16 @@
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="8" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="B44" s="7" t="s">
         <v>93</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E44" s="8" t="s">
         <v>88</v>
@@ -2492,16 +2496,16 @@
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="8" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E45" s="8" t="s">
         <v>88</v>
@@ -2509,16 +2513,16 @@
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="8" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="B46" s="7" t="s">
         <v>48</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E46" s="8" t="s">
         <v>88</v>
@@ -2526,16 +2530,16 @@
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="8" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="B47" s="7" t="s">
         <v>94</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E47" s="8" t="s">
         <v>88</v>
@@ -2543,16 +2547,16 @@
     </row>
     <row r="48" spans="1:5" ht="120">
       <c r="A48" s="8" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="B48" s="7" t="s">
         <v>95</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E48" s="8" t="s">
         <v>88</v>
@@ -2560,7 +2564,7 @@
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="8" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="B49" s="7" t="s">
         <v>50</v>
@@ -2569,7 +2573,7 @@
         <v>49</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E49" s="8" t="s">
         <v>88</v>
@@ -2577,7 +2581,7 @@
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="8" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="B50" s="7" t="s">
         <v>97</v>
@@ -2586,7 +2590,7 @@
         <v>96</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E50" s="8" t="s">
         <v>88</v>
@@ -2594,7 +2598,7 @@
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="8" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="B51" s="7" t="s">
         <v>98</v>
@@ -2603,7 +2607,7 @@
         <v>99</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E51" s="8" t="s">
         <v>88</v>
@@ -2611,7 +2615,7 @@
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="8" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="B52" s="7" t="s">
         <v>101</v>
@@ -2620,7 +2624,7 @@
         <v>100</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E52" s="8" t="s">
         <v>88</v>
@@ -2628,16 +2632,16 @@
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="8" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="C53" s="7" t="s">
         <v>102</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E53" s="8" t="s">
         <v>88</v>
@@ -2645,16 +2649,16 @@
     </row>
     <row r="54" spans="1:5" ht="30">
       <c r="A54" s="8" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="B54" s="7" t="s">
         <v>103</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E54" s="8" t="s">
         <v>88</v>
@@ -2662,16 +2666,16 @@
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="8" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="B55" s="7" t="s">
         <v>104</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E55" s="8" t="s">
         <v>88</v>
@@ -2679,16 +2683,16 @@
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="8" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="B56" s="7" t="s">
         <v>105</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E56" s="8" t="s">
         <v>88</v>
@@ -2696,16 +2700,16 @@
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="8" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="B57" s="7" t="s">
         <v>106</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E57" s="8" t="s">
         <v>88</v>
@@ -2713,16 +2717,16 @@
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="8" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="B58" s="7" t="s">
         <v>107</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E58" s="8" t="s">
         <v>88</v>
@@ -2730,7 +2734,7 @@
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="8" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="B59" s="7" t="s">
         <v>108</v>
@@ -2739,7 +2743,7 @@
         <v>109</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E59" s="8" t="s">
         <v>88</v>
@@ -2747,16 +2751,16 @@
     </row>
     <row r="60" spans="1:5" ht="90">
       <c r="A60" s="8" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="B60" s="7" t="s">
         <v>110</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E60" s="8" t="s">
         <v>88</v>
@@ -2764,16 +2768,16 @@
     </row>
     <row r="61" spans="1:5" ht="75">
       <c r="A61" s="8" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="B61" s="7" t="s">
         <v>111</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E61" s="8" t="s">
         <v>88</v>
@@ -2781,7 +2785,7 @@
     </row>
     <row r="62" spans="1:5">
       <c r="A62" s="8" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="B62" s="7" t="s">
         <v>112</v>
@@ -2790,7 +2794,7 @@
         <v>113</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E62" s="8" t="s">
         <v>88</v>
@@ -2798,7 +2802,7 @@
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="8" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="B63" s="7" t="s">
         <v>114</v>
@@ -2807,7 +2811,7 @@
         <v>115</v>
       </c>
       <c r="D63" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E63" s="8" t="s">
         <v>88</v>
@@ -2815,7 +2819,7 @@
     </row>
     <row r="64" spans="1:5">
       <c r="A64" s="8" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="B64" s="7" t="s">
         <v>117</v>
@@ -2824,7 +2828,7 @@
         <v>116</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E64" s="8" t="s">
         <v>88</v>
@@ -2832,33 +2836,33 @@
     </row>
     <row r="65" spans="1:5" ht="120">
       <c r="A65" s="8" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C65" s="7" t="s">
         <v>118</v>
       </c>
       <c r="D65" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E65" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="66" spans="1:5" ht="120">
+    <row r="66" spans="1:5" ht="135">
       <c r="A66" s="8" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>121</v>
+        <v>381</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>119</v>
+        <v>380</v>
       </c>
       <c r="D66" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E66" s="8" t="s">
         <v>88</v>
@@ -2866,16 +2870,16 @@
     </row>
     <row r="67" spans="1:5" ht="195">
       <c r="A67" s="8" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C67" s="7" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D67" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E67" s="8" t="s">
         <v>88</v>
@@ -2883,16 +2887,16 @@
     </row>
     <row r="68" spans="1:5">
       <c r="A68" s="8" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="D68" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E68" s="8" t="s">
         <v>88</v>
@@ -2900,16 +2904,16 @@
     </row>
     <row r="69" spans="1:5">
       <c r="A69" s="8" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D69" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E69" s="8" t="s">
         <v>88</v>
@@ -2917,16 +2921,16 @@
     </row>
     <row r="70" spans="1:5">
       <c r="A70" s="8" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D70" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E70" s="8" t="s">
         <v>88</v>
@@ -2934,16 +2938,16 @@
     </row>
     <row r="71" spans="1:5" ht="30">
       <c r="A71" s="8" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D71" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E71" s="8" t="s">
         <v>88</v>
@@ -2951,16 +2955,16 @@
     </row>
     <row r="72" spans="1:5">
       <c r="A72" s="8" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D72" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E72" s="8" t="s">
         <v>88</v>
@@ -2968,16 +2972,16 @@
     </row>
     <row r="73" spans="1:5">
       <c r="A73" s="8" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C73" s="8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D73" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E73" s="8" t="s">
         <v>88</v>
@@ -2985,16 +2989,16 @@
     </row>
     <row r="74" spans="1:5">
       <c r="A74" s="8" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C74" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D74" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E74" s="8" t="s">
         <v>88</v>
@@ -3002,33 +3006,33 @@
     </row>
     <row r="75" spans="1:5">
       <c r="A75" s="8" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C75" s="8" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D75" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E75" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="76" spans="1:5" ht="105">
+    <row r="76" spans="1:5" ht="135">
       <c r="A76" s="8" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>140</v>
+        <v>379</v>
       </c>
       <c r="C76" s="7" t="s">
-        <v>142</v>
+        <v>378</v>
       </c>
       <c r="D76" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E76" s="8" t="s">
         <v>88</v>
@@ -3036,16 +3040,16 @@
     </row>
     <row r="77" spans="1:5" ht="105">
       <c r="A77" s="8" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C77" s="7" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="D77" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E77" s="8" t="s">
         <v>88</v>
@@ -3053,16 +3057,16 @@
     </row>
     <row r="78" spans="1:5">
       <c r="A78" s="8" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C78" s="7" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D78" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E78" s="8" t="s">
         <v>88</v>
@@ -3070,16 +3074,16 @@
     </row>
     <row r="79" spans="1:5">
       <c r="A79" s="8" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C79" s="7" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D79" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E79" s="8" t="s">
         <v>88</v>
@@ -3087,16 +3091,16 @@
     </row>
     <row r="80" spans="1:5" ht="45">
       <c r="A80" s="8" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C80" s="7" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D80" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E80" s="8" t="s">
         <v>88</v>
@@ -3104,16 +3108,16 @@
     </row>
     <row r="81" spans="1:5">
       <c r="A81" s="8" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C81" s="8" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D81" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E81" s="8" t="s">
         <v>88</v>
@@ -3121,16 +3125,16 @@
     </row>
     <row r="82" spans="1:5">
       <c r="A82" s="8" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="B82" s="8" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C82" s="8" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="D82" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E82" s="8" t="s">
         <v>88</v>
@@ -3138,16 +3142,16 @@
     </row>
     <row r="83" spans="1:5">
       <c r="A83" s="8" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="B83" s="8" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C83" s="8" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D83" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E83" s="8" t="s">
         <v>88</v>
@@ -3155,16 +3159,16 @@
     </row>
     <row r="84" spans="1:5">
       <c r="A84" s="8" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="B84" s="8" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C84" s="8" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="D84" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E84" s="8" t="s">
         <v>88</v>
@@ -3172,16 +3176,16 @@
     </row>
     <row r="85" spans="1:5">
       <c r="A85" s="8" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="B85" s="8" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C85" s="8" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="D85" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E85" s="8" t="s">
         <v>88</v>
@@ -3189,16 +3193,16 @@
     </row>
     <row r="86" spans="1:5" ht="165">
       <c r="A86" s="8" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="B86" s="8" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C86" s="7" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D86" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E86" s="8" t="s">
         <v>88</v>
@@ -3206,16 +3210,16 @@
     </row>
     <row r="87" spans="1:5" ht="75">
       <c r="A87" s="8" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="B87" s="9" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C87" s="7" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="D87" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E87" s="8" t="s">
         <v>88</v>
@@ -3223,16 +3227,16 @@
     </row>
     <row r="88" spans="1:5">
       <c r="A88" s="8" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="B88" s="7" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C88" s="7" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="D88" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E88" s="8" t="s">
         <v>88</v>
@@ -3240,16 +3244,16 @@
     </row>
     <row r="89" spans="1:5">
       <c r="A89" s="8" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C89" s="7" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="D89" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E89" s="8" t="s">
         <v>88</v>
@@ -3257,16 +3261,16 @@
     </row>
     <row r="90" spans="1:5">
       <c r="A90" s="8" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="B90" s="8" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C90" s="8" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="D90" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E90" s="8" t="s">
         <v>88</v>
@@ -3274,16 +3278,16 @@
     </row>
     <row r="91" spans="1:5">
       <c r="A91" s="8" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="B91" s="8" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C91" s="8" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="D91" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E91" s="8" t="s">
         <v>88</v>
@@ -3291,16 +3295,16 @@
     </row>
     <row r="92" spans="1:5">
       <c r="A92" s="8" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="B92" s="8" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C92" s="8" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D92" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E92" s="8" t="s">
         <v>88</v>
@@ -3308,16 +3312,16 @@
     </row>
     <row r="93" spans="1:5">
       <c r="A93" s="8" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="B93" s="8" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C93" s="8" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D93" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E93" s="8" t="s">
         <v>88</v>
@@ -3325,16 +3329,16 @@
     </row>
     <row r="94" spans="1:5">
       <c r="A94" s="8" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="B94" s="8" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C94" s="8" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D94" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E94" s="8" t="s">
         <v>88</v>
@@ -3342,16 +3346,16 @@
     </row>
     <row r="95" spans="1:5">
       <c r="A95" s="8" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="B95" s="8" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="C95" s="8" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="D95" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E95" s="8" t="s">
         <v>88</v>
@@ -3359,16 +3363,16 @@
     </row>
     <row r="96" spans="1:5">
       <c r="A96" s="8" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="B96" s="9" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C96" s="9" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="D96" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E96" s="8" t="s">
         <v>88</v>
@@ -3376,16 +3380,16 @@
     </row>
     <row r="97" spans="1:5" ht="30">
       <c r="A97" s="8" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="B97" s="9" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C97" s="10" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="D97" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E97" s="8" t="s">
         <v>88</v>
@@ -3393,16 +3397,16 @@
     </row>
     <row r="98" spans="1:5" ht="75">
       <c r="A98" s="8" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="B98" s="8" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C98" s="7" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D98" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E98" s="8" t="s">
         <v>88</v>
@@ -3410,16 +3414,16 @@
     </row>
     <row r="99" spans="1:5" ht="60">
       <c r="A99" s="8" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="B99" s="7" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C99" s="7" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="D99" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E99" s="8" t="s">
         <v>88</v>
@@ -3427,33 +3431,33 @@
     </row>
     <row r="100" spans="1:5" ht="105">
       <c r="A100" s="8" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="B100" s="7" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C100" s="7" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="D100" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E100" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="101" spans="1:5" ht="105">
+    <row r="101" spans="1:5" ht="120">
       <c r="A101" s="8" t="s">
-        <v>320</v>
+        <v>376</v>
       </c>
       <c r="B101" s="7" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C101" s="7" t="s">
-        <v>190</v>
+        <v>377</v>
       </c>
       <c r="D101" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E101" s="8" t="s">
         <v>88</v>
@@ -3461,16 +3465,16 @@
     </row>
     <row r="102" spans="1:5">
       <c r="A102" s="8" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="B102" s="7" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="C102" s="8" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="D102" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E102" s="8" t="s">
         <v>88</v>
@@ -3478,93 +3482,93 @@
     </row>
     <row r="103" spans="1:5">
       <c r="A103" s="8" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="B103" s="7" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="D103" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E103" s="8" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="104" spans="1:5">
       <c r="A104" s="8" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="D104" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E104" s="3"/>
     </row>
     <row r="105" spans="1:5">
       <c r="A105" s="8" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="D105" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E105" s="3"/>
     </row>
     <row r="106" spans="1:5" ht="150">
       <c r="A106" s="8" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="D106" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E106" s="3"/>
     </row>
     <row r="107" spans="1:5">
       <c r="A107" s="8" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
       <c r="C107" s="11" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="D107" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E107" s="3"/>
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="8" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>380</v>
+        <v>374</v>
       </c>
       <c r="C108" s="11" t="s">
-        <v>381</v>
+        <v>375</v>
       </c>
       <c r="D108" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E108" s="3"/>
     </row>
@@ -3591,13 +3595,13 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="B1" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="C1" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
@@ -3605,200 +3609,200 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="B2" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="C2" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="B3" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="C3" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="B4" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="C4" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="B5" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="C5" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="B6" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="C6" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
       <c r="B7" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="C7" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="B8" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="C8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
       <c r="B9" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="C9" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="B10" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="C10" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="B11" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="C11" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="B12" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="C12" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="B13" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="C13" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="B14" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="C14" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
       <c r="B15" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="C15" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
       <c r="B16" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="C16" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
       <c r="B17" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="C17" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
       <c r="B18" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="C18" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="B19" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="C19" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
failed test cases in search module
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Search.xlsx
+++ b/src/test/resources/xls/Search.xlsx
@@ -681,18 +681,6 @@
 c)Search drop down content type</t>
   </si>
   <si>
-    <t>OPQA-578</t>
-  </si>
-  <si>
-    <t>Verify that following fields get displayed correctly for an article in ALL search results page:
-a)Title
-b)Authors
-c)Publication name
-d)Publication date
-e)Times cited count
-f)Comments count</t>
-  </si>
-  <si>
     <t>OPQA-1245</t>
   </si>
   <si>
@@ -1330,6 +1318,19 @@
   </si>
   <si>
     <t>OPQA-580|OPQA-3173</t>
+  </si>
+  <si>
+    <t>OPQA-578|OPQA-3175</t>
+  </si>
+  <si>
+    <t>Verify that following fields get displayed correctly for an article in ALL search results page:
+a)Title
+b)Authors
+c)Publication name
+d)Publication date
+e)Times cited count
+f)Comments count
+g)Authors count</t>
   </si>
 </sst>
 </file>
@@ -1734,7 +1735,7 @@
   <dimension ref="A1:E108"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
-      <selection activeCell="B101" sqref="B101"/>
+      <selection activeCell="C100" sqref="C100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1765,7 +1766,7 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="8" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
@@ -1774,7 +1775,7 @@
         <v>70</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>88</v>
@@ -1782,7 +1783,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="8" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>32</v>
@@ -1791,7 +1792,7 @@
         <v>52</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>88</v>
@@ -1799,7 +1800,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="8" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>33</v>
@@ -1808,7 +1809,7 @@
         <v>53</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>88</v>
@@ -1816,7 +1817,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="8" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>34</v>
@@ -1825,7 +1826,7 @@
         <v>54</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E5" s="8" t="s">
         <v>88</v>
@@ -1833,7 +1834,7 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="8" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>35</v>
@@ -1842,7 +1843,7 @@
         <v>55</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>88</v>
@@ -1850,7 +1851,7 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="8" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>36</v>
@@ -1859,7 +1860,7 @@
         <v>56</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E7" s="8" t="s">
         <v>88</v>
@@ -1867,7 +1868,7 @@
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1">
       <c r="A8" s="8" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>50</v>
@@ -1876,7 +1877,7 @@
         <v>49</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E8" s="8" t="s">
         <v>88</v>
@@ -1884,16 +1885,16 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="8" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>57</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E9" s="8" t="s">
         <v>88</v>
@@ -1901,7 +1902,7 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="8" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>47</v>
@@ -1910,7 +1911,7 @@
         <v>58</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E10" s="8" t="s">
         <v>88</v>
@@ -1918,7 +1919,7 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="8" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>37</v>
@@ -1927,7 +1928,7 @@
         <v>59</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E11" s="8" t="s">
         <v>88</v>
@@ -1935,7 +1936,7 @@
     </row>
     <row r="12" spans="1:5" ht="16.5" customHeight="1">
       <c r="A12" s="8" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>38</v>
@@ -1944,7 +1945,7 @@
         <v>60</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E12" s="8" t="s">
         <v>88</v>
@@ -1952,7 +1953,7 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="8" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>46</v>
@@ -1961,7 +1962,7 @@
         <v>61</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E13" s="8" t="s">
         <v>88</v>
@@ -1969,16 +1970,16 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="8" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>62</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E14" s="8" t="s">
         <v>88</v>
@@ -1986,7 +1987,7 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="8" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>51</v>
@@ -1995,7 +1996,7 @@
         <v>83</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E15" s="8" t="s">
         <v>88</v>
@@ -2003,7 +2004,7 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="8" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>45</v>
@@ -2012,7 +2013,7 @@
         <v>63</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E16" s="8" t="s">
         <v>88</v>
@@ -2020,7 +2021,7 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="8" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>44</v>
@@ -2029,7 +2030,7 @@
         <v>64</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E17" s="8" t="s">
         <v>88</v>
@@ -2037,7 +2038,7 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="8" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>43</v>
@@ -2046,7 +2047,7 @@
         <v>65</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E18" s="8" t="s">
         <v>88</v>
@@ -2054,7 +2055,7 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="8" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>39</v>
@@ -2063,7 +2064,7 @@
         <v>66</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E19" s="8" t="s">
         <v>88</v>
@@ -2071,7 +2072,7 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>40</v>
@@ -2080,7 +2081,7 @@
         <v>67</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E20" s="8" t="s">
         <v>88</v>
@@ -2088,7 +2089,7 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="8" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B21" s="7" t="s">
         <v>41</v>
@@ -2097,7 +2098,7 @@
         <v>68</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E21" s="8" t="s">
         <v>88</v>
@@ -2105,7 +2106,7 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="8" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>42</v>
@@ -2114,7 +2115,7 @@
         <v>69</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E22" s="8" t="s">
         <v>88</v>
@@ -2122,16 +2123,16 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="8" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C23" s="8" t="s">
         <v>71</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E23" s="8" t="s">
         <v>88</v>
@@ -2139,16 +2140,16 @@
     </row>
     <row r="24" spans="1:5" ht="75">
       <c r="A24" s="8" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>72</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E24" s="8" t="s">
         <v>88</v>
@@ -2156,16 +2157,16 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="8" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C25" s="8" t="s">
         <v>73</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E25" s="8" t="s">
         <v>88</v>
@@ -2173,16 +2174,16 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>74</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E26" s="8" t="s">
         <v>88</v>
@@ -2190,16 +2191,16 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="8" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C27" s="8" t="s">
         <v>75</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E27" s="8" t="s">
         <v>88</v>
@@ -2207,16 +2208,16 @@
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="8" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C28" s="8" t="s">
         <v>76</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E28" s="8" t="s">
         <v>88</v>
@@ -2224,16 +2225,16 @@
     </row>
     <row r="29" spans="1:5" ht="90">
       <c r="A29" s="8" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C29" s="7" t="s">
         <v>77</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E29" s="8" t="s">
         <v>88</v>
@@ -2241,16 +2242,16 @@
     </row>
     <row r="30" spans="1:5" ht="60">
       <c r="A30" s="8" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C30" s="7" t="s">
         <v>78</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E30" s="8" t="s">
         <v>88</v>
@@ -2258,16 +2259,16 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="8" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C31" s="7" t="s">
         <v>79</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E31" s="8" t="s">
         <v>88</v>
@@ -2275,16 +2276,16 @@
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="8" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C32" s="7" t="s">
         <v>80</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E32" s="8" t="s">
         <v>88</v>
@@ -2292,16 +2293,16 @@
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="8" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C33" s="8" t="s">
         <v>81</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E33" s="8" t="s">
         <v>88</v>
@@ -2309,16 +2310,16 @@
     </row>
     <row r="34" spans="1:5" ht="90">
       <c r="A34" s="8" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C34" s="7" t="s">
         <v>82</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E34" s="8" t="s">
         <v>88</v>
@@ -2326,16 +2327,16 @@
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="8" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C35" s="8" t="s">
         <v>83</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E35" s="8" t="s">
         <v>88</v>
@@ -2343,16 +2344,16 @@
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="8" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C36" s="8" t="s">
         <v>84</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E36" s="8" t="s">
         <v>88</v>
@@ -2360,16 +2361,16 @@
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="8" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C37" s="8" t="s">
         <v>85</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E37" s="8" t="s">
         <v>88</v>
@@ -2377,16 +2378,16 @@
     </row>
     <row r="38" spans="1:5" ht="90">
       <c r="A38" s="8" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C38" s="7" t="s">
         <v>86</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E38" s="8" t="s">
         <v>88</v>
@@ -2394,16 +2395,16 @@
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="8" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C39" s="7" t="s">
         <v>87</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E39" s="8" t="s">
         <v>88</v>
@@ -2411,16 +2412,16 @@
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="8" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C40" s="7" t="s">
         <v>89</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E40" s="8" t="s">
         <v>88</v>
@@ -2428,16 +2429,16 @@
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="8" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C41" s="7" t="s">
         <v>90</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E41" s="8" t="s">
         <v>88</v>
@@ -2445,16 +2446,16 @@
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="8" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C42" s="7" t="s">
         <v>91</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E42" s="8" t="s">
         <v>88</v>
@@ -2462,16 +2463,16 @@
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="8" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B43" s="7" t="s">
         <v>92</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E43" s="8" t="s">
         <v>88</v>
@@ -2479,16 +2480,16 @@
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="8" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B44" s="7" t="s">
         <v>93</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E44" s="8" t="s">
         <v>88</v>
@@ -2496,16 +2497,16 @@
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="8" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E45" s="8" t="s">
         <v>88</v>
@@ -2513,16 +2514,16 @@
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="8" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B46" s="7" t="s">
         <v>48</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E46" s="8" t="s">
         <v>88</v>
@@ -2530,16 +2531,16 @@
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="8" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B47" s="7" t="s">
         <v>94</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E47" s="8" t="s">
         <v>88</v>
@@ -2547,16 +2548,16 @@
     </row>
     <row r="48" spans="1:5" ht="120">
       <c r="A48" s="8" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B48" s="7" t="s">
         <v>95</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E48" s="8" t="s">
         <v>88</v>
@@ -2564,7 +2565,7 @@
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="8" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B49" s="7" t="s">
         <v>50</v>
@@ -2573,7 +2574,7 @@
         <v>49</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E49" s="8" t="s">
         <v>88</v>
@@ -2581,7 +2582,7 @@
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="8" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B50" s="7" t="s">
         <v>97</v>
@@ -2590,7 +2591,7 @@
         <v>96</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E50" s="8" t="s">
         <v>88</v>
@@ -2598,7 +2599,7 @@
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="8" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B51" s="7" t="s">
         <v>98</v>
@@ -2607,7 +2608,7 @@
         <v>99</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E51" s="8" t="s">
         <v>88</v>
@@ -2615,7 +2616,7 @@
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="8" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B52" s="7" t="s">
         <v>101</v>
@@ -2624,7 +2625,7 @@
         <v>100</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E52" s="8" t="s">
         <v>88</v>
@@ -2632,16 +2633,16 @@
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="8" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C53" s="7" t="s">
         <v>102</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E53" s="8" t="s">
         <v>88</v>
@@ -2649,16 +2650,16 @@
     </row>
     <row r="54" spans="1:5" ht="30">
       <c r="A54" s="8" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B54" s="7" t="s">
         <v>103</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E54" s="8" t="s">
         <v>88</v>
@@ -2666,16 +2667,16 @@
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="8" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B55" s="7" t="s">
         <v>104</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E55" s="8" t="s">
         <v>88</v>
@@ -2683,16 +2684,16 @@
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="8" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B56" s="7" t="s">
         <v>105</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E56" s="8" t="s">
         <v>88</v>
@@ -2700,16 +2701,16 @@
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="8" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B57" s="7" t="s">
         <v>106</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E57" s="8" t="s">
         <v>88</v>
@@ -2717,16 +2718,16 @@
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="8" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B58" s="7" t="s">
         <v>107</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E58" s="8" t="s">
         <v>88</v>
@@ -2734,7 +2735,7 @@
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="8" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B59" s="7" t="s">
         <v>108</v>
@@ -2743,7 +2744,7 @@
         <v>109</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E59" s="8" t="s">
         <v>88</v>
@@ -2751,16 +2752,16 @@
     </row>
     <row r="60" spans="1:5" ht="90">
       <c r="A60" s="8" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B60" s="7" t="s">
         <v>110</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E60" s="8" t="s">
         <v>88</v>
@@ -2768,16 +2769,16 @@
     </row>
     <row r="61" spans="1:5" ht="75">
       <c r="A61" s="8" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B61" s="7" t="s">
         <v>111</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E61" s="8" t="s">
         <v>88</v>
@@ -2785,7 +2786,7 @@
     </row>
     <row r="62" spans="1:5">
       <c r="A62" s="8" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B62" s="7" t="s">
         <v>112</v>
@@ -2794,7 +2795,7 @@
         <v>113</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E62" s="8" t="s">
         <v>88</v>
@@ -2802,7 +2803,7 @@
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="8" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B63" s="7" t="s">
         <v>114</v>
@@ -2811,7 +2812,7 @@
         <v>115</v>
       </c>
       <c r="D63" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E63" s="8" t="s">
         <v>88</v>
@@ -2819,7 +2820,7 @@
     </row>
     <row r="64" spans="1:5">
       <c r="A64" s="8" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B64" s="7" t="s">
         <v>117</v>
@@ -2828,7 +2829,7 @@
         <v>116</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E64" s="8" t="s">
         <v>88</v>
@@ -2836,7 +2837,7 @@
     </row>
     <row r="65" spans="1:5" ht="120">
       <c r="A65" s="8" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B65" s="7" t="s">
         <v>119</v>
@@ -2845,7 +2846,7 @@
         <v>118</v>
       </c>
       <c r="D65" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E65" s="8" t="s">
         <v>88</v>
@@ -2853,16 +2854,16 @@
     </row>
     <row r="66" spans="1:5" ht="135">
       <c r="A66" s="8" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="D66" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E66" s="8" t="s">
         <v>88</v>
@@ -2870,7 +2871,7 @@
     </row>
     <row r="67" spans="1:5" ht="195">
       <c r="A67" s="8" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B67" s="7" t="s">
         <v>121</v>
@@ -2879,7 +2880,7 @@
         <v>120</v>
       </c>
       <c r="D67" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E67" s="8" t="s">
         <v>88</v>
@@ -2887,16 +2888,16 @@
     </row>
     <row r="68" spans="1:5">
       <c r="A68" s="8" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B68" s="7" t="s">
         <v>123</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="D68" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E68" s="8" t="s">
         <v>88</v>
@@ -2904,7 +2905,7 @@
     </row>
     <row r="69" spans="1:5">
       <c r="A69" s="8" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B69" s="7" t="s">
         <v>124</v>
@@ -2913,7 +2914,7 @@
         <v>122</v>
       </c>
       <c r="D69" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E69" s="8" t="s">
         <v>88</v>
@@ -2921,7 +2922,7 @@
     </row>
     <row r="70" spans="1:5">
       <c r="A70" s="8" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B70" s="7" t="s">
         <v>125</v>
@@ -2930,7 +2931,7 @@
         <v>126</v>
       </c>
       <c r="D70" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E70" s="8" t="s">
         <v>88</v>
@@ -2938,7 +2939,7 @@
     </row>
     <row r="71" spans="1:5" ht="30">
       <c r="A71" s="8" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B71" s="7" t="s">
         <v>128</v>
@@ -2947,7 +2948,7 @@
         <v>127</v>
       </c>
       <c r="D71" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E71" s="8" t="s">
         <v>88</v>
@@ -2955,7 +2956,7 @@
     </row>
     <row r="72" spans="1:5">
       <c r="A72" s="8" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B72" s="7" t="s">
         <v>129</v>
@@ -2964,7 +2965,7 @@
         <v>130</v>
       </c>
       <c r="D72" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E72" s="8" t="s">
         <v>88</v>
@@ -2972,7 +2973,7 @@
     </row>
     <row r="73" spans="1:5">
       <c r="A73" s="8" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B73" s="7" t="s">
         <v>133</v>
@@ -2981,7 +2982,7 @@
         <v>132</v>
       </c>
       <c r="D73" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E73" s="8" t="s">
         <v>88</v>
@@ -2989,7 +2990,7 @@
     </row>
     <row r="74" spans="1:5">
       <c r="A74" s="8" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B74" s="7" t="s">
         <v>134</v>
@@ -2998,7 +2999,7 @@
         <v>135</v>
       </c>
       <c r="D74" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E74" s="8" t="s">
         <v>88</v>
@@ -3006,7 +3007,7 @@
     </row>
     <row r="75" spans="1:5">
       <c r="A75" s="8" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B75" s="7" t="s">
         <v>137</v>
@@ -3015,7 +3016,7 @@
         <v>136</v>
       </c>
       <c r="D75" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E75" s="8" t="s">
         <v>88</v>
@@ -3023,16 +3024,16 @@
     </row>
     <row r="76" spans="1:5" ht="135">
       <c r="A76" s="8" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C76" s="7" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="D76" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E76" s="8" t="s">
         <v>88</v>
@@ -3040,7 +3041,7 @@
     </row>
     <row r="77" spans="1:5" ht="105">
       <c r="A77" s="8" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B77" s="7" t="s">
         <v>138</v>
@@ -3049,7 +3050,7 @@
         <v>139</v>
       </c>
       <c r="D77" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E77" s="8" t="s">
         <v>88</v>
@@ -3057,7 +3058,7 @@
     </row>
     <row r="78" spans="1:5">
       <c r="A78" s="8" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B78" s="7" t="s">
         <v>140</v>
@@ -3066,7 +3067,7 @@
         <v>141</v>
       </c>
       <c r="D78" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E78" s="8" t="s">
         <v>88</v>
@@ -3074,7 +3075,7 @@
     </row>
     <row r="79" spans="1:5">
       <c r="A79" s="8" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B79" s="7" t="s">
         <v>142</v>
@@ -3083,7 +3084,7 @@
         <v>143</v>
       </c>
       <c r="D79" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E79" s="8" t="s">
         <v>88</v>
@@ -3091,7 +3092,7 @@
     </row>
     <row r="80" spans="1:5" ht="45">
       <c r="A80" s="8" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B80" s="7" t="s">
         <v>145</v>
@@ -3100,7 +3101,7 @@
         <v>144</v>
       </c>
       <c r="D80" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E80" s="8" t="s">
         <v>88</v>
@@ -3108,7 +3109,7 @@
     </row>
     <row r="81" spans="1:5">
       <c r="A81" s="8" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B81" s="8" t="s">
         <v>146</v>
@@ -3117,7 +3118,7 @@
         <v>147</v>
       </c>
       <c r="D81" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E81" s="8" t="s">
         <v>88</v>
@@ -3125,7 +3126,7 @@
     </row>
     <row r="82" spans="1:5">
       <c r="A82" s="8" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B82" s="8" t="s">
         <v>148</v>
@@ -3134,7 +3135,7 @@
         <v>149</v>
       </c>
       <c r="D82" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E82" s="8" t="s">
         <v>88</v>
@@ -3142,7 +3143,7 @@
     </row>
     <row r="83" spans="1:5">
       <c r="A83" s="8" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B83" s="8" t="s">
         <v>150</v>
@@ -3151,7 +3152,7 @@
         <v>151</v>
       </c>
       <c r="D83" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E83" s="8" t="s">
         <v>88</v>
@@ -3159,7 +3160,7 @@
     </row>
     <row r="84" spans="1:5">
       <c r="A84" s="8" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B84" s="8" t="s">
         <v>152</v>
@@ -3168,7 +3169,7 @@
         <v>153</v>
       </c>
       <c r="D84" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E84" s="8" t="s">
         <v>88</v>
@@ -3176,7 +3177,7 @@
     </row>
     <row r="85" spans="1:5">
       <c r="A85" s="8" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B85" s="8" t="s">
         <v>154</v>
@@ -3185,7 +3186,7 @@
         <v>155</v>
       </c>
       <c r="D85" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E85" s="8" t="s">
         <v>88</v>
@@ -3193,7 +3194,7 @@
     </row>
     <row r="86" spans="1:5" ht="165">
       <c r="A86" s="8" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B86" s="8" t="s">
         <v>157</v>
@@ -3202,7 +3203,7 @@
         <v>156</v>
       </c>
       <c r="D86" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E86" s="8" t="s">
         <v>88</v>
@@ -3210,7 +3211,7 @@
     </row>
     <row r="87" spans="1:5" ht="75">
       <c r="A87" s="8" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B87" s="9" t="s">
         <v>175</v>
@@ -3219,7 +3220,7 @@
         <v>174</v>
       </c>
       <c r="D87" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E87" s="8" t="s">
         <v>88</v>
@@ -3227,7 +3228,7 @@
     </row>
     <row r="88" spans="1:5">
       <c r="A88" s="8" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B88" s="7" t="s">
         <v>158</v>
@@ -3236,7 +3237,7 @@
         <v>159</v>
       </c>
       <c r="D88" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E88" s="8" t="s">
         <v>88</v>
@@ -3244,7 +3245,7 @@
     </row>
     <row r="89" spans="1:5">
       <c r="A89" s="8" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B89" s="7" t="s">
         <v>160</v>
@@ -3253,7 +3254,7 @@
         <v>161</v>
       </c>
       <c r="D89" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E89" s="8" t="s">
         <v>88</v>
@@ -3261,7 +3262,7 @@
     </row>
     <row r="90" spans="1:5">
       <c r="A90" s="8" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B90" s="8" t="s">
         <v>164</v>
@@ -3270,7 +3271,7 @@
         <v>165</v>
       </c>
       <c r="D90" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E90" s="8" t="s">
         <v>88</v>
@@ -3278,7 +3279,7 @@
     </row>
     <row r="91" spans="1:5">
       <c r="A91" s="8" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B91" s="8" t="s">
         <v>162</v>
@@ -3287,7 +3288,7 @@
         <v>163</v>
       </c>
       <c r="D91" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E91" s="8" t="s">
         <v>88</v>
@@ -3295,7 +3296,7 @@
     </row>
     <row r="92" spans="1:5">
       <c r="A92" s="8" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B92" s="8" t="s">
         <v>166</v>
@@ -3304,7 +3305,7 @@
         <v>167</v>
       </c>
       <c r="D92" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E92" s="8" t="s">
         <v>88</v>
@@ -3312,7 +3313,7 @@
     </row>
     <row r="93" spans="1:5">
       <c r="A93" s="8" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B93" s="8" t="s">
         <v>169</v>
@@ -3321,7 +3322,7 @@
         <v>168</v>
       </c>
       <c r="D93" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E93" s="8" t="s">
         <v>88</v>
@@ -3329,7 +3330,7 @@
     </row>
     <row r="94" spans="1:5">
       <c r="A94" s="8" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B94" s="8" t="s">
         <v>170</v>
@@ -3338,7 +3339,7 @@
         <v>171</v>
       </c>
       <c r="D94" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E94" s="8" t="s">
         <v>88</v>
@@ -3346,7 +3347,7 @@
     </row>
     <row r="95" spans="1:5">
       <c r="A95" s="8" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B95" s="8" t="s">
         <v>172</v>
@@ -3355,7 +3356,7 @@
         <v>173</v>
       </c>
       <c r="D95" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E95" s="8" t="s">
         <v>88</v>
@@ -3363,7 +3364,7 @@
     </row>
     <row r="96" spans="1:5">
       <c r="A96" s="8" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B96" s="9" t="s">
         <v>177</v>
@@ -3372,7 +3373,7 @@
         <v>176</v>
       </c>
       <c r="D96" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E96" s="8" t="s">
         <v>88</v>
@@ -3380,16 +3381,16 @@
     </row>
     <row r="97" spans="1:5" ht="30">
       <c r="A97" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B97" s="9" t="s">
         <v>178</v>
       </c>
       <c r="C97" s="10" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D97" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E97" s="8" t="s">
         <v>88</v>
@@ -3397,7 +3398,7 @@
     </row>
     <row r="98" spans="1:5" ht="75">
       <c r="A98" s="8" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B98" s="8" t="s">
         <v>179</v>
@@ -3406,7 +3407,7 @@
         <v>180</v>
       </c>
       <c r="D98" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E98" s="8" t="s">
         <v>88</v>
@@ -3414,7 +3415,7 @@
     </row>
     <row r="99" spans="1:5" ht="60">
       <c r="A99" s="8" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B99" s="7" t="s">
         <v>181</v>
@@ -3423,24 +3424,24 @@
         <v>182</v>
       </c>
       <c r="D99" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E99" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="100" spans="1:5" ht="105">
+    <row r="100" spans="1:5" ht="120">
       <c r="A100" s="8" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B100" s="7" t="s">
-        <v>183</v>
+        <v>380</v>
       </c>
       <c r="C100" s="7" t="s">
-        <v>184</v>
+        <v>381</v>
       </c>
       <c r="D100" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E100" s="8" t="s">
         <v>88</v>
@@ -3448,16 +3449,16 @@
     </row>
     <row r="101" spans="1:5" ht="120">
       <c r="A101" s="8" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B101" s="7" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C101" s="7" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D101" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E101" s="8" t="s">
         <v>88</v>
@@ -3465,16 +3466,16 @@
     </row>
     <row r="102" spans="1:5">
       <c r="A102" s="8" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B102" s="7" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C102" s="8" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D102" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E102" s="8" t="s">
         <v>88</v>
@@ -3482,16 +3483,16 @@
     </row>
     <row r="103" spans="1:5">
       <c r="A103" s="8" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B103" s="7" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D103" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E103" s="8" t="s">
         <v>131</v>
@@ -3499,76 +3500,76 @@
     </row>
     <row r="104" spans="1:5">
       <c r="A104" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D104" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E104" s="3"/>
     </row>
     <row r="105" spans="1:5">
       <c r="A105" s="8" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D105" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E105" s="3"/>
     </row>
     <row r="106" spans="1:5" ht="150">
       <c r="A106" s="8" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D106" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E106" s="3"/>
     </row>
     <row r="107" spans="1:5">
       <c r="A107" s="8" t="s">
+        <v>349</v>
+      </c>
+      <c r="B107" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="C107" s="11" t="s">
         <v>351</v>
       </c>
-      <c r="B107" s="3" t="s">
-        <v>352</v>
-      </c>
-      <c r="C107" s="11" t="s">
-        <v>353</v>
-      </c>
       <c r="D107" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E107" s="3"/>
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="8" t="s">
+        <v>370</v>
+      </c>
+      <c r="B108" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="C108" s="11" t="s">
         <v>372</v>
       </c>
-      <c r="B108" s="3" t="s">
-        <v>373</v>
-      </c>
-      <c r="C108" s="11" t="s">
-        <v>374</v>
-      </c>
       <c r="D108" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E108" s="3"/>
     </row>
@@ -3595,13 +3596,13 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
+        <v>337</v>
+      </c>
+      <c r="B1" t="s">
+        <v>338</v>
+      </c>
+      <c r="C1" t="s">
         <v>339</v>
-      </c>
-      <c r="B1" t="s">
-        <v>340</v>
-      </c>
-      <c r="C1" t="s">
-        <v>341</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
@@ -3609,200 +3610,200 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B2" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C2" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B3" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C3" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B4" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C4" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B5" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C5" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C6" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B7" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C7" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B9" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C9" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B10" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C10" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B11" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C11" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B12" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C12" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B13" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C13" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B14" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C14" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B15" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C15" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B16" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C16" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="B17" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C17" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B18" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C18" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="B19" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C19" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified testcases in Search module
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Search.xlsx
+++ b/src/test/resources/xls/Search.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="382">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="381">
   <si>
     <t>TCID</t>
   </si>
@@ -796,9 +796,6 @@
   </si>
   <si>
     <t>Search6</t>
-  </si>
-  <si>
-    <t>Search7</t>
   </si>
   <si>
     <t>Search8</t>
@@ -1732,10 +1729,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E108"/>
+  <dimension ref="A1:E107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
-      <selection activeCell="C100" sqref="C100"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1775,7 +1772,7 @@
         <v>70</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>88</v>
@@ -1792,7 +1789,7 @@
         <v>52</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>88</v>
@@ -1809,7 +1806,7 @@
         <v>53</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>88</v>
@@ -1826,7 +1823,7 @@
         <v>54</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E5" s="8" t="s">
         <v>88</v>
@@ -1843,7 +1840,7 @@
         <v>55</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>88</v>
@@ -1860,7 +1857,7 @@
         <v>56</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E7" s="8" t="s">
         <v>88</v>
@@ -1871,13 +1868,13 @@
         <v>219</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>50</v>
+        <v>319</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E8" s="8" t="s">
         <v>88</v>
@@ -1888,13 +1885,13 @@
         <v>220</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>320</v>
+        <v>47</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E9" s="8" t="s">
         <v>88</v>
@@ -1905,13 +1902,13 @@
         <v>221</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E10" s="8" t="s">
         <v>88</v>
@@ -1922,13 +1919,13 @@
         <v>222</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E11" s="8" t="s">
         <v>88</v>
@@ -1939,13 +1936,13 @@
         <v>223</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>60</v>
+        <v>46</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>61</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E12" s="8" t="s">
         <v>88</v>
@@ -1956,13 +1953,13 @@
         <v>224</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>46</v>
+        <v>320</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E13" s="8" t="s">
         <v>88</v>
@@ -1973,13 +1970,13 @@
         <v>225</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>321</v>
+        <v>51</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>62</v>
+        <v>83</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E14" s="8" t="s">
         <v>88</v>
@@ -1990,13 +1987,13 @@
         <v>226</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>83</v>
+        <v>63</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E15" s="8" t="s">
         <v>88</v>
@@ -2007,13 +2004,13 @@
         <v>227</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E16" s="8" t="s">
         <v>88</v>
@@ -2024,13 +2021,13 @@
         <v>228</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E17" s="8" t="s">
         <v>88</v>
@@ -2041,13 +2038,13 @@
         <v>229</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>65</v>
+        <v>39</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>66</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E18" s="8" t="s">
         <v>88</v>
@@ -2058,13 +2055,13 @@
         <v>230</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E19" s="8" t="s">
         <v>88</v>
@@ -2075,13 +2072,13 @@
         <v>231</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E20" s="8" t="s">
         <v>88</v>
@@ -2092,13 +2089,13 @@
         <v>232</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E21" s="8" t="s">
         <v>88</v>
@@ -2109,47 +2106,47 @@
         <v>233</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>69</v>
+        <v>193</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>71</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E22" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" ht="75">
       <c r="A23" s="8" t="s">
         <v>234</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>71</v>
+        <v>194</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>72</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E23" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="75">
+    <row r="24" spans="1:5">
       <c r="A24" s="8" t="s">
         <v>235</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>194</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>72</v>
+        <v>195</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>73</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E24" s="8" t="s">
         <v>88</v>
@@ -2160,13 +2157,13 @@
         <v>236</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E25" s="8" t="s">
         <v>88</v>
@@ -2177,13 +2174,13 @@
         <v>237</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E26" s="8" t="s">
         <v>88</v>
@@ -2194,64 +2191,64 @@
         <v>238</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E27" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" ht="90">
       <c r="A28" s="8" t="s">
         <v>239</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>76</v>
+        <v>199</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>77</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E28" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="90">
+    <row r="29" spans="1:5" ht="60">
       <c r="A29" s="8" t="s">
         <v>240</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E29" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="60">
+    <row r="30" spans="1:5">
       <c r="A30" s="8" t="s">
         <v>241</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E30" s="8" t="s">
         <v>88</v>
@@ -2262,13 +2259,13 @@
         <v>242</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E31" s="8" t="s">
         <v>88</v>
@@ -2278,48 +2275,48 @@
       <c r="A32" s="8" t="s">
         <v>243</v>
       </c>
-      <c r="B32" s="7" t="s">
-        <v>202</v>
-      </c>
-      <c r="C32" s="7" t="s">
-        <v>80</v>
+      <c r="B32" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>81</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E32" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" ht="90">
       <c r="A33" s="8" t="s">
         <v>244</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>203</v>
-      </c>
-      <c r="C33" s="8" t="s">
-        <v>81</v>
+        <v>204</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>82</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E33" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="90">
+    <row r="34" spans="1:5">
       <c r="A34" s="8" t="s">
         <v>245</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>204</v>
-      </c>
-      <c r="C34" s="7" t="s">
-        <v>82</v>
+        <v>205</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E34" s="8" t="s">
         <v>88</v>
@@ -2330,13 +2327,13 @@
         <v>246</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E35" s="8" t="s">
         <v>88</v>
@@ -2347,47 +2344,47 @@
         <v>247</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E36" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" ht="90">
       <c r="A37" s="8" t="s">
         <v>248</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>207</v>
-      </c>
-      <c r="C37" s="8" t="s">
-        <v>85</v>
+        <v>208</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>86</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E37" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="90">
+    <row r="38" spans="1:5">
       <c r="A38" s="8" t="s">
         <v>249</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E38" s="8" t="s">
         <v>88</v>
@@ -2398,13 +2395,13 @@
         <v>250</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E39" s="8" t="s">
         <v>88</v>
@@ -2415,13 +2412,13 @@
         <v>251</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E40" s="8" t="s">
         <v>88</v>
@@ -2432,13 +2429,13 @@
         <v>252</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E41" s="8" t="s">
         <v>88</v>
@@ -2448,14 +2445,14 @@
       <c r="A42" s="8" t="s">
         <v>253</v>
       </c>
-      <c r="B42" s="8" t="s">
-        <v>212</v>
+      <c r="B42" s="7" t="s">
+        <v>92</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>91</v>
+        <v>325</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E42" s="8" t="s">
         <v>88</v>
@@ -2466,13 +2463,13 @@
         <v>254</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E43" s="8" t="s">
         <v>88</v>
@@ -2483,13 +2480,13 @@
         <v>255</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>93</v>
+        <v>326</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E44" s="8" t="s">
         <v>88</v>
@@ -2500,13 +2497,13 @@
         <v>256</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>327</v>
+        <v>48</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E45" s="8" t="s">
         <v>88</v>
@@ -2517,47 +2514,47 @@
         <v>257</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>48</v>
+        <v>94</v>
       </c>
       <c r="C46" s="7" t="s">
         <v>324</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E46" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" ht="120">
       <c r="A47" s="8" t="s">
         <v>258</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E47" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="120">
+    <row r="48" spans="1:5">
       <c r="A48" s="8" t="s">
         <v>259</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>95</v>
+        <v>50</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>318</v>
+        <v>49</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E48" s="8" t="s">
         <v>88</v>
@@ -2568,13 +2565,13 @@
         <v>260</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>50</v>
+        <v>97</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>49</v>
+        <v>96</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E49" s="8" t="s">
         <v>88</v>
@@ -2585,13 +2582,13 @@
         <v>261</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E50" s="8" t="s">
         <v>88</v>
@@ -2602,13 +2599,13 @@
         <v>262</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E51" s="8" t="s">
         <v>88</v>
@@ -2619,47 +2616,47 @@
         <v>263</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>101</v>
+        <v>327</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E52" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" ht="30">
       <c r="A53" s="8" t="s">
         <v>264</v>
       </c>
       <c r="B53" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C53" s="7" t="s">
         <v>328</v>
       </c>
-      <c r="C53" s="7" t="s">
-        <v>102</v>
-      </c>
       <c r="D53" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E53" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="30">
+    <row r="54" spans="1:5">
       <c r="A54" s="8" t="s">
         <v>265</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>329</v>
+        <v>335</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E54" s="8" t="s">
         <v>88</v>
@@ -2670,13 +2667,13 @@
         <v>266</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E55" s="8" t="s">
         <v>88</v>
@@ -2687,13 +2684,13 @@
         <v>267</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C56" s="7" t="s">
         <v>333</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E56" s="8" t="s">
         <v>88</v>
@@ -2704,13 +2701,13 @@
         <v>268</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C57" s="7" t="s">
         <v>334</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E57" s="8" t="s">
         <v>88</v>
@@ -2721,64 +2718,64 @@
         <v>269</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>335</v>
+        <v>109</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E58" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:5" ht="90">
       <c r="A59" s="8" t="s">
         <v>270</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>109</v>
+        <v>329</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E59" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="90">
+    <row r="60" spans="1:5" ht="75">
       <c r="A60" s="8" t="s">
         <v>271</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C60" s="7" t="s">
         <v>330</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E60" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="75">
+    <row r="61" spans="1:5">
       <c r="A61" s="8" t="s">
         <v>272</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>331</v>
+        <v>113</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E61" s="8" t="s">
         <v>88</v>
@@ -2789,13 +2786,13 @@
         <v>273</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E62" s="8" t="s">
         <v>88</v>
@@ -2806,81 +2803,81 @@
         <v>274</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D63" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E63" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:5" ht="120">
       <c r="A64" s="8" t="s">
         <v>275</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E64" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="120">
+    <row r="65" spans="1:5" ht="135">
       <c r="A65" s="8" t="s">
         <v>276</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>119</v>
+        <v>376</v>
       </c>
       <c r="C65" s="7" t="s">
-        <v>118</v>
+        <v>375</v>
       </c>
       <c r="D65" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E65" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="66" spans="1:5" ht="135">
+    <row r="66" spans="1:5" ht="195">
       <c r="A66" s="8" t="s">
         <v>277</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>377</v>
+        <v>121</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>376</v>
+        <v>120</v>
       </c>
       <c r="D66" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E66" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="195">
+    <row r="67" spans="1:5">
       <c r="A67" s="8" t="s">
         <v>278</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C67" s="7" t="s">
-        <v>120</v>
+        <v>331</v>
       </c>
       <c r="D67" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E67" s="8" t="s">
         <v>88</v>
@@ -2891,13 +2888,13 @@
         <v>279</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>332</v>
+        <v>122</v>
       </c>
       <c r="D68" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E68" s="8" t="s">
         <v>88</v>
@@ -2908,47 +2905,47 @@
         <v>280</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="D69" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E69" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="70" spans="1:5">
+    <row r="70" spans="1:5" ht="30">
       <c r="A70" s="8" t="s">
         <v>281</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D70" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E70" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="71" spans="1:5" ht="30">
+    <row r="71" spans="1:5">
       <c r="A71" s="8" t="s">
         <v>282</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="D71" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E71" s="8" t="s">
         <v>88</v>
@@ -2959,13 +2956,13 @@
         <v>283</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="C72" s="7" t="s">
-        <v>130</v>
+        <v>133</v>
+      </c>
+      <c r="C72" s="8" t="s">
+        <v>132</v>
       </c>
       <c r="D72" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E72" s="8" t="s">
         <v>88</v>
@@ -2976,13 +2973,13 @@
         <v>284</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C73" s="8" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="D73" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E73" s="8" t="s">
         <v>88</v>
@@ -2993,64 +2990,64 @@
         <v>285</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="C74" s="8" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D74" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E74" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="75" spans="1:5">
+    <row r="75" spans="1:5" ht="135">
       <c r="A75" s="8" t="s">
         <v>286</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="C75" s="8" t="s">
-        <v>136</v>
+        <v>374</v>
+      </c>
+      <c r="C75" s="7" t="s">
+        <v>373</v>
       </c>
       <c r="D75" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E75" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="76" spans="1:5" ht="135">
+    <row r="76" spans="1:5" ht="105">
       <c r="A76" s="8" t="s">
         <v>287</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>375</v>
+        <v>138</v>
       </c>
       <c r="C76" s="7" t="s">
-        <v>374</v>
+        <v>139</v>
       </c>
       <c r="D76" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E76" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="77" spans="1:5" ht="105">
+    <row r="77" spans="1:5">
       <c r="A77" s="8" t="s">
         <v>288</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C77" s="7" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="D77" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E77" s="8" t="s">
         <v>88</v>
@@ -3061,47 +3058,47 @@
         <v>289</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C78" s="7" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D78" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E78" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="79" spans="1:5">
+    <row r="79" spans="1:5" ht="45">
       <c r="A79" s="8" t="s">
         <v>290</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="C79" s="7" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D79" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E79" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="80" spans="1:5" ht="45">
+    <row r="80" spans="1:5">
       <c r="A80" s="8" t="s">
         <v>291</v>
       </c>
-      <c r="B80" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="C80" s="7" t="s">
-        <v>144</v>
+      <c r="B80" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="C80" s="8" t="s">
+        <v>147</v>
       </c>
       <c r="D80" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E80" s="8" t="s">
         <v>88</v>
@@ -3112,13 +3109,13 @@
         <v>292</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C81" s="8" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="D81" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E81" s="8" t="s">
         <v>88</v>
@@ -3129,13 +3126,13 @@
         <v>293</v>
       </c>
       <c r="B82" s="8" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C82" s="8" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="D82" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E82" s="8" t="s">
         <v>88</v>
@@ -3146,13 +3143,13 @@
         <v>294</v>
       </c>
       <c r="B83" s="8" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="C83" s="8" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="D83" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E83" s="8" t="s">
         <v>88</v>
@@ -3163,64 +3160,64 @@
         <v>295</v>
       </c>
       <c r="B84" s="8" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C84" s="8" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="D84" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E84" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="85" spans="1:5">
+    <row r="85" spans="1:5" ht="165">
       <c r="A85" s="8" t="s">
         <v>296</v>
       </c>
       <c r="B85" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="C85" s="8" t="s">
-        <v>155</v>
+        <v>157</v>
+      </c>
+      <c r="C85" s="7" t="s">
+        <v>156</v>
       </c>
       <c r="D85" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E85" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="86" spans="1:5" ht="165">
+    <row r="86" spans="1:5" ht="75">
       <c r="A86" s="8" t="s">
         <v>297</v>
       </c>
-      <c r="B86" s="8" t="s">
-        <v>157</v>
+      <c r="B86" s="9" t="s">
+        <v>175</v>
       </c>
       <c r="C86" s="7" t="s">
-        <v>156</v>
+        <v>174</v>
       </c>
       <c r="D86" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E86" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="87" spans="1:5" ht="75">
+    <row r="87" spans="1:5">
       <c r="A87" s="8" t="s">
         <v>298</v>
       </c>
-      <c r="B87" s="9" t="s">
-        <v>175</v>
+      <c r="B87" s="7" t="s">
+        <v>158</v>
       </c>
       <c r="C87" s="7" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
       <c r="D87" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E87" s="8" t="s">
         <v>88</v>
@@ -3231,13 +3228,13 @@
         <v>299</v>
       </c>
       <c r="B88" s="7" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C88" s="7" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="D88" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E88" s="8" t="s">
         <v>88</v>
@@ -3247,14 +3244,14 @@
       <c r="A89" s="8" t="s">
         <v>300</v>
       </c>
-      <c r="B89" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="C89" s="7" t="s">
-        <v>161</v>
+      <c r="B89" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="C89" s="8" t="s">
+        <v>165</v>
       </c>
       <c r="D89" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E89" s="8" t="s">
         <v>88</v>
@@ -3265,13 +3262,13 @@
         <v>301</v>
       </c>
       <c r="B90" s="8" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C90" s="8" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D90" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E90" s="8" t="s">
         <v>88</v>
@@ -3282,13 +3279,13 @@
         <v>302</v>
       </c>
       <c r="B91" s="8" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="C91" s="8" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="D91" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E91" s="8" t="s">
         <v>88</v>
@@ -3299,13 +3296,13 @@
         <v>303</v>
       </c>
       <c r="B92" s="8" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="C92" s="8" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D92" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E92" s="8" t="s">
         <v>88</v>
@@ -3316,13 +3313,13 @@
         <v>304</v>
       </c>
       <c r="B93" s="8" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C93" s="8" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="D93" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E93" s="8" t="s">
         <v>88</v>
@@ -3333,13 +3330,13 @@
         <v>305</v>
       </c>
       <c r="B94" s="8" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C94" s="8" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="D94" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E94" s="8" t="s">
         <v>88</v>
@@ -3349,82 +3346,82 @@
       <c r="A95" s="8" t="s">
         <v>306</v>
       </c>
-      <c r="B95" s="8" t="s">
-        <v>172</v>
-      </c>
-      <c r="C95" s="8" t="s">
-        <v>173</v>
+      <c r="B95" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="C95" s="9" t="s">
+        <v>176</v>
       </c>
       <c r="D95" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E95" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="96" spans="1:5">
+    <row r="96" spans="1:5" ht="30">
       <c r="A96" s="8" t="s">
         <v>307</v>
       </c>
       <c r="B96" s="9" t="s">
-        <v>177</v>
-      </c>
-      <c r="C96" s="9" t="s">
-        <v>176</v>
+        <v>178</v>
+      </c>
+      <c r="C96" s="10" t="s">
+        <v>318</v>
       </c>
       <c r="D96" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E96" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="97" spans="1:5" ht="30">
+    <row r="97" spans="1:5" ht="75">
       <c r="A97" s="8" t="s">
         <v>308</v>
       </c>
-      <c r="B97" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="C97" s="10" t="s">
-        <v>319</v>
+      <c r="B97" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="C97" s="7" t="s">
+        <v>180</v>
       </c>
       <c r="D97" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E97" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="98" spans="1:5" ht="75">
+    <row r="98" spans="1:5" ht="60">
       <c r="A98" s="8" t="s">
         <v>309</v>
       </c>
-      <c r="B98" s="8" t="s">
-        <v>179</v>
+      <c r="B98" s="7" t="s">
+        <v>181</v>
       </c>
       <c r="C98" s="7" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="D98" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E98" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="99" spans="1:5" ht="60">
+    <row r="99" spans="1:5" ht="120">
       <c r="A99" s="8" t="s">
         <v>310</v>
       </c>
       <c r="B99" s="7" t="s">
-        <v>181</v>
+        <v>379</v>
       </c>
       <c r="C99" s="7" t="s">
-        <v>182</v>
+        <v>380</v>
       </c>
       <c r="D99" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E99" s="8" t="s">
         <v>88</v>
@@ -3432,33 +3429,33 @@
     </row>
     <row r="100" spans="1:5" ht="120">
       <c r="A100" s="8" t="s">
+        <v>377</v>
+      </c>
+      <c r="B100" s="7" t="s">
+        <v>378</v>
+      </c>
+      <c r="C100" s="7" t="s">
+        <v>372</v>
+      </c>
+      <c r="D100" s="8" t="s">
+        <v>316</v>
+      </c>
+      <c r="E100" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5">
+      <c r="A101" s="8" t="s">
         <v>311</v>
       </c>
-      <c r="B100" s="7" t="s">
-        <v>380</v>
-      </c>
-      <c r="C100" s="7" t="s">
-        <v>381</v>
-      </c>
-      <c r="D100" s="8" t="s">
-        <v>317</v>
-      </c>
-      <c r="E100" s="8" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" ht="120">
-      <c r="A101" s="8" t="s">
-        <v>378</v>
-      </c>
       <c r="B101" s="7" t="s">
-        <v>379</v>
-      </c>
-      <c r="C101" s="7" t="s">
-        <v>373</v>
+        <v>183</v>
+      </c>
+      <c r="C101" s="8" t="s">
+        <v>184</v>
       </c>
       <c r="D101" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E101" s="8" t="s">
         <v>88</v>
@@ -3469,109 +3466,92 @@
         <v>312</v>
       </c>
       <c r="B102" s="7" t="s">
-        <v>183</v>
-      </c>
-      <c r="C102" s="8" t="s">
-        <v>184</v>
+        <v>185</v>
+      </c>
+      <c r="C102" s="3" t="s">
+        <v>186</v>
       </c>
       <c r="D102" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E102" s="8" t="s">
-        <v>88</v>
+        <v>131</v>
       </c>
     </row>
     <row r="103" spans="1:5">
       <c r="A103" s="8" t="s">
         <v>313</v>
       </c>
-      <c r="B103" s="7" t="s">
-        <v>185</v>
+      <c r="B103" s="3" t="s">
+        <v>187</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="D103" s="8" t="s">
-        <v>317</v>
-      </c>
-      <c r="E103" s="8" t="s">
-        <v>131</v>
-      </c>
+        <v>316</v>
+      </c>
+      <c r="E103" s="3"/>
     </row>
     <row r="104" spans="1:5">
       <c r="A104" s="8" t="s">
         <v>314</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="D104" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E104" s="3"/>
     </row>
-    <row r="105" spans="1:5">
+    <row r="105" spans="1:5" ht="150">
       <c r="A105" s="8" t="s">
         <v>315</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="C105" s="3" t="s">
-        <v>190</v>
+        <v>191</v>
+      </c>
+      <c r="C105" s="4" t="s">
+        <v>192</v>
       </c>
       <c r="D105" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E105" s="3"/>
     </row>
-    <row r="106" spans="1:5" ht="150">
+    <row r="106" spans="1:5">
       <c r="A106" s="8" t="s">
-        <v>316</v>
+        <v>348</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="C106" s="4" t="s">
-        <v>192</v>
+        <v>349</v>
+      </c>
+      <c r="C106" s="11" t="s">
+        <v>350</v>
       </c>
       <c r="D106" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E106" s="3"/>
     </row>
     <row r="107" spans="1:5">
       <c r="A107" s="8" t="s">
-        <v>349</v>
+        <v>369</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>350</v>
+        <v>370</v>
       </c>
       <c r="C107" s="11" t="s">
-        <v>351</v>
+        <v>371</v>
       </c>
       <c r="D107" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E107" s="3"/>
-    </row>
-    <row r="108" spans="1:5">
-      <c r="A108" s="8" t="s">
-        <v>370</v>
-      </c>
-      <c r="B108" s="3" t="s">
-        <v>371</v>
-      </c>
-      <c r="C108" s="11" t="s">
-        <v>372</v>
-      </c>
-      <c r="D108" s="8" t="s">
-        <v>317</v>
-      </c>
-      <c r="E108" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3596,13 +3576,13 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
+        <v>336</v>
+      </c>
+      <c r="B1" t="s">
         <v>337</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>338</v>
-      </c>
-      <c r="C1" t="s">
-        <v>339</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
@@ -3610,200 +3590,200 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B3" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C3" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B4" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C4" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B5" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C5" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B6" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C6" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B7" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C7" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B8" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B9" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C9" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B10" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C10" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B11" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C11" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B12" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C12" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B13" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C13" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B14" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C14" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B15" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C15" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B16" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C16" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B17" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C17" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B18" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C18" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B19" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C19" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified scripts in search module
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Search.xlsx
+++ b/src/test/resources/xls/Search.xlsx
@@ -1150,9 +1150,6 @@
 d)Date(Oldest)</t>
   </si>
   <si>
-    <t>Verify that record view page of a artcle gets displayed when user clicks on article title in ALL search results page</t>
-  </si>
-  <si>
     <t xml:space="preserve">Verify that record view of a patent gets displayed when user clicks on any patent option in the search type ahead </t>
   </si>
   <si>
@@ -1328,6 +1325,9 @@
 e)Times cited count
 f)Comments count
 g)Authors count</t>
+  </si>
+  <si>
+    <t>Verify that record view page of a article gets displayed when user clicks on article title in ALL search results page</t>
   </si>
 </sst>
 </file>
@@ -1731,8 +1731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E107"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:E8"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="C68" sqref="C68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2653,7 +2653,7 @@
         <v>104</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D54" s="8" t="s">
         <v>316</v>
@@ -2670,7 +2670,7 @@
         <v>105</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D55" s="8" t="s">
         <v>316</v>
@@ -2687,7 +2687,7 @@
         <v>106</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D56" s="8" t="s">
         <v>316</v>
@@ -2704,7 +2704,7 @@
         <v>107</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D57" s="8" t="s">
         <v>316</v>
@@ -2837,10 +2837,10 @@
         <v>276</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C65" s="7" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D65" s="8" t="s">
         <v>316</v>
@@ -2874,7 +2874,7 @@
         <v>123</v>
       </c>
       <c r="C67" s="7" t="s">
-        <v>331</v>
+        <v>380</v>
       </c>
       <c r="D67" s="8" t="s">
         <v>316</v>
@@ -3007,10 +3007,10 @@
         <v>286</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C75" s="7" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D75" s="8" t="s">
         <v>316</v>
@@ -3415,10 +3415,10 @@
         <v>310</v>
       </c>
       <c r="B99" s="7" t="s">
+        <v>378</v>
+      </c>
+      <c r="C99" s="7" t="s">
         <v>379</v>
-      </c>
-      <c r="C99" s="7" t="s">
-        <v>380</v>
       </c>
       <c r="D99" s="8" t="s">
         <v>316</v>
@@ -3429,13 +3429,13 @@
     </row>
     <row r="100" spans="1:5" ht="120">
       <c r="A100" s="8" t="s">
+        <v>376</v>
+      </c>
+      <c r="B100" s="7" t="s">
         <v>377</v>
       </c>
-      <c r="B100" s="7" t="s">
-        <v>378</v>
-      </c>
       <c r="C100" s="7" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D100" s="8" t="s">
         <v>316</v>
@@ -3525,13 +3525,13 @@
     </row>
     <row r="106" spans="1:5">
       <c r="A106" s="8" t="s">
+        <v>347</v>
+      </c>
+      <c r="B106" s="3" t="s">
         <v>348</v>
       </c>
-      <c r="B106" s="3" t="s">
+      <c r="C106" s="11" t="s">
         <v>349</v>
-      </c>
-      <c r="C106" s="11" t="s">
-        <v>350</v>
       </c>
       <c r="D106" s="8" t="s">
         <v>316</v>
@@ -3540,13 +3540,13 @@
     </row>
     <row r="107" spans="1:5">
       <c r="A107" s="8" t="s">
+        <v>368</v>
+      </c>
+      <c r="B107" s="3" t="s">
         <v>369</v>
       </c>
-      <c r="B107" s="3" t="s">
+      <c r="C107" s="11" t="s">
         <v>370</v>
-      </c>
-      <c r="C107" s="11" t="s">
-        <v>371</v>
       </c>
       <c r="D107" s="8" t="s">
         <v>316</v>
@@ -3576,13 +3576,13 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
+        <v>335</v>
+      </c>
+      <c r="B1" t="s">
         <v>336</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>337</v>
-      </c>
-      <c r="C1" t="s">
-        <v>338</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
@@ -3590,10 +3590,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C2" t="s">
         <v>316</v>
@@ -3601,10 +3601,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B3" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C3" t="s">
         <v>316</v>
@@ -3612,10 +3612,10 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C4" t="s">
         <v>316</v>
@@ -3623,10 +3623,10 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B5" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C5" t="s">
         <v>316</v>
@@ -3634,10 +3634,10 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B6" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C6" t="s">
         <v>316</v>
@@ -3645,10 +3645,10 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B7" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C7" t="s">
         <v>316</v>
@@ -3656,10 +3656,10 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B8" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C8" t="s">
         <v>316</v>
@@ -3667,10 +3667,10 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B9" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C9" t="s">
         <v>316</v>
@@ -3678,10 +3678,10 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B10" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C10" t="s">
         <v>316</v>
@@ -3689,10 +3689,10 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B11" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C11" t="s">
         <v>316</v>
@@ -3700,10 +3700,10 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B12" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C12" t="s">
         <v>316</v>
@@ -3711,10 +3711,10 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B13" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C13" t="s">
         <v>316</v>
@@ -3722,10 +3722,10 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B14" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C14" t="s">
         <v>316</v>
@@ -3733,10 +3733,10 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B15" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C15" t="s">
         <v>316</v>
@@ -3744,10 +3744,10 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B16" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C16" t="s">
         <v>316</v>
@@ -3755,10 +3755,10 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B17" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C17" t="s">
         <v>316</v>
@@ -3766,10 +3766,10 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B18" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C18" t="s">
         <v>316</v>
@@ -3777,10 +3777,10 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B19" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C19" t="s">
         <v>316</v>

</xml_diff>

<commit_message>
Added new testcase in search module
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Search.xlsx
+++ b/src/test/resources/xls/Search.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="384">
   <si>
     <t>TCID</t>
   </si>
@@ -1329,12 +1329,21 @@
   <si>
     <t>Verify that record view page of a article gets displayed when user clicks on article title in ALL search results page</t>
   </si>
+  <si>
+    <t>Search129</t>
+  </si>
+  <si>
+    <t>Verify that Deep linking is working for Search result page using Linkedin account</t>
+  </si>
+  <si>
+    <t>OPQA-2839|OPQA-2842|OPQA-2843|OPQA-2844|OPQA-2845|OPQA-2846|OPQA-2847|OPQA-2848|OPQA-2849|OPQA-2850|OPQA-2851|OPQA-2852|OPQA-2853|OPQA-2854|OPQA-2855|OPQA-2856|OPQA-2857|OPQA-2858</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1356,6 +1365,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1402,10 +1424,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1430,8 +1456,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1729,10 +1757,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E107"/>
+  <dimension ref="A1:E108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="C68" sqref="C68"/>
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="B108" sqref="B108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3553,9 +3581,27 @@
       </c>
       <c r="E107" s="3"/>
     </row>
+    <row r="108" spans="1:5">
+      <c r="A108" s="8" t="s">
+        <v>381</v>
+      </c>
+      <c r="B108" s="12" t="s">
+        <v>383</v>
+      </c>
+      <c r="C108" s="11" t="s">
+        <v>382</v>
+      </c>
+      <c r="D108" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="E108" s="3"/>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B108" r:id="rId1" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-2839"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
added test script in search
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Search.xlsx
+++ b/src/test/resources/xls/Search.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="386">
   <si>
     <t>TCID</t>
   </si>
@@ -1337,6 +1337,12 @@
   </si>
   <si>
     <t>OPQA-2839|OPQA-2842|OPQA-2843|OPQA-2844|OPQA-2845|OPQA-2846|OPQA-2847|OPQA-2848|OPQA-2849|OPQA-2850|OPQA-2851|OPQA-2852|OPQA-2853|OPQA-2854|OPQA-2855|OPQA-2856|OPQA-2857|OPQA-2858</t>
+  </si>
+  <si>
+    <t>Search130</t>
+  </si>
+  <si>
+    <t>Verify that Deep linking is working for Search result page using Facebook account</t>
   </si>
 </sst>
 </file>
@@ -1757,10 +1763,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E108"/>
+  <dimension ref="A1:E109"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="B108" sqref="B108"/>
+      <selection activeCell="C116" sqref="C116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3596,12 +3602,28 @@
       </c>
       <c r="E108" s="3"/>
     </row>
+    <row r="109" spans="1:5">
+      <c r="A109" s="8" t="s">
+        <v>384</v>
+      </c>
+      <c r="B109" s="12" t="s">
+        <v>383</v>
+      </c>
+      <c r="C109" s="11" t="s">
+        <v>385</v>
+      </c>
+      <c r="D109" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="E109" s="3"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B108" r:id="rId1" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-2839"/>
+    <hyperlink ref="B109" r:id="rId2" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-2839"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Modidified xlsx file data
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Search.xlsx
+++ b/src/test/resources/xls/Search.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2580" windowWidth="14715" windowHeight="8040"/>
@@ -711,9 +711,6 @@
     <t>OPQA-1435</t>
   </si>
   <si>
-    <t>OPQA-1436</t>
-  </si>
-  <si>
     <t>OPQA-1437</t>
   </si>
   <si>
@@ -1344,12 +1341,15 @@
   <si>
     <t>Verify that search left navigationpane  content type is retained when user navigates back to PATENTS search results page from record view page</t>
   </si>
+  <si>
+    <t>OPQA-1436||OPQA-1408</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1524,7 +1524,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1556,10 +1556,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1591,7 +1590,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1767,14 +1765,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
-      <selection activeCell="C82" sqref="C82"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.42578125" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1" collapsed="1"/>
@@ -1783,7 +1781,7 @@
     <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1800,9 +1798,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
@@ -1811,15 +1809,15 @@
         <v>70</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="8" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>32</v>
@@ -1828,15 +1826,15 @@
         <v>52</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="8" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>33</v>
@@ -1845,15 +1843,15 @@
         <v>53</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>34</v>
@@ -1862,15 +1860,15 @@
         <v>54</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E5" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>35</v>
@@ -1879,15 +1877,15 @@
         <v>55</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>36</v>
@@ -1896,32 +1894,32 @@
         <v>56</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E7" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="15" customHeight="1">
       <c r="A8" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>57</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E8" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="8" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>47</v>
@@ -1930,15 +1928,15 @@
         <v>58</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E9" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>37</v>
@@ -1947,15 +1945,15 @@
         <v>59</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E10" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" s="8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>38</v>
@@ -1964,15 +1962,15 @@
         <v>60</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E11" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="16.5" customHeight="1">
       <c r="A12" s="8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>46</v>
@@ -1981,32 +1979,32 @@
         <v>61</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E12" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" s="8" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>62</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E13" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" s="8" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>51</v>
@@ -2015,15 +2013,15 @@
         <v>83</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E14" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" s="8" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>45</v>
@@ -2032,15 +2030,15 @@
         <v>63</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E15" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" s="8" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>44</v>
@@ -2049,15 +2047,15 @@
         <v>64</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E16" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" s="8" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>43</v>
@@ -2066,15 +2064,15 @@
         <v>65</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E17" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" s="8" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>39</v>
@@ -2083,15 +2081,15 @@
         <v>66</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E18" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19" s="8" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>40</v>
@@ -2100,15 +2098,15 @@
         <v>67</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E19" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="A20" s="8" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>41</v>
@@ -2117,15 +2115,15 @@
         <v>68</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E20" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="A21" s="8" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B21" s="7" t="s">
         <v>42</v>
@@ -2134,15 +2132,15 @@
         <v>69</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E21" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22" s="8" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>188</v>
@@ -2151,15 +2149,15 @@
         <v>71</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E22" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="75">
       <c r="A23" s="8" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B23" s="7" t="s">
         <v>189</v>
@@ -2168,423 +2166,423 @@
         <v>72</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E23" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5">
       <c r="A24" s="8" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>190</v>
+        <v>385</v>
       </c>
       <c r="C24" s="8" t="s">
         <v>73</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E24" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5">
       <c r="A25" s="8" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C25" s="8" t="s">
         <v>74</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E25" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5">
       <c r="A26" s="8" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>75</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E26" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5">
       <c r="A27" s="8" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C27" s="8" t="s">
         <v>76</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E27" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="90">
       <c r="A28" s="8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C28" s="7" t="s">
         <v>77</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E28" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="60">
       <c r="A29" s="8" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C29" s="7" t="s">
         <v>78</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E29" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5">
       <c r="A30" s="8" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C30" s="7" t="s">
         <v>79</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E30" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5">
       <c r="A31" s="8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C31" s="7" t="s">
         <v>80</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E31" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5">
       <c r="A32" s="8" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C32" s="8" t="s">
         <v>81</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E32" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" ht="90">
       <c r="A33" s="8" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C33" s="7" t="s">
         <v>82</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E33" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5">
       <c r="A34" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C34" s="8" t="s">
         <v>83</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E34" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5">
       <c r="A35" s="8" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C35" s="8" t="s">
         <v>84</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E35" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5">
       <c r="A36" s="8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C36" s="8" t="s">
         <v>85</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E36" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" ht="90">
       <c r="A37" s="8" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C37" s="7" t="s">
         <v>86</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E37" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5">
       <c r="A38" s="8" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C38" s="7" t="s">
         <v>87</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E38" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5">
       <c r="A39" s="8" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C39" s="7" t="s">
         <v>89</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E39" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5">
       <c r="A40" s="8" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C40" s="7" t="s">
         <v>90</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E40" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5">
       <c r="A41" s="8" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C41" s="7" t="s">
         <v>91</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E41" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5">
       <c r="A42" s="8" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B42" s="7" t="s">
         <v>92</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E42" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5">
       <c r="A43" s="8" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B43" s="7" t="s">
         <v>93</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E43" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5">
       <c r="A44" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>320</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>315</v>
+      </c>
+      <c r="D44" s="8" t="s">
+        <v>310</v>
+      </c>
+      <c r="E44" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" s="8" t="s">
         <v>250</v>
-      </c>
-      <c r="B44" s="7" t="s">
-        <v>321</v>
-      </c>
-      <c r="C44" s="7" t="s">
-        <v>316</v>
-      </c>
-      <c r="D44" s="8" t="s">
-        <v>311</v>
-      </c>
-      <c r="E44" s="8" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="8" t="s">
-        <v>251</v>
       </c>
       <c r="B45" s="7" t="s">
         <v>48</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E45" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5">
       <c r="A46" s="8" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B46" s="7" t="s">
         <v>94</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E46" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" ht="120">
       <c r="A47" s="8" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B47" s="7" t="s">
         <v>95</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E47" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5">
       <c r="A48" s="8" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B48" s="7" t="s">
         <v>50</v>
@@ -2593,15 +2591,15 @@
         <v>49</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E48" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5">
       <c r="A49" s="8" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B49" s="7" t="s">
         <v>97</v>
@@ -2610,15 +2608,15 @@
         <v>96</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E49" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5">
       <c r="A50" s="8" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B50" s="7" t="s">
         <v>98</v>
@@ -2627,15 +2625,15 @@
         <v>99</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E50" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5">
       <c r="A51" s="8" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B51" s="7" t="s">
         <v>101</v>
@@ -2644,117 +2642,117 @@
         <v>100</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E51" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5">
       <c r="A52" s="8" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C52" s="7" t="s">
         <v>102</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E52" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" ht="30">
       <c r="A53" s="8" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B53" s="7" t="s">
         <v>103</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E53" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5">
       <c r="A54" s="8" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B54" s="7" t="s">
         <v>104</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E54" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5">
       <c r="A55" s="8" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B55" s="7" t="s">
         <v>105</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E55" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5">
       <c r="A56" s="8" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B56" s="7" t="s">
         <v>106</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E56" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5">
       <c r="A57" s="8" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B57" s="7" t="s">
         <v>107</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E57" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5">
       <c r="A58" s="8" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B58" s="7" t="s">
         <v>108</v>
@@ -2763,49 +2761,49 @@
         <v>109</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E58" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" ht="90">
       <c r="A59" s="8" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B59" s="7" t="s">
         <v>110</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E59" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" ht="75">
       <c r="A60" s="8" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B60" s="7" t="s">
         <v>111</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E60" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5">
       <c r="A61" s="8" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B61" s="7" t="s">
         <v>112</v>
@@ -2814,15 +2812,15 @@
         <v>113</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E61" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5">
       <c r="A62" s="8" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B62" s="7" t="s">
         <v>114</v>
@@ -2831,15 +2829,15 @@
         <v>115</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E62" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5">
       <c r="A63" s="8" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B63" s="7" t="s">
         <v>117</v>
@@ -2848,15 +2846,15 @@
         <v>116</v>
       </c>
       <c r="D63" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E63" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" ht="120">
       <c r="A64" s="8" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B64" s="7" t="s">
         <v>119</v>
@@ -2865,32 +2863,32 @@
         <v>118</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E64" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" ht="135">
       <c r="A65" s="8" t="s">
+        <v>270</v>
+      </c>
+      <c r="B65" s="7" t="s">
+        <v>373</v>
+      </c>
+      <c r="C65" s="7" t="s">
+        <v>365</v>
+      </c>
+      <c r="D65" s="8" t="s">
+        <v>310</v>
+      </c>
+      <c r="E65" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="195">
+      <c r="A66" s="8" t="s">
         <v>271</v>
-      </c>
-      <c r="B65" s="7" t="s">
-        <v>374</v>
-      </c>
-      <c r="C65" s="7" t="s">
-        <v>366</v>
-      </c>
-      <c r="D65" s="8" t="s">
-        <v>311</v>
-      </c>
-      <c r="E65" s="8" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" ht="195" x14ac:dyDescent="0.25">
-      <c r="A66" s="8" t="s">
-        <v>272</v>
       </c>
       <c r="B66" s="7" t="s">
         <v>121</v>
@@ -2899,32 +2897,32 @@
         <v>120</v>
       </c>
       <c r="D66" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E66" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5">
       <c r="A67" s="8" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B67" s="7" t="s">
         <v>123</v>
       </c>
       <c r="C67" s="7" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D67" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E67" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5">
       <c r="A68" s="8" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B68" s="7" t="s">
         <v>124</v>
@@ -2933,15 +2931,15 @@
         <v>122</v>
       </c>
       <c r="D68" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E68" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5">
       <c r="A69" s="8" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B69" s="7" t="s">
         <v>125</v>
@@ -2950,15 +2948,15 @@
         <v>126</v>
       </c>
       <c r="D69" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E69" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="70" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" ht="30">
       <c r="A70" s="8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B70" s="7" t="s">
         <v>128</v>
@@ -2967,15 +2965,15 @@
         <v>127</v>
       </c>
       <c r="D70" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E70" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5">
       <c r="A71" s="8" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B71" s="7" t="s">
         <v>129</v>
@@ -2984,15 +2982,15 @@
         <v>130</v>
       </c>
       <c r="D71" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E71" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5">
       <c r="A72" s="8" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B72" s="7" t="s">
         <v>133</v>
@@ -3001,15 +2999,15 @@
         <v>132</v>
       </c>
       <c r="D72" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E72" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5">
       <c r="A73" s="8" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B73" s="7" t="s">
         <v>134</v>
@@ -3018,15 +3016,15 @@
         <v>135</v>
       </c>
       <c r="D73" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E73" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5">
       <c r="A74" s="8" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B74" s="7" t="s">
         <v>137</v>
@@ -3035,32 +3033,32 @@
         <v>136</v>
       </c>
       <c r="D74" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E74" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="75" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" ht="135">
       <c r="A75" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="B75" s="7" t="s">
+        <v>374</v>
+      </c>
+      <c r="C75" s="7" t="s">
+        <v>364</v>
+      </c>
+      <c r="D75" s="8" t="s">
+        <v>310</v>
+      </c>
+      <c r="E75" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="105">
+      <c r="A76" s="8" t="s">
         <v>281</v>
-      </c>
-      <c r="B75" s="7" t="s">
-        <v>375</v>
-      </c>
-      <c r="C75" s="7" t="s">
-        <v>365</v>
-      </c>
-      <c r="D75" s="8" t="s">
-        <v>311</v>
-      </c>
-      <c r="E75" s="8" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A76" s="8" t="s">
-        <v>282</v>
       </c>
       <c r="B76" s="7" t="s">
         <v>138</v>
@@ -3069,15 +3067,15 @@
         <v>139</v>
       </c>
       <c r="D76" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E76" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5">
       <c r="A77" s="8" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B77" s="7" t="s">
         <v>140</v>
@@ -3086,15 +3084,15 @@
         <v>141</v>
       </c>
       <c r="D77" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E77" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5">
       <c r="A78" s="8" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B78" s="7" t="s">
         <v>142</v>
@@ -3103,32 +3101,32 @@
         <v>143</v>
       </c>
       <c r="D78" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E78" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="79" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" ht="45">
       <c r="A79" s="8" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C79" s="7" t="s">
         <v>144</v>
       </c>
       <c r="D79" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E79" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5">
       <c r="A80" s="8" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B80" s="8" t="s">
         <v>145</v>
@@ -3137,15 +3135,15 @@
         <v>146</v>
       </c>
       <c r="D80" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E80" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5">
       <c r="A81" s="8" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B81" s="8" t="s">
         <v>147</v>
@@ -3154,32 +3152,32 @@
         <v>148</v>
       </c>
       <c r="D81" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E81" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5">
       <c r="A82" s="8" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B82" s="8" t="s">
         <v>149</v>
       </c>
       <c r="C82" s="8" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D82" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E82" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5">
       <c r="A83" s="8" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B83" s="8" t="s">
         <v>150</v>
@@ -3188,15 +3186,15 @@
         <v>151</v>
       </c>
       <c r="D83" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E83" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5">
       <c r="A84" s="8" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B84" s="8" t="s">
         <v>152</v>
@@ -3205,49 +3203,49 @@
         <v>153</v>
       </c>
       <c r="D84" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E84" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="85" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" ht="165">
       <c r="A85" s="8" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B85" s="8" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C85" s="7" t="s">
         <v>154</v>
       </c>
       <c r="D85" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E85" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="86" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" ht="75">
       <c r="A86" s="8" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B86" s="9" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C86" s="7" t="s">
         <v>171</v>
       </c>
       <c r="D86" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E86" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5">
       <c r="A87" s="8" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B87" s="7" t="s">
         <v>155</v>
@@ -3256,15 +3254,15 @@
         <v>156</v>
       </c>
       <c r="D87" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E87" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5">
       <c r="A88" s="8" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B88" s="7" t="s">
         <v>157</v>
@@ -3273,15 +3271,15 @@
         <v>158</v>
       </c>
       <c r="D88" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E88" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5">
       <c r="A89" s="8" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B89" s="8" t="s">
         <v>161</v>
@@ -3290,15 +3288,15 @@
         <v>162</v>
       </c>
       <c r="D89" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E89" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5">
       <c r="A90" s="8" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B90" s="8" t="s">
         <v>159</v>
@@ -3307,15 +3305,15 @@
         <v>160</v>
       </c>
       <c r="D90" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E90" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5">
       <c r="A91" s="8" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B91" s="8" t="s">
         <v>163</v>
@@ -3324,15 +3322,15 @@
         <v>164</v>
       </c>
       <c r="D91" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E91" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5">
       <c r="A92" s="8" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B92" s="8" t="s">
         <v>166</v>
@@ -3341,15 +3339,15 @@
         <v>165</v>
       </c>
       <c r="D92" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E92" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5">
       <c r="A93" s="8" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B93" s="8" t="s">
         <v>167</v>
@@ -3358,15 +3356,15 @@
         <v>168</v>
       </c>
       <c r="D93" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E93" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5">
       <c r="A94" s="8" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B94" s="8" t="s">
         <v>169</v>
@@ -3375,15 +3373,15 @@
         <v>170</v>
       </c>
       <c r="D94" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E94" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5">
       <c r="A95" s="8" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B95" s="9" t="s">
         <v>173</v>
@@ -3392,32 +3390,32 @@
         <v>172</v>
       </c>
       <c r="D95" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E95" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="96" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" ht="30">
       <c r="A96" s="8" t="s">
+        <v>301</v>
+      </c>
+      <c r="B96" s="9" t="s">
+        <v>378</v>
+      </c>
+      <c r="C96" s="10" t="s">
+        <v>312</v>
+      </c>
+      <c r="D96" s="8" t="s">
+        <v>310</v>
+      </c>
+      <c r="E96" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" ht="75">
+      <c r="A97" s="8" t="s">
         <v>302</v>
-      </c>
-      <c r="B96" s="9" t="s">
-        <v>379</v>
-      </c>
-      <c r="C96" s="10" t="s">
-        <v>313</v>
-      </c>
-      <c r="D96" s="8" t="s">
-        <v>311</v>
-      </c>
-      <c r="E96" s="8" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A97" s="8" t="s">
-        <v>303</v>
       </c>
       <c r="B97" s="8" t="s">
         <v>174</v>
@@ -3426,15 +3424,15 @@
         <v>175</v>
       </c>
       <c r="D97" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E97" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="98" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" ht="60">
       <c r="A98" s="8" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B98" s="7" t="s">
         <v>176</v>
@@ -3443,49 +3441,49 @@
         <v>177</v>
       </c>
       <c r="D98" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E98" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="99" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" ht="120">
       <c r="A99" s="8" t="s">
+        <v>304</v>
+      </c>
+      <c r="B99" s="7" t="s">
+        <v>379</v>
+      </c>
+      <c r="C99" s="7" t="s">
+        <v>367</v>
+      </c>
+      <c r="D99" s="8" t="s">
+        <v>310</v>
+      </c>
+      <c r="E99" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" ht="120">
+      <c r="A100" s="8" t="s">
+        <v>366</v>
+      </c>
+      <c r="B100" s="7" t="s">
+        <v>380</v>
+      </c>
+      <c r="C100" s="7" t="s">
+        <v>363</v>
+      </c>
+      <c r="D100" s="8" t="s">
+        <v>310</v>
+      </c>
+      <c r="E100" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5">
+      <c r="A101" s="8" t="s">
         <v>305</v>
-      </c>
-      <c r="B99" s="7" t="s">
-        <v>380</v>
-      </c>
-      <c r="C99" s="7" t="s">
-        <v>368</v>
-      </c>
-      <c r="D99" s="8" t="s">
-        <v>311</v>
-      </c>
-      <c r="E99" s="8" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" ht="120" x14ac:dyDescent="0.25">
-      <c r="A100" s="8" t="s">
-        <v>367</v>
-      </c>
-      <c r="B100" s="7" t="s">
-        <v>381</v>
-      </c>
-      <c r="C100" s="7" t="s">
-        <v>364</v>
-      </c>
-      <c r="D100" s="8" t="s">
-        <v>311</v>
-      </c>
-      <c r="E100" s="8" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A101" s="8" t="s">
-        <v>306</v>
       </c>
       <c r="B101" s="7" t="s">
         <v>178</v>
@@ -3494,15 +3492,15 @@
         <v>179</v>
       </c>
       <c r="D101" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E101" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5">
       <c r="A102" s="8" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B102" s="7" t="s">
         <v>180</v>
@@ -3511,15 +3509,15 @@
         <v>181</v>
       </c>
       <c r="D102" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E102" s="8" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5">
       <c r="A103" s="8" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B103" s="3" t="s">
         <v>182</v>
@@ -3528,13 +3526,13 @@
         <v>183</v>
       </c>
       <c r="D103" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E103" s="3"/>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5">
       <c r="A104" s="8" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B104" s="3" t="s">
         <v>184</v>
@@ -3543,13 +3541,13 @@
         <v>185</v>
       </c>
       <c r="D104" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E104" s="3"/>
     </row>
-    <row r="105" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" ht="150">
       <c r="A105" s="8" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B105" s="3" t="s">
         <v>186</v>
@@ -3558,67 +3556,67 @@
         <v>187</v>
       </c>
       <c r="D105" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E105" s="3"/>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5">
       <c r="A106" s="8" t="s">
+        <v>341</v>
+      </c>
+      <c r="B106" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="C106" s="11" t="s">
         <v>342</v>
       </c>
-      <c r="B106" s="3" t="s">
+      <c r="D106" s="8" t="s">
+        <v>310</v>
+      </c>
+      <c r="E106" s="3"/>
+    </row>
+    <row r="107" spans="1:5">
+      <c r="A107" s="8" t="s">
+        <v>361</v>
+      </c>
+      <c r="B107" s="3" t="s">
         <v>382</v>
       </c>
-      <c r="C106" s="11" t="s">
-        <v>343</v>
-      </c>
-      <c r="D106" s="8" t="s">
-        <v>311</v>
-      </c>
-      <c r="E106" s="3"/>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A107" s="8" t="s">
+      <c r="C107" s="11" t="s">
         <v>362</v>
       </c>
-      <c r="B107" s="3" t="s">
+      <c r="D107" s="8" t="s">
+        <v>310</v>
+      </c>
+      <c r="E107" s="3"/>
+    </row>
+    <row r="108" spans="1:5">
+      <c r="A108" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="B108" s="12" t="s">
         <v>383</v>
       </c>
-      <c r="C107" s="11" t="s">
-        <v>363</v>
-      </c>
-      <c r="D107" s="8" t="s">
-        <v>311</v>
-      </c>
-      <c r="E107" s="3"/>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A108" s="8" t="s">
+      <c r="C108" s="11" t="s">
         <v>370</v>
       </c>
-      <c r="B108" s="12" t="s">
-        <v>384</v>
-      </c>
-      <c r="C108" s="11" t="s">
+      <c r="D108" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="E108" s="3"/>
+    </row>
+    <row r="109" spans="1:5">
+      <c r="A109" s="8" t="s">
         <v>371</v>
       </c>
-      <c r="D108" s="3" t="s">
-        <v>311</v>
-      </c>
-      <c r="E108" s="3"/>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A109" s="8" t="s">
+      <c r="B109" s="12" t="s">
+        <v>383</v>
+      </c>
+      <c r="C109" s="11" t="s">
         <v>372</v>
       </c>
-      <c r="B109" s="12" t="s">
-        <v>384</v>
-      </c>
-      <c r="C109" s="11" t="s">
-        <v>373</v>
-      </c>
       <c r="D109" s="3" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E109" s="3"/>
     </row>
@@ -3633,230 +3631,230 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="89.28515625" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
+        <v>329</v>
+      </c>
+      <c r="B1" t="s">
         <v>330</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>331</v>
-      </c>
-      <c r="C1" t="s">
-        <v>332</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
+        <v>343</v>
+      </c>
+      <c r="B2" t="s">
+        <v>332</v>
+      </c>
+      <c r="C2" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
         <v>344</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>333</v>
       </c>
-      <c r="C2" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="C3" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
         <v>345</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>334</v>
       </c>
-      <c r="C3" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="C4" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
         <v>346</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>335</v>
       </c>
-      <c r="C4" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="C5" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
         <v>347</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>336</v>
       </c>
-      <c r="C5" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="C6" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
         <v>348</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
+        <v>332</v>
+      </c>
+      <c r="C7" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>349</v>
+      </c>
+      <c r="B8" t="s">
+        <v>332</v>
+      </c>
+      <c r="C8" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>350</v>
+      </c>
+      <c r="B9" t="s">
+        <v>332</v>
+      </c>
+      <c r="C9" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>351</v>
+      </c>
+      <c r="B10" t="s">
         <v>337</v>
       </c>
-      <c r="C6" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>349</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="C10" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>352</v>
+      </c>
+      <c r="B11" t="s">
         <v>333</v>
       </c>
-      <c r="C7" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>350</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="C11" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>353</v>
+      </c>
+      <c r="B12" t="s">
         <v>333</v>
       </c>
-      <c r="C8" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>351</v>
-      </c>
-      <c r="B9" t="s">
-        <v>333</v>
-      </c>
-      <c r="C9" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>352</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="C12" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>354</v>
+      </c>
+      <c r="B13" t="s">
         <v>338</v>
       </c>
-      <c r="C10" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>353</v>
-      </c>
-      <c r="B11" t="s">
-        <v>334</v>
-      </c>
-      <c r="C11" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>354</v>
-      </c>
-      <c r="B12" t="s">
-        <v>334</v>
-      </c>
-      <c r="C12" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="C13" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
         <v>355</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>339</v>
       </c>
-      <c r="C13" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="C14" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
         <v>356</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
+        <v>339</v>
+      </c>
+      <c r="C15" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>357</v>
+      </c>
+      <c r="B16" t="s">
+        <v>335</v>
+      </c>
+      <c r="C16" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>358</v>
+      </c>
+      <c r="B17" t="s">
         <v>340</v>
       </c>
-      <c r="C14" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>357</v>
-      </c>
-      <c r="B15" t="s">
+      <c r="C17" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>359</v>
+      </c>
+      <c r="B18" t="s">
         <v>340</v>
       </c>
-      <c r="C15" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>358</v>
-      </c>
-      <c r="B16" t="s">
-        <v>336</v>
-      </c>
-      <c r="C16" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>359</v>
-      </c>
-      <c r="B17" t="s">
-        <v>341</v>
-      </c>
-      <c r="C17" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="C18" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
         <v>360</v>
       </c>
-      <c r="B18" t="s">
-        <v>341</v>
-      </c>
-      <c r="C18" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>361</v>
-      </c>
       <c r="B19" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C19" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
   </sheetData>
@@ -3866,14 +3864,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12" style="5" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="52.5703125" style="5" customWidth="1" collapsed="1"/>
@@ -3881,7 +3879,7 @@
     <col min="4" max="16384" width="9.140625" style="5" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="35.25" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3892,7 +3890,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="206.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="206.25" customHeight="1">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -3903,7 +3901,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="203.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="203.25" customHeight="1">
       <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
@@ -3914,7 +3912,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="295.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="295.5" customHeight="1">
       <c r="A4" s="4" t="s">
         <v>12</v>
       </c>
@@ -3925,7 +3923,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="147" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="147" customHeight="1">
       <c r="A5" s="6" t="s">
         <v>14</v>
       </c>
@@ -3936,7 +3934,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="73.5" customHeight="1">
       <c r="A6" s="6" t="s">
         <v>18</v>
       </c>
@@ -3947,7 +3945,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="60">
       <c r="A7" s="4" t="s">
         <v>22</v>
       </c>
@@ -3958,7 +3956,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="165.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="165.75" customHeight="1">
       <c r="A8" s="4" t="s">
         <v>24</v>
       </c>
@@ -3969,7 +3967,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="69.75" customHeight="1">
       <c r="A9" s="4" t="s">
         <v>27</v>
       </c>

</xml_diff>

<commit_message>
Added new testcase to search module
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Search.xlsx
+++ b/src/test/resources/xls/Search.xlsx
@@ -506,12 +506,6 @@
     <t>OPQA-1237</t>
   </si>
   <si>
-    <t>OPQA-1238</t>
-  </si>
-  <si>
-    <t>Verify that profile page of a person gets displayed when clicks on any PEOPLE search result in ALL search results page</t>
-  </si>
-  <si>
     <t>Verify that record view page of a person gets displayed when user clicks on any PEOPLE in PEOPLE search results page.</t>
   </si>
   <si>
@@ -1342,7 +1336,13 @@
     <t>Verify that search left navigationpane  content type is retained when user navigates back to PATENTS search results page from record view page</t>
   </si>
   <si>
-    <t>OPQA-1436||OPQA-1408</t>
+    <t>OPQA-1436||OPQA-1408||OPQA-1406</t>
+  </si>
+  <si>
+    <t>OPQA-3918||OPQA-3919||OPQA-1238</t>
+  </si>
+  <si>
+    <t>Verify that profile page of a person gets displayed when clicks on any PEOPLE page and verify that comments and posts are labels are displaying for people in people result page</t>
   </si>
 </sst>
 </file>
@@ -1768,8 +1768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="C73" sqref="C73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1800,7 +1800,7 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="8" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
@@ -1809,7 +1809,7 @@
         <v>70</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>88</v>
@@ -1817,7 +1817,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="8" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>32</v>
@@ -1826,7 +1826,7 @@
         <v>52</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>88</v>
@@ -1834,7 +1834,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="8" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>33</v>
@@ -1843,7 +1843,7 @@
         <v>53</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>88</v>
@@ -1851,7 +1851,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="8" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>34</v>
@@ -1860,7 +1860,7 @@
         <v>54</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E5" s="8" t="s">
         <v>88</v>
@@ -1868,7 +1868,7 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="8" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>35</v>
@@ -1877,7 +1877,7 @@
         <v>55</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>88</v>
@@ -1885,7 +1885,7 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="8" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>36</v>
@@ -1894,7 +1894,7 @@
         <v>56</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E7" s="8" t="s">
         <v>88</v>
@@ -1902,16 +1902,16 @@
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1">
       <c r="A8" s="8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>57</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E8" s="8" t="s">
         <v>88</v>
@@ -1919,7 +1919,7 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="8" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>47</v>
@@ -1928,7 +1928,7 @@
         <v>58</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E9" s="8" t="s">
         <v>88</v>
@@ -1936,7 +1936,7 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="8" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>37</v>
@@ -1945,7 +1945,7 @@
         <v>59</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E10" s="8" t="s">
         <v>88</v>
@@ -1953,7 +1953,7 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="8" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>38</v>
@@ -1962,7 +1962,7 @@
         <v>60</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E11" s="8" t="s">
         <v>88</v>
@@ -1970,7 +1970,7 @@
     </row>
     <row r="12" spans="1:5" ht="16.5" customHeight="1">
       <c r="A12" s="8" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>46</v>
@@ -1979,7 +1979,7 @@
         <v>61</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E12" s="8" t="s">
         <v>88</v>
@@ -1987,16 +1987,16 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="8" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>62</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E13" s="8" t="s">
         <v>88</v>
@@ -2004,7 +2004,7 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="8" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>51</v>
@@ -2013,7 +2013,7 @@
         <v>83</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E14" s="8" t="s">
         <v>88</v>
@@ -2021,7 +2021,7 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="8" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>45</v>
@@ -2030,7 +2030,7 @@
         <v>63</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E15" s="8" t="s">
         <v>88</v>
@@ -2038,7 +2038,7 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="8" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>44</v>
@@ -2047,7 +2047,7 @@
         <v>64</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E16" s="8" t="s">
         <v>88</v>
@@ -2055,7 +2055,7 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="8" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>43</v>
@@ -2064,7 +2064,7 @@
         <v>65</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E17" s="8" t="s">
         <v>88</v>
@@ -2072,7 +2072,7 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="8" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>39</v>
@@ -2081,7 +2081,7 @@
         <v>66</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E18" s="8" t="s">
         <v>88</v>
@@ -2089,7 +2089,7 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="8" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>40</v>
@@ -2098,7 +2098,7 @@
         <v>67</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E19" s="8" t="s">
         <v>88</v>
@@ -2106,7 +2106,7 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="8" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>41</v>
@@ -2115,7 +2115,7 @@
         <v>68</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E20" s="8" t="s">
         <v>88</v>
@@ -2123,7 +2123,7 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="8" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B21" s="7" t="s">
         <v>42</v>
@@ -2132,7 +2132,7 @@
         <v>69</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E21" s="8" t="s">
         <v>88</v>
@@ -2140,16 +2140,16 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="8" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C22" s="8" t="s">
         <v>71</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E22" s="8" t="s">
         <v>88</v>
@@ -2157,33 +2157,33 @@
     </row>
     <row r="23" spans="1:5" ht="75">
       <c r="A23" s="8" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>72</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E23" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" ht="30">
       <c r="A24" s="8" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C24" s="8" t="s">
         <v>73</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E24" s="8" t="s">
         <v>88</v>
@@ -2191,16 +2191,16 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="8" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C25" s="8" t="s">
         <v>74</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E25" s="8" t="s">
         <v>88</v>
@@ -2208,16 +2208,16 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="8" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>75</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E26" s="8" t="s">
         <v>88</v>
@@ -2225,16 +2225,16 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="8" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C27" s="8" t="s">
         <v>76</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E27" s="8" t="s">
         <v>88</v>
@@ -2242,16 +2242,16 @@
     </row>
     <row r="28" spans="1:5" ht="90">
       <c r="A28" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C28" s="7" t="s">
         <v>77</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E28" s="8" t="s">
         <v>88</v>
@@ -2259,16 +2259,16 @@
     </row>
     <row r="29" spans="1:5" ht="60">
       <c r="A29" s="8" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C29" s="7" t="s">
         <v>78</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E29" s="8" t="s">
         <v>88</v>
@@ -2276,16 +2276,16 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="8" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C30" s="7" t="s">
         <v>79</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E30" s="8" t="s">
         <v>88</v>
@@ -2293,16 +2293,16 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="8" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C31" s="7" t="s">
         <v>80</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E31" s="8" t="s">
         <v>88</v>
@@ -2310,16 +2310,16 @@
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="8" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C32" s="8" t="s">
         <v>81</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E32" s="8" t="s">
         <v>88</v>
@@ -2327,16 +2327,16 @@
     </row>
     <row r="33" spans="1:5" ht="90">
       <c r="A33" s="8" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C33" s="7" t="s">
         <v>82</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E33" s="8" t="s">
         <v>88</v>
@@ -2344,16 +2344,16 @@
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C34" s="8" t="s">
         <v>83</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E34" s="8" t="s">
         <v>88</v>
@@ -2361,16 +2361,16 @@
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="8" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C35" s="8" t="s">
         <v>84</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E35" s="8" t="s">
         <v>88</v>
@@ -2378,16 +2378,16 @@
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="8" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C36" s="8" t="s">
         <v>85</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E36" s="8" t="s">
         <v>88</v>
@@ -2395,16 +2395,16 @@
     </row>
     <row r="37" spans="1:5" ht="90">
       <c r="A37" s="8" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C37" s="7" t="s">
         <v>86</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E37" s="8" t="s">
         <v>88</v>
@@ -2412,16 +2412,16 @@
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="8" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C38" s="7" t="s">
         <v>87</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E38" s="8" t="s">
         <v>88</v>
@@ -2429,16 +2429,16 @@
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="8" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C39" s="7" t="s">
         <v>89</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E39" s="8" t="s">
         <v>88</v>
@@ -2446,16 +2446,16 @@
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="8" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C40" s="7" t="s">
         <v>90</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E40" s="8" t="s">
         <v>88</v>
@@ -2463,16 +2463,16 @@
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="8" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C41" s="7" t="s">
         <v>91</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E41" s="8" t="s">
         <v>88</v>
@@ -2480,16 +2480,16 @@
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="8" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B42" s="7" t="s">
         <v>92</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E42" s="8" t="s">
         <v>88</v>
@@ -2497,16 +2497,16 @@
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="8" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B43" s="7" t="s">
         <v>93</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E43" s="8" t="s">
         <v>88</v>
@@ -2514,16 +2514,16 @@
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="8" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E44" s="8" t="s">
         <v>88</v>
@@ -2531,16 +2531,16 @@
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="8" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B45" s="7" t="s">
         <v>48</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E45" s="8" t="s">
         <v>88</v>
@@ -2548,16 +2548,16 @@
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="8" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B46" s="7" t="s">
         <v>94</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E46" s="8" t="s">
         <v>88</v>
@@ -2565,16 +2565,16 @@
     </row>
     <row r="47" spans="1:5" ht="120">
       <c r="A47" s="8" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B47" s="7" t="s">
         <v>95</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E47" s="8" t="s">
         <v>88</v>
@@ -2582,7 +2582,7 @@
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="8" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B48" s="7" t="s">
         <v>50</v>
@@ -2591,7 +2591,7 @@
         <v>49</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E48" s="8" t="s">
         <v>88</v>
@@ -2599,7 +2599,7 @@
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="8" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B49" s="7" t="s">
         <v>97</v>
@@ -2608,7 +2608,7 @@
         <v>96</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E49" s="8" t="s">
         <v>88</v>
@@ -2616,7 +2616,7 @@
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="8" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B50" s="7" t="s">
         <v>98</v>
@@ -2625,7 +2625,7 @@
         <v>99</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E50" s="8" t="s">
         <v>88</v>
@@ -2633,7 +2633,7 @@
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="8" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B51" s="7" t="s">
         <v>101</v>
@@ -2642,7 +2642,7 @@
         <v>100</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E51" s="8" t="s">
         <v>88</v>
@@ -2650,16 +2650,16 @@
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="8" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C52" s="7" t="s">
         <v>102</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E52" s="8" t="s">
         <v>88</v>
@@ -2667,16 +2667,16 @@
     </row>
     <row r="53" spans="1:5" ht="30">
       <c r="A53" s="8" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B53" s="7" t="s">
         <v>103</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E53" s="8" t="s">
         <v>88</v>
@@ -2684,16 +2684,16 @@
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="8" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B54" s="7" t="s">
         <v>104</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E54" s="8" t="s">
         <v>88</v>
@@ -2701,16 +2701,16 @@
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="8" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B55" s="7" t="s">
         <v>105</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E55" s="8" t="s">
         <v>88</v>
@@ -2718,16 +2718,16 @@
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="8" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B56" s="7" t="s">
         <v>106</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E56" s="8" t="s">
         <v>88</v>
@@ -2735,16 +2735,16 @@
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="8" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B57" s="7" t="s">
         <v>107</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E57" s="8" t="s">
         <v>88</v>
@@ -2752,7 +2752,7 @@
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="8" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B58" s="7" t="s">
         <v>108</v>
@@ -2761,7 +2761,7 @@
         <v>109</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E58" s="8" t="s">
         <v>88</v>
@@ -2769,16 +2769,16 @@
     </row>
     <row r="59" spans="1:5" ht="90">
       <c r="A59" s="8" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B59" s="7" t="s">
         <v>110</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E59" s="8" t="s">
         <v>88</v>
@@ -2786,16 +2786,16 @@
     </row>
     <row r="60" spans="1:5" ht="75">
       <c r="A60" s="8" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B60" s="7" t="s">
         <v>111</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E60" s="8" t="s">
         <v>88</v>
@@ -2803,7 +2803,7 @@
     </row>
     <row r="61" spans="1:5">
       <c r="A61" s="8" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B61" s="7" t="s">
         <v>112</v>
@@ -2812,7 +2812,7 @@
         <v>113</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E61" s="8" t="s">
         <v>88</v>
@@ -2820,7 +2820,7 @@
     </row>
     <row r="62" spans="1:5">
       <c r="A62" s="8" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B62" s="7" t="s">
         <v>114</v>
@@ -2829,7 +2829,7 @@
         <v>115</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E62" s="8" t="s">
         <v>88</v>
@@ -2837,7 +2837,7 @@
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="8" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B63" s="7" t="s">
         <v>117</v>
@@ -2846,7 +2846,7 @@
         <v>116</v>
       </c>
       <c r="D63" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E63" s="8" t="s">
         <v>88</v>
@@ -2854,7 +2854,7 @@
     </row>
     <row r="64" spans="1:5" ht="120">
       <c r="A64" s="8" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B64" s="7" t="s">
         <v>119</v>
@@ -2863,7 +2863,7 @@
         <v>118</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E64" s="8" t="s">
         <v>88</v>
@@ -2871,16 +2871,16 @@
     </row>
     <row r="65" spans="1:5" ht="135">
       <c r="A65" s="8" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C65" s="7" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="D65" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E65" s="8" t="s">
         <v>88</v>
@@ -2888,7 +2888,7 @@
     </row>
     <row r="66" spans="1:5" ht="195">
       <c r="A66" s="8" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B66" s="7" t="s">
         <v>121</v>
@@ -2897,7 +2897,7 @@
         <v>120</v>
       </c>
       <c r="D66" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E66" s="8" t="s">
         <v>88</v>
@@ -2905,16 +2905,16 @@
     </row>
     <row r="67" spans="1:5">
       <c r="A67" s="8" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B67" s="7" t="s">
         <v>123</v>
       </c>
       <c r="C67" s="7" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="D67" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E67" s="8" t="s">
         <v>88</v>
@@ -2922,7 +2922,7 @@
     </row>
     <row r="68" spans="1:5">
       <c r="A68" s="8" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B68" s="7" t="s">
         <v>124</v>
@@ -2931,7 +2931,7 @@
         <v>122</v>
       </c>
       <c r="D68" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E68" s="8" t="s">
         <v>88</v>
@@ -2939,7 +2939,7 @@
     </row>
     <row r="69" spans="1:5">
       <c r="A69" s="8" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B69" s="7" t="s">
         <v>125</v>
@@ -2948,7 +2948,7 @@
         <v>126</v>
       </c>
       <c r="D69" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E69" s="8" t="s">
         <v>88</v>
@@ -2956,7 +2956,7 @@
     </row>
     <row r="70" spans="1:5" ht="30">
       <c r="A70" s="8" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B70" s="7" t="s">
         <v>128</v>
@@ -2965,7 +2965,7 @@
         <v>127</v>
       </c>
       <c r="D70" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E70" s="8" t="s">
         <v>88</v>
@@ -2973,7 +2973,7 @@
     </row>
     <row r="71" spans="1:5">
       <c r="A71" s="8" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B71" s="7" t="s">
         <v>129</v>
@@ -2982,7 +2982,7 @@
         <v>130</v>
       </c>
       <c r="D71" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E71" s="8" t="s">
         <v>88</v>
@@ -2990,7 +2990,7 @@
     </row>
     <row r="72" spans="1:5">
       <c r="A72" s="8" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B72" s="7" t="s">
         <v>133</v>
@@ -2999,24 +2999,24 @@
         <v>132</v>
       </c>
       <c r="D72" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E72" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="73" spans="1:5">
+    <row r="73" spans="1:5" ht="30">
       <c r="A73" s="8" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>134</v>
+        <v>384</v>
       </c>
       <c r="C73" s="8" t="s">
-        <v>135</v>
+        <v>385</v>
       </c>
       <c r="D73" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E73" s="8" t="s">
         <v>88</v>
@@ -3024,16 +3024,16 @@
     </row>
     <row r="74" spans="1:5">
       <c r="A74" s="8" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C74" s="8" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D74" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E74" s="8" t="s">
         <v>88</v>
@@ -3041,16 +3041,16 @@
     </row>
     <row r="75" spans="1:5" ht="135">
       <c r="A75" s="8" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C75" s="7" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="D75" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E75" s="8" t="s">
         <v>88</v>
@@ -3058,16 +3058,16 @@
     </row>
     <row r="76" spans="1:5" ht="105">
       <c r="A76" s="8" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C76" s="7" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D76" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E76" s="8" t="s">
         <v>88</v>
@@ -3075,16 +3075,16 @@
     </row>
     <row r="77" spans="1:5">
       <c r="A77" s="8" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C77" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D77" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E77" s="8" t="s">
         <v>88</v>
@@ -3092,16 +3092,16 @@
     </row>
     <row r="78" spans="1:5">
       <c r="A78" s="8" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C78" s="7" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D78" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E78" s="8" t="s">
         <v>88</v>
@@ -3109,16 +3109,16 @@
     </row>
     <row r="79" spans="1:5" ht="45">
       <c r="A79" s="8" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C79" s="7" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D79" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E79" s="8" t="s">
         <v>88</v>
@@ -3126,16 +3126,16 @@
     </row>
     <row r="80" spans="1:5">
       <c r="A80" s="8" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B80" s="8" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C80" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D80" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E80" s="8" t="s">
         <v>88</v>
@@ -3143,16 +3143,16 @@
     </row>
     <row r="81" spans="1:5">
       <c r="A81" s="8" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C81" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D81" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E81" s="8" t="s">
         <v>88</v>
@@ -3160,16 +3160,16 @@
     </row>
     <row r="82" spans="1:5">
       <c r="A82" s="8" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B82" s="8" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C82" s="8" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="D82" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E82" s="8" t="s">
         <v>88</v>
@@ -3177,16 +3177,16 @@
     </row>
     <row r="83" spans="1:5">
       <c r="A83" s="8" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B83" s="8" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C83" s="8" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D83" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E83" s="8" t="s">
         <v>88</v>
@@ -3194,16 +3194,16 @@
     </row>
     <row r="84" spans="1:5">
       <c r="A84" s="8" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B84" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C84" s="8" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D84" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E84" s="8" t="s">
         <v>88</v>
@@ -3211,16 +3211,16 @@
     </row>
     <row r="85" spans="1:5" ht="165">
       <c r="A85" s="8" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B85" s="8" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C85" s="7" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D85" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E85" s="8" t="s">
         <v>88</v>
@@ -3228,16 +3228,16 @@
     </row>
     <row r="86" spans="1:5" ht="75">
       <c r="A86" s="8" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B86" s="9" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C86" s="7" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D86" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E86" s="8" t="s">
         <v>88</v>
@@ -3245,16 +3245,16 @@
     </row>
     <row r="87" spans="1:5">
       <c r="A87" s="8" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B87" s="7" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C87" s="7" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D87" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E87" s="8" t="s">
         <v>88</v>
@@ -3262,16 +3262,16 @@
     </row>
     <row r="88" spans="1:5">
       <c r="A88" s="8" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B88" s="7" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C88" s="7" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D88" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E88" s="8" t="s">
         <v>88</v>
@@ -3279,16 +3279,16 @@
     </row>
     <row r="89" spans="1:5">
       <c r="A89" s="8" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B89" s="8" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C89" s="8" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D89" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E89" s="8" t="s">
         <v>88</v>
@@ -3296,16 +3296,16 @@
     </row>
     <row r="90" spans="1:5">
       <c r="A90" s="8" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B90" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C90" s="8" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D90" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E90" s="8" t="s">
         <v>88</v>
@@ -3313,16 +3313,16 @@
     </row>
     <row r="91" spans="1:5">
       <c r="A91" s="8" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B91" s="8" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C91" s="8" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D91" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E91" s="8" t="s">
         <v>88</v>
@@ -3330,16 +3330,16 @@
     </row>
     <row r="92" spans="1:5">
       <c r="A92" s="8" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B92" s="8" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C92" s="8" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D92" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E92" s="8" t="s">
         <v>88</v>
@@ -3347,16 +3347,16 @@
     </row>
     <row r="93" spans="1:5">
       <c r="A93" s="8" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B93" s="8" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C93" s="8" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D93" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E93" s="8" t="s">
         <v>88</v>
@@ -3364,16 +3364,16 @@
     </row>
     <row r="94" spans="1:5">
       <c r="A94" s="8" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B94" s="8" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C94" s="8" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D94" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E94" s="8" t="s">
         <v>88</v>
@@ -3381,16 +3381,16 @@
     </row>
     <row r="95" spans="1:5">
       <c r="A95" s="8" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B95" s="9" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C95" s="9" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D95" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E95" s="8" t="s">
         <v>88</v>
@@ -3398,16 +3398,16 @@
     </row>
     <row r="96" spans="1:5" ht="30">
       <c r="A96" s="8" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B96" s="9" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C96" s="10" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D96" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E96" s="8" t="s">
         <v>88</v>
@@ -3415,16 +3415,16 @@
     </row>
     <row r="97" spans="1:5" ht="75">
       <c r="A97" s="8" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B97" s="8" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C97" s="7" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D97" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E97" s="8" t="s">
         <v>88</v>
@@ -3432,16 +3432,16 @@
     </row>
     <row r="98" spans="1:5" ht="60">
       <c r="A98" s="8" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B98" s="7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C98" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D98" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E98" s="8" t="s">
         <v>88</v>
@@ -3449,16 +3449,16 @@
     </row>
     <row r="99" spans="1:5" ht="120">
       <c r="A99" s="8" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B99" s="7" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C99" s="7" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="D99" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E99" s="8" t="s">
         <v>88</v>
@@ -3466,16 +3466,16 @@
     </row>
     <row r="100" spans="1:5" ht="120">
       <c r="A100" s="8" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B100" s="7" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C100" s="7" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="D100" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E100" s="8" t="s">
         <v>88</v>
@@ -3483,16 +3483,16 @@
     </row>
     <row r="101" spans="1:5">
       <c r="A101" s="8" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B101" s="7" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C101" s="8" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D101" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E101" s="8" t="s">
         <v>88</v>
@@ -3500,16 +3500,16 @@
     </row>
     <row r="102" spans="1:5">
       <c r="A102" s="8" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B102" s="7" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D102" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E102" s="8" t="s">
         <v>131</v>
@@ -3517,106 +3517,106 @@
     </row>
     <row r="103" spans="1:5">
       <c r="A103" s="8" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D103" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E103" s="3"/>
     </row>
     <row r="104" spans="1:5">
       <c r="A104" s="8" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D104" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E104" s="3"/>
     </row>
     <row r="105" spans="1:5" ht="150">
       <c r="A105" s="8" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D105" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E105" s="3"/>
     </row>
     <row r="106" spans="1:5">
       <c r="A106" s="8" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C106" s="11" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="D106" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E106" s="3"/>
     </row>
     <row r="107" spans="1:5">
       <c r="A107" s="8" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C107" s="11" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D107" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E107" s="3"/>
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="8" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="B108" s="12" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C108" s="11" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E108" s="3"/>
     </row>
     <row r="109" spans="1:5">
       <c r="A109" s="8" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="B109" s="12" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C109" s="11" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E109" s="3"/>
     </row>
@@ -3647,13 +3647,13 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
+        <v>327</v>
+      </c>
+      <c r="B1" t="s">
+        <v>328</v>
+      </c>
+      <c r="C1" t="s">
         <v>329</v>
-      </c>
-      <c r="B1" t="s">
-        <v>330</v>
-      </c>
-      <c r="C1" t="s">
-        <v>331</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
@@ -3661,200 +3661,200 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B2" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C2" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B3" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C3" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B4" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C4" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B5" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C5" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B6" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C6" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B7" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C7" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B8" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B9" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C9" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B10" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C10" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B11" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C11" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B12" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C12" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B13" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C13" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B14" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C14" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B15" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C15" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B16" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C16" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B17" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C17" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B18" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C18" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B19" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C19" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new test case to search module
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Search.xlsx
+++ b/src/test/resources/xls/Search.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="389">
   <si>
     <t>TCID</t>
   </si>
@@ -1343,6 +1343,18 @@
   </si>
   <si>
     <t>Verify that profile page of a person gets displayed when clicks on any PEOPLE page and verify that comments and posts are labels are displaying for people in people result page</t>
+  </si>
+  <si>
+    <t>Search131</t>
+  </si>
+  <si>
+    <t>OPQA-1234||OPQA-1235||OPQA-1236</t>
+  </si>
+  <si>
+    <t>Verify that following sections are working correctly in post search result page
+1)INSTITUTIONS filter is present in POSTS search results page 
+2) More and Less Buttons for filters are working as expected in posts search result page
+3) Reset Button is working in posts search result page</t>
   </si>
 </sst>
 </file>
@@ -1766,10 +1778,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E109"/>
+  <dimension ref="A1:E110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="C73" sqref="C73"/>
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="B110" sqref="B110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3619,6 +3631,21 @@
         <v>308</v>
       </c>
       <c r="E109" s="3"/>
+    </row>
+    <row r="110" spans="1:5" ht="60">
+      <c r="A110" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="B110" s="11" t="s">
+        <v>387</v>
+      </c>
+      <c r="C110" s="4" t="s">
+        <v>388</v>
+      </c>
+      <c r="D110" s="8" t="s">
+        <v>308</v>
+      </c>
+      <c r="E110" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Added new test script for search module
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Search.xlsx
+++ b/src/test/resources/xls/Search.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="389">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="392">
   <si>
     <t>TCID</t>
   </si>
@@ -1355,6 +1355,18 @@
 1)INSTITUTIONS filter is present in POSTS search results page 
 2) More and Less Buttons for filters are working as expected in posts search result page
 3) Reset Button is working in posts search result page</t>
+  </si>
+  <si>
+    <t>Search132</t>
+  </si>
+  <si>
+    <t>Verify that following sections are working correctly in people search result page
+1)Filters are present in People search results page 
+2) More and Less Buttons for filters are working as expected in People search result page
+3) Reset Button is working in People search result page</t>
+  </si>
+  <si>
+    <t>OPQA-1249||OPQA-1250||OPQA-1251</t>
   </si>
 </sst>
 </file>
@@ -1778,10 +1790,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E110"/>
+  <dimension ref="A1:E111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="B110" sqref="B110"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="B113" sqref="B113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3646,6 +3658,21 @@
         <v>308</v>
       </c>
       <c r="E110" s="3"/>
+    </row>
+    <row r="111" spans="1:5" ht="60">
+      <c r="A111" s="8" t="s">
+        <v>389</v>
+      </c>
+      <c r="B111" s="11" t="s">
+        <v>391</v>
+      </c>
+      <c r="C111" s="4" t="s">
+        <v>390</v>
+      </c>
+      <c r="D111" s="8" t="s">
+        <v>308</v>
+      </c>
+      <c r="E111" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Modified url for deeplinking urls in search.xls
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Search.xlsx
+++ b/src/test/resources/xls/Search.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="14715" windowHeight="8040"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="14715" windowHeight="8040" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -1180,60 +1180,6 @@
     <t>Verify that Deep linking is working for Search result page using steam account</t>
   </si>
   <si>
-    <t>/#/search?query=science&amp;offsetIndex=0&amp;searchType=ALL</t>
-  </si>
-  <si>
-    <t>/#/search?query=science&amp;offsetIndex=0&amp;sortType=_score:desc&amp;searchType=ARTICLES</t>
-  </si>
-  <si>
-    <t>/#/search?query=science&amp;offsetIndex=0&amp;sortType=_score:desc&amp;searchType=PATENTS</t>
-  </si>
-  <si>
-    <t>/#/search?query=science&amp;offsetIndex=0&amp;sortType=_score:desc&amp;searchType=PEOPLE</t>
-  </si>
-  <si>
-    <t>/#/search?query=science&amp;offsetIndex=0&amp;sortType=sortdate:desc&amp;searchType=POSTS</t>
-  </si>
-  <si>
-    <t>/#/search?query=biology&amp;offsetIndex=0&amp;sortType=citingsrcslocalcount:desc&amp;searchType=ALL</t>
-  </si>
-  <si>
-    <t>/#/search?query=biology&amp;offsetIndex=0&amp;sortType=sortdate:desc&amp;searchType=ALL</t>
-  </si>
-  <si>
-    <t>/#/search?query=biology&amp;offsetIndex=0&amp;sortType=sortdate:asc&amp;searchType=ALL</t>
-  </si>
-  <si>
-    <t>/#/search?query=biology&amp;offsetIndex=0&amp;sortType=citingsrcslocalcount:desc&amp;searchType=ARTICLES</t>
-  </si>
-  <si>
-    <t>/#/search?query=biology&amp;offsetIndex=0&amp;sortType=sortdate:desc&amp;searchType=ARTICLES</t>
-  </si>
-  <si>
-    <t>/#/search?query=biology&amp;offsetIndex=0&amp;sortType=sortdate:asc&amp;searchType=ARTICLES</t>
-  </si>
-  <si>
-    <t>/#/search?query=biology&amp;offsetIndex=0&amp;sortType=citingsrcscount:desc&amp;searchType=PATENTS</t>
-  </si>
-  <si>
-    <t>/#/search?query=biology&amp;offsetIndex=0&amp;sortType=sortdate:desc&amp;searchType=PATENTS</t>
-  </si>
-  <si>
-    <t>/#/search?query=biology&amp;offsetIndex=0&amp;sortType=sortdate:asc&amp;searchType=PATENTS</t>
-  </si>
-  <si>
-    <t>/#/search?query=biology&amp;offsetIndex=0&amp;sortType=loadtime:desc&amp;searchType=PEOPLE</t>
-  </si>
-  <si>
-    <t>/#/search?query=post&amp;offsetIndex=0&amp;sortType=sortdate:desc&amp;searchType=POSTS</t>
-  </si>
-  <si>
-    <t>/#/search?query=biology&amp;offsetIndex=0&amp;sortType=sortdate:asc&amp;searchType=POSTS</t>
-  </si>
-  <si>
-    <t>/#/search?query=biology&amp;offsetIndex=0&amp;sortType=_score:desc&amp;searchType=POSTS</t>
-  </si>
-  <si>
     <t>Search128</t>
   </si>
   <si>
@@ -1367,6 +1313,60 @@
   </si>
   <si>
     <t>OPQA-1249||OPQA-1250||OPQA-1251</t>
+  </si>
+  <si>
+    <t>/cmty/#/search?query=science&amp;offsetIndex=0&amp;searchType=ALL</t>
+  </si>
+  <si>
+    <t>/cmty/#/search?query=science&amp;offsetIndex=0&amp;sortType=_score:desc&amp;searchType=ARTICLES</t>
+  </si>
+  <si>
+    <t>/cmty/#/search?query=science&amp;offsetIndex=0&amp;sortType=_score:desc&amp;searchType=PATENTS</t>
+  </si>
+  <si>
+    <t>/cmty/#/search?query=science&amp;offsetIndex=0&amp;sortType=_score:desc&amp;searchType=PEOPLE</t>
+  </si>
+  <si>
+    <t>/cmty/#/search?query=science&amp;offsetIndex=0&amp;sortType=sortdate:desc&amp;searchType=POSTS</t>
+  </si>
+  <si>
+    <t>/cmty/#/search?query=biology&amp;offsetIndex=0&amp;sortType=citingsrcslocalcount:desc&amp;searchType=ALL</t>
+  </si>
+  <si>
+    <t>/cmty/#/search?query=biology&amp;offsetIndex=0&amp;sortType=sortdate:desc&amp;searchType=ALL</t>
+  </si>
+  <si>
+    <t>/cmty/#/search?query=biology&amp;offsetIndex=0&amp;sortType=sortdate:asc&amp;searchType=ALL</t>
+  </si>
+  <si>
+    <t>/cmty/#/search?query=biology&amp;offsetIndex=0&amp;sortType=citingsrcslocalcount:desc&amp;searchType=ARTICLES</t>
+  </si>
+  <si>
+    <t>/cmty/#/search?query=biology&amp;offsetIndex=0&amp;sortType=sortdate:desc&amp;searchType=ARTICLES</t>
+  </si>
+  <si>
+    <t>/cmty/#/search?query=biology&amp;offsetIndex=0&amp;sortType=sortdate:asc&amp;searchType=ARTICLES</t>
+  </si>
+  <si>
+    <t>/cmty/#/search?query=biology&amp;offsetIndex=0&amp;sortType=citingsrcscount:desc&amp;searchType=PATENTS</t>
+  </si>
+  <si>
+    <t>/cmty/#/search?query=biology&amp;offsetIndex=0&amp;sortType=sortdate:desc&amp;searchType=PATENTS</t>
+  </si>
+  <si>
+    <t>/cmty/#/search?query=biology&amp;offsetIndex=0&amp;sortType=sortdate:asc&amp;searchType=PATENTS</t>
+  </si>
+  <si>
+    <t>/cmty/#/search?query=biology&amp;offsetIndex=0&amp;sortType=loadtime:desc&amp;searchType=PEOPLE</t>
+  </si>
+  <si>
+    <t>/cmty/#/search?query=post&amp;offsetIndex=0&amp;sortType=sortdate:desc&amp;searchType=POSTS</t>
+  </si>
+  <si>
+    <t>/cmty/#/search?query=biology&amp;offsetIndex=0&amp;sortType=sortdate:asc&amp;searchType=POSTS</t>
+  </si>
+  <si>
+    <t>/cmty/#/search?query=biology&amp;offsetIndex=0&amp;sortType=_score:desc&amp;searchType=POSTS</t>
   </si>
 </sst>
 </file>
@@ -1792,7 +1792,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B113" sqref="B113"/>
     </sheetView>
   </sheetViews>
@@ -2201,7 +2201,7 @@
         <v>227</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>383</v>
+        <v>365</v>
       </c>
       <c r="C24" s="8" t="s">
         <v>73</v>
@@ -2898,10 +2898,10 @@
         <v>268</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>371</v>
+        <v>353</v>
       </c>
       <c r="C65" s="7" t="s">
-        <v>363</v>
+        <v>345</v>
       </c>
       <c r="D65" s="8" t="s">
         <v>308</v>
@@ -2935,7 +2935,7 @@
         <v>123</v>
       </c>
       <c r="C67" s="7" t="s">
-        <v>366</v>
+        <v>348</v>
       </c>
       <c r="D67" s="8" t="s">
         <v>308</v>
@@ -3034,10 +3034,10 @@
         <v>276</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>384</v>
+        <v>366</v>
       </c>
       <c r="C73" s="8" t="s">
-        <v>385</v>
+        <v>367</v>
       </c>
       <c r="D73" s="8" t="s">
         <v>308</v>
@@ -3068,10 +3068,10 @@
         <v>278</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>372</v>
+        <v>354</v>
       </c>
       <c r="C75" s="7" t="s">
-        <v>362</v>
+        <v>344</v>
       </c>
       <c r="D75" s="8" t="s">
         <v>308</v>
@@ -3136,7 +3136,7 @@
         <v>282</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>373</v>
+        <v>355</v>
       </c>
       <c r="C79" s="7" t="s">
         <v>142</v>
@@ -3190,7 +3190,7 @@
         <v>147</v>
       </c>
       <c r="C82" s="8" t="s">
-        <v>382</v>
+        <v>364</v>
       </c>
       <c r="D82" s="8" t="s">
         <v>308</v>
@@ -3238,7 +3238,7 @@
         <v>288</v>
       </c>
       <c r="B85" s="8" t="s">
-        <v>374</v>
+        <v>356</v>
       </c>
       <c r="C85" s="7" t="s">
         <v>152</v>
@@ -3255,7 +3255,7 @@
         <v>289</v>
       </c>
       <c r="B86" s="9" t="s">
-        <v>375</v>
+        <v>357</v>
       </c>
       <c r="C86" s="7" t="s">
         <v>169</v>
@@ -3425,7 +3425,7 @@
         <v>299</v>
       </c>
       <c r="B96" s="9" t="s">
-        <v>376</v>
+        <v>358</v>
       </c>
       <c r="C96" s="10" t="s">
         <v>310</v>
@@ -3476,10 +3476,10 @@
         <v>302</v>
       </c>
       <c r="B99" s="7" t="s">
-        <v>377</v>
+        <v>359</v>
       </c>
       <c r="C99" s="7" t="s">
-        <v>365</v>
+        <v>347</v>
       </c>
       <c r="D99" s="8" t="s">
         <v>308</v>
@@ -3490,13 +3490,13 @@
     </row>
     <row r="100" spans="1:5" ht="120">
       <c r="A100" s="8" t="s">
-        <v>364</v>
+        <v>346</v>
       </c>
       <c r="B100" s="7" t="s">
-        <v>378</v>
+        <v>360</v>
       </c>
       <c r="C100" s="7" t="s">
-        <v>361</v>
+        <v>343</v>
       </c>
       <c r="D100" s="8" t="s">
         <v>308</v>
@@ -3589,7 +3589,7 @@
         <v>339</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>379</v>
+        <v>361</v>
       </c>
       <c r="C106" s="11" t="s">
         <v>340</v>
@@ -3601,13 +3601,13 @@
     </row>
     <row r="107" spans="1:5">
       <c r="A107" s="8" t="s">
-        <v>359</v>
+        <v>341</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>380</v>
+        <v>362</v>
       </c>
       <c r="C107" s="11" t="s">
-        <v>360</v>
+        <v>342</v>
       </c>
       <c r="D107" s="8" t="s">
         <v>308</v>
@@ -3616,13 +3616,13 @@
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="8" t="s">
-        <v>367</v>
+        <v>349</v>
       </c>
       <c r="B108" s="12" t="s">
-        <v>381</v>
+        <v>363</v>
       </c>
       <c r="C108" s="11" t="s">
-        <v>368</v>
+        <v>350</v>
       </c>
       <c r="D108" s="3" t="s">
         <v>308</v>
@@ -3631,13 +3631,13 @@
     </row>
     <row r="109" spans="1:5">
       <c r="A109" s="8" t="s">
-        <v>369</v>
+        <v>351</v>
       </c>
       <c r="B109" s="12" t="s">
-        <v>381</v>
+        <v>363</v>
       </c>
       <c r="C109" s="11" t="s">
-        <v>370</v>
+        <v>352</v>
       </c>
       <c r="D109" s="3" t="s">
         <v>308</v>
@@ -3646,13 +3646,13 @@
     </row>
     <row r="110" spans="1:5" ht="60">
       <c r="A110" s="8" t="s">
-        <v>386</v>
+        <v>368</v>
       </c>
       <c r="B110" s="11" t="s">
-        <v>387</v>
+        <v>369</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>388</v>
+        <v>370</v>
       </c>
       <c r="D110" s="8" t="s">
         <v>308</v>
@@ -3661,13 +3661,13 @@
     </row>
     <row r="111" spans="1:5" ht="60">
       <c r="A111" s="8" t="s">
-        <v>389</v>
+        <v>371</v>
       </c>
       <c r="B111" s="11" t="s">
-        <v>391</v>
+        <v>373</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>390</v>
+        <v>372</v>
       </c>
       <c r="D111" s="8" t="s">
         <v>308</v>
@@ -3688,8 +3688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A27" activeCellId="1" sqref="A19 A27:A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3715,7 +3715,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>341</v>
+        <v>374</v>
       </c>
       <c r="B2" t="s">
         <v>330</v>
@@ -3726,7 +3726,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>342</v>
+        <v>375</v>
       </c>
       <c r="B3" t="s">
         <v>331</v>
@@ -3737,7 +3737,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>343</v>
+        <v>376</v>
       </c>
       <c r="B4" t="s">
         <v>332</v>
@@ -3748,7 +3748,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>344</v>
+        <v>377</v>
       </c>
       <c r="B5" t="s">
         <v>333</v>
@@ -3759,7 +3759,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>345</v>
+        <v>378</v>
       </c>
       <c r="B6" t="s">
         <v>334</v>
@@ -3770,7 +3770,7 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>346</v>
+        <v>379</v>
       </c>
       <c r="B7" t="s">
         <v>330</v>
@@ -3781,7 +3781,7 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>347</v>
+        <v>380</v>
       </c>
       <c r="B8" t="s">
         <v>330</v>
@@ -3792,7 +3792,7 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>348</v>
+        <v>381</v>
       </c>
       <c r="B9" t="s">
         <v>330</v>
@@ -3803,7 +3803,7 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>349</v>
+        <v>382</v>
       </c>
       <c r="B10" t="s">
         <v>335</v>
@@ -3814,7 +3814,7 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>350</v>
+        <v>383</v>
       </c>
       <c r="B11" t="s">
         <v>331</v>
@@ -3825,7 +3825,7 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>351</v>
+        <v>384</v>
       </c>
       <c r="B12" t="s">
         <v>331</v>
@@ -3836,7 +3836,7 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>352</v>
+        <v>385</v>
       </c>
       <c r="B13" t="s">
         <v>336</v>
@@ -3847,7 +3847,7 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>353</v>
+        <v>386</v>
       </c>
       <c r="B14" t="s">
         <v>337</v>
@@ -3858,7 +3858,7 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>354</v>
+        <v>387</v>
       </c>
       <c r="B15" t="s">
         <v>337</v>
@@ -3869,7 +3869,7 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>355</v>
+        <v>388</v>
       </c>
       <c r="B16" t="s">
         <v>333</v>
@@ -3880,7 +3880,7 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>356</v>
+        <v>389</v>
       </c>
       <c r="B17" t="s">
         <v>338</v>
@@ -3891,7 +3891,7 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>357</v>
+        <v>390</v>
       </c>
       <c r="B18" t="s">
         <v>338</v>
@@ -3902,7 +3902,7 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>358</v>
+        <v>391</v>
       </c>
       <c r="B19" t="s">
         <v>338</v>
@@ -3921,7 +3921,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Commented testcases related to patents,postand articles in xml file and changed runmode for deeplinking testcases
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Search.xlsx
+++ b/src/test/resources/xls/Search.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2580" windowWidth="14715" windowHeight="8040" activeTab="1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="392">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="393">
   <si>
     <t>TCID</t>
   </si>
@@ -1368,12 +1368,15 @@
   <si>
     <t>/cmty/#/search?query=biology&amp;offsetIndex=0&amp;sortType=_score:desc&amp;searchType=POSTS</t>
   </si>
+  <si>
+    <t>N</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1548,7 +1551,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1580,9 +1583,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1614,6 +1618,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1789,14 +1794,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E111"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B113" sqref="B113"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.42578125" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1" collapsed="1"/>
@@ -1805,7 +1810,7 @@
     <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1822,7 +1827,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>205</v>
       </c>
@@ -1839,7 +1844,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>206</v>
       </c>
@@ -1856,7 +1861,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>207</v>
       </c>
@@ -1873,7 +1878,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>208</v>
       </c>
@@ -1890,7 +1895,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>209</v>
       </c>
@@ -1907,7 +1912,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>210</v>
       </c>
@@ -1924,7 +1929,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15" customHeight="1">
+    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>211</v>
       </c>
@@ -1941,7 +1946,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>212</v>
       </c>
@@ -1958,7 +1963,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>213</v>
       </c>
@@ -1975,7 +1980,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>214</v>
       </c>
@@ -1992,7 +1997,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="16.5" customHeight="1">
+    <row r="12" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>215</v>
       </c>
@@ -2009,7 +2014,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>216</v>
       </c>
@@ -2026,7 +2031,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>217</v>
       </c>
@@ -2043,7 +2048,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>218</v>
       </c>
@@ -2060,7 +2065,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>219</v>
       </c>
@@ -2077,7 +2082,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>220</v>
       </c>
@@ -2094,7 +2099,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>221</v>
       </c>
@@ -2111,7 +2116,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>222</v>
       </c>
@@ -2128,7 +2133,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>223</v>
       </c>
@@ -2145,7 +2150,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>224</v>
       </c>
@@ -2162,7 +2167,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
         <v>225</v>
       </c>
@@ -2179,7 +2184,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="75">
+    <row r="23" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>226</v>
       </c>
@@ -2196,7 +2201,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="30">
+    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
         <v>227</v>
       </c>
@@ -2213,7 +2218,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
         <v>228</v>
       </c>
@@ -2230,7 +2235,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
         <v>229</v>
       </c>
@@ -2247,7 +2252,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
         <v>230</v>
       </c>
@@ -2264,7 +2269,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="90">
+    <row r="28" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
         <v>231</v>
       </c>
@@ -2281,7 +2286,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="60">
+    <row r="29" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
         <v>232</v>
       </c>
@@ -2298,7 +2303,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
         <v>233</v>
       </c>
@@ -2315,7 +2320,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
         <v>234</v>
       </c>
@@ -2332,7 +2337,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
         <v>235</v>
       </c>
@@ -2349,7 +2354,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="90">
+    <row r="33" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
         <v>236</v>
       </c>
@@ -2366,7 +2371,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
         <v>237</v>
       </c>
@@ -2383,7 +2388,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
         <v>238</v>
       </c>
@@ -2400,7 +2405,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
         <v>239</v>
       </c>
@@ -2417,7 +2422,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="90">
+    <row r="37" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
         <v>240</v>
       </c>
@@ -2434,7 +2439,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
         <v>241</v>
       </c>
@@ -2451,7 +2456,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
         <v>242</v>
       </c>
@@ -2468,7 +2473,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
         <v>243</v>
       </c>
@@ -2485,7 +2490,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
         <v>244</v>
       </c>
@@ -2502,7 +2507,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="8" t="s">
         <v>245</v>
       </c>
@@ -2519,7 +2524,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="8" t="s">
         <v>246</v>
       </c>
@@ -2536,7 +2541,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="8" t="s">
         <v>247</v>
       </c>
@@ -2553,7 +2558,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="8" t="s">
         <v>248</v>
       </c>
@@ -2570,7 +2575,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="s">
         <v>249</v>
       </c>
@@ -2587,7 +2592,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="120">
+    <row r="47" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A47" s="8" t="s">
         <v>250</v>
       </c>
@@ -2604,7 +2609,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="8" t="s">
         <v>251</v>
       </c>
@@ -2621,7 +2626,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="8" t="s">
         <v>252</v>
       </c>
@@ -2638,7 +2643,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="8" t="s">
         <v>253</v>
       </c>
@@ -2655,7 +2660,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="8" t="s">
         <v>254</v>
       </c>
@@ -2672,7 +2677,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="8" t="s">
         <v>255</v>
       </c>
@@ -2689,7 +2694,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="30">
+    <row r="53" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="8" t="s">
         <v>256</v>
       </c>
@@ -2706,7 +2711,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="8" t="s">
         <v>257</v>
       </c>
@@ -2723,7 +2728,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="8" t="s">
         <v>258</v>
       </c>
@@ -2740,7 +2745,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="8" t="s">
         <v>259</v>
       </c>
@@ -2757,7 +2762,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="57" spans="1:5">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="8" t="s">
         <v>260</v>
       </c>
@@ -2774,7 +2779,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="8" t="s">
         <v>261</v>
       </c>
@@ -2791,7 +2796,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="90">
+    <row r="59" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A59" s="8" t="s">
         <v>262</v>
       </c>
@@ -2808,7 +2813,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="75">
+    <row r="60" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A60" s="8" t="s">
         <v>263</v>
       </c>
@@ -2825,7 +2830,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="8" t="s">
         <v>264</v>
       </c>
@@ -2842,7 +2847,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="8" t="s">
         <v>265</v>
       </c>
@@ -2859,7 +2864,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="8" t="s">
         <v>266</v>
       </c>
@@ -2876,7 +2881,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="120">
+    <row r="64" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A64" s="8" t="s">
         <v>267</v>
       </c>
@@ -2893,7 +2898,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="135">
+    <row r="65" spans="1:5" ht="135" x14ac:dyDescent="0.25">
       <c r="A65" s="8" t="s">
         <v>268</v>
       </c>
@@ -2910,7 +2915,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="66" spans="1:5" ht="195">
+    <row r="66" spans="1:5" ht="195" x14ac:dyDescent="0.25">
       <c r="A66" s="8" t="s">
         <v>269</v>
       </c>
@@ -2927,7 +2932,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="67" spans="1:5">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="8" t="s">
         <v>270</v>
       </c>
@@ -2944,7 +2949,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="68" spans="1:5">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="8" t="s">
         <v>271</v>
       </c>
@@ -2961,7 +2966,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="69" spans="1:5">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="8" t="s">
         <v>272</v>
       </c>
@@ -2978,7 +2983,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="70" spans="1:5" ht="30">
+    <row r="70" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="8" t="s">
         <v>273</v>
       </c>
@@ -2995,7 +3000,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="71" spans="1:5">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="8" t="s">
         <v>274</v>
       </c>
@@ -3012,7 +3017,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="72" spans="1:5">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="8" t="s">
         <v>275</v>
       </c>
@@ -3029,7 +3034,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="73" spans="1:5" ht="30">
+    <row r="73" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A73" s="8" t="s">
         <v>276</v>
       </c>
@@ -3046,7 +3051,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="74" spans="1:5">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="8" t="s">
         <v>277</v>
       </c>
@@ -3063,7 +3068,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="75" spans="1:5" ht="135">
+    <row r="75" spans="1:5" ht="135" x14ac:dyDescent="0.25">
       <c r="A75" s="8" t="s">
         <v>278</v>
       </c>
@@ -3080,7 +3085,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="76" spans="1:5" ht="105">
+    <row r="76" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A76" s="8" t="s">
         <v>279</v>
       </c>
@@ -3097,7 +3102,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="77" spans="1:5">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="8" t="s">
         <v>280</v>
       </c>
@@ -3114,7 +3119,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="78" spans="1:5">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="8" t="s">
         <v>281</v>
       </c>
@@ -3131,7 +3136,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="79" spans="1:5" ht="45">
+    <row r="79" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A79" s="8" t="s">
         <v>282</v>
       </c>
@@ -3148,7 +3153,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="80" spans="1:5">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="8" t="s">
         <v>283</v>
       </c>
@@ -3165,7 +3170,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="81" spans="1:5">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="8" t="s">
         <v>284</v>
       </c>
@@ -3182,7 +3187,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="82" spans="1:5">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="8" t="s">
         <v>285</v>
       </c>
@@ -3199,7 +3204,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="83" spans="1:5">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="8" t="s">
         <v>286</v>
       </c>
@@ -3216,7 +3221,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="84" spans="1:5">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="8" t="s">
         <v>287</v>
       </c>
@@ -3233,7 +3238,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="85" spans="1:5" ht="165">
+    <row r="85" spans="1:5" ht="165" x14ac:dyDescent="0.25">
       <c r="A85" s="8" t="s">
         <v>288</v>
       </c>
@@ -3250,7 +3255,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="86" spans="1:5" ht="75">
+    <row r="86" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A86" s="8" t="s">
         <v>289</v>
       </c>
@@ -3267,7 +3272,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="87" spans="1:5">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="8" t="s">
         <v>290</v>
       </c>
@@ -3284,7 +3289,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="88" spans="1:5">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="8" t="s">
         <v>291</v>
       </c>
@@ -3301,7 +3306,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="89" spans="1:5">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="8" t="s">
         <v>292</v>
       </c>
@@ -3318,7 +3323,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="90" spans="1:5">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="8" t="s">
         <v>293</v>
       </c>
@@ -3335,7 +3340,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="91" spans="1:5">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="8" t="s">
         <v>294</v>
       </c>
@@ -3352,7 +3357,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="92" spans="1:5">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="8" t="s">
         <v>295</v>
       </c>
@@ -3369,7 +3374,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="93" spans="1:5">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="8" t="s">
         <v>296</v>
       </c>
@@ -3386,7 +3391,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="94" spans="1:5">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="8" t="s">
         <v>297</v>
       </c>
@@ -3403,7 +3408,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="95" spans="1:5">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="8" t="s">
         <v>298</v>
       </c>
@@ -3420,7 +3425,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="96" spans="1:5" ht="30">
+    <row r="96" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A96" s="8" t="s">
         <v>299</v>
       </c>
@@ -3437,7 +3442,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="97" spans="1:5" ht="75">
+    <row r="97" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A97" s="8" t="s">
         <v>300</v>
       </c>
@@ -3454,7 +3459,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="98" spans="1:5" ht="60">
+    <row r="98" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A98" s="8" t="s">
         <v>301</v>
       </c>
@@ -3471,7 +3476,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="99" spans="1:5" ht="120">
+    <row r="99" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A99" s="8" t="s">
         <v>302</v>
       </c>
@@ -3488,7 +3493,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="100" spans="1:5" ht="120">
+    <row r="100" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A100" s="8" t="s">
         <v>346</v>
       </c>
@@ -3505,7 +3510,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="101" spans="1:5">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="8" t="s">
         <v>303</v>
       </c>
@@ -3522,7 +3527,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="102" spans="1:5">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="8" t="s">
         <v>304</v>
       </c>
@@ -3539,7 +3544,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="103" spans="1:5">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="8" t="s">
         <v>305</v>
       </c>
@@ -3554,7 +3559,7 @@
       </c>
       <c r="E103" s="3"/>
     </row>
-    <row r="104" spans="1:5">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="8" t="s">
         <v>306</v>
       </c>
@@ -3569,7 +3574,7 @@
       </c>
       <c r="E104" s="3"/>
     </row>
-    <row r="105" spans="1:5" ht="150">
+    <row r="105" spans="1:5" ht="150" x14ac:dyDescent="0.25">
       <c r="A105" s="8" t="s">
         <v>307</v>
       </c>
@@ -3584,7 +3589,7 @@
       </c>
       <c r="E105" s="3"/>
     </row>
-    <row r="106" spans="1:5">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="8" t="s">
         <v>339</v>
       </c>
@@ -3599,7 +3604,7 @@
       </c>
       <c r="E106" s="3"/>
     </row>
-    <row r="107" spans="1:5">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="8" t="s">
         <v>341</v>
       </c>
@@ -3614,7 +3619,7 @@
       </c>
       <c r="E107" s="3"/>
     </row>
-    <row r="108" spans="1:5">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="8" t="s">
         <v>349</v>
       </c>
@@ -3629,7 +3634,7 @@
       </c>
       <c r="E108" s="3"/>
     </row>
-    <row r="109" spans="1:5">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="8" t="s">
         <v>351</v>
       </c>
@@ -3644,7 +3649,7 @@
       </c>
       <c r="E109" s="3"/>
     </row>
-    <row r="110" spans="1:5" ht="60">
+    <row r="110" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A110" s="8" t="s">
         <v>368</v>
       </c>
@@ -3659,7 +3664,7 @@
       </c>
       <c r="E110" s="3"/>
     </row>
-    <row r="111" spans="1:5" ht="60">
+    <row r="111" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A111" s="8" t="s">
         <v>371</v>
       </c>
@@ -3685,21 +3690,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A27" activeCellId="1" sqref="A19 A27:A28"/>
+      <selection activeCell="C13" sqref="C13:C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="89.28515625" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>327</v>
       </c>
@@ -3713,7 +3718,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>374</v>
       </c>
@@ -3724,7 +3729,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>375</v>
       </c>
@@ -3735,7 +3740,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>376</v>
       </c>
@@ -3743,10 +3748,10 @@
         <v>332</v>
       </c>
       <c r="C4" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>377</v>
       </c>
@@ -3754,10 +3759,10 @@
         <v>333</v>
       </c>
       <c r="C5" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>378</v>
       </c>
@@ -3765,10 +3770,10 @@
         <v>334</v>
       </c>
       <c r="C6" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>379</v>
       </c>
@@ -3779,7 +3784,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>380</v>
       </c>
@@ -3790,7 +3795,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>381</v>
       </c>
@@ -3801,7 +3806,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>382</v>
       </c>
@@ -3812,7 +3817,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>383</v>
       </c>
@@ -3823,7 +3828,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>384</v>
       </c>
@@ -3834,7 +3839,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>385</v>
       </c>
@@ -3842,10 +3847,10 @@
         <v>336</v>
       </c>
       <c r="C13" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>386</v>
       </c>
@@ -3853,10 +3858,10 @@
         <v>337</v>
       </c>
       <c r="C14" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>387</v>
       </c>
@@ -3864,10 +3869,10 @@
         <v>337</v>
       </c>
       <c r="C15" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>388</v>
       </c>
@@ -3875,10 +3880,10 @@
         <v>333</v>
       </c>
       <c r="C16" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>389</v>
       </c>
@@ -3886,10 +3891,10 @@
         <v>338</v>
       </c>
       <c r="C17" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>390</v>
       </c>
@@ -3897,10 +3902,10 @@
         <v>338</v>
       </c>
       <c r="C18" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>391</v>
       </c>
@@ -3908,7 +3913,7 @@
         <v>338</v>
       </c>
       <c r="C19" t="s">
-        <v>308</v>
+        <v>392</v>
       </c>
     </row>
   </sheetData>
@@ -3918,14 +3923,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" style="5" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="52.5703125" style="5" customWidth="1" collapsed="1"/>
@@ -3933,7 +3938,7 @@
     <col min="4" max="16384" width="9.140625" style="5" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="35.25" customHeight="1">
+    <row r="1" spans="1:3" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3944,7 +3949,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="206.25" customHeight="1">
+    <row r="2" spans="1:3" ht="206.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -3955,7 +3960,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="203.25" customHeight="1">
+    <row r="3" spans="1:3" ht="203.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
@@ -3966,7 +3971,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="295.5" customHeight="1">
+    <row r="4" spans="1:3" ht="295.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>12</v>
       </c>
@@ -3977,7 +3982,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="147" customHeight="1">
+    <row r="5" spans="1:3" ht="147" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>14</v>
       </c>
@@ -3988,7 +3993,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="73.5" customHeight="1">
+    <row r="6" spans="1:3" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>18</v>
       </c>
@@ -3999,7 +4004,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="60">
+    <row r="7" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>22</v>
       </c>
@@ -4010,7 +4015,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="165.75" customHeight="1">
+    <row r="8" spans="1:3" ht="165.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>24</v>
       </c>
@@ -4021,7 +4026,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="69.75" customHeight="1">
+    <row r="9" spans="1:3" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>27</v>
       </c>

</xml_diff>